<commit_message>
Complete JavaDoc for packages and types
</commit_message>
<xml_diff>
--- a/plugins/org.eclipse.emf.cdo.doc/Tables.xlsx
+++ b/plugins/org.eclipse.emf.cdo.doc/Tables.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="28515" windowHeight="14025"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="28515" windowHeight="14025" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="StoreFeatures" sheetId="1" r:id="rId1"/>
-    <sheet name="MappingStrategies" sheetId="2" r:id="rId2"/>
+    <sheet name="MappingStrategies" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="44">
   <si>
     <t>Branching</t>
   </si>
@@ -99,13 +99,61 @@
   </si>
   <si>
     <t>CopyOnBranch</t>
+  </si>
+  <si>
+    <t>Supports Audit revisions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supports Branching </t>
+  </si>
+  <si>
+    <t>Supports Revision Deltas</t>
+  </si>
+  <si>
+    <t>Performance considerations:</t>
+  </si>
+  <si>
+    <t>- list insert (middle)</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>- list append/insert (end)</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>- list delete (middle)</t>
+  </si>
+  <si>
+    <t>- list delete (end)</t>
+  </si>
+  <si>
+    <t>- list clear</t>
+  </si>
+  <si>
+    <t>- list move</t>
+  </si>
+  <si>
+    <t>- create first revision in branch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- first list modification in branch </t>
+  </si>
+  <si>
+    <t xml:space="preserve">- subsequent list modification in branch </t>
+  </si>
+  <si>
+    <t>- read access in branch</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -133,14 +181,26 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
+      <sz val="11"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -159,8 +219,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="26">
+  <borders count="37">
     <border>
       <left/>
       <right/>
@@ -494,30 +560,200 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -576,46 +812,21 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -640,9 +851,62 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Excel Built-in Normal" xfId="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -657,9 +921,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -697,7 +961,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -767,7 +1031,7 @@
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -943,11 +1207,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="26.7109375" style="19" customWidth="1"/>
     <col min="2" max="2" width="10" style="5" customWidth="1"/>
@@ -1245,218 +1507,818 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="20.140625" style="27" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="11.42578125" style="27"/>
-    <col min="4" max="4" width="13.140625" style="27" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" style="27" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" style="27"/>
-    <col min="7" max="7" width="23.7109375" style="27" customWidth="1"/>
-    <col min="8" max="16384" width="11.42578125" style="27"/>
+    <col min="1" max="1" width="43" style="38" customWidth="1"/>
+    <col min="2" max="3" width="11.42578125" style="38"/>
+    <col min="4" max="4" width="13.28515625" style="38" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" style="38" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" style="38"/>
+    <col min="7" max="7" width="23.85546875" style="38" customWidth="1"/>
+    <col min="8" max="256" width="11.42578125" style="38"/>
+    <col min="257" max="257" width="43" style="38" customWidth="1"/>
+    <col min="258" max="259" width="11.42578125" style="38"/>
+    <col min="260" max="260" width="13.28515625" style="38" customWidth="1"/>
+    <col min="261" max="261" width="12.42578125" style="38" customWidth="1"/>
+    <col min="262" max="262" width="11.42578125" style="38"/>
+    <col min="263" max="263" width="23.85546875" style="38" customWidth="1"/>
+    <col min="264" max="512" width="11.42578125" style="38"/>
+    <col min="513" max="513" width="43" style="38" customWidth="1"/>
+    <col min="514" max="515" width="11.42578125" style="38"/>
+    <col min="516" max="516" width="13.28515625" style="38" customWidth="1"/>
+    <col min="517" max="517" width="12.42578125" style="38" customWidth="1"/>
+    <col min="518" max="518" width="11.42578125" style="38"/>
+    <col min="519" max="519" width="23.85546875" style="38" customWidth="1"/>
+    <col min="520" max="768" width="11.42578125" style="38"/>
+    <col min="769" max="769" width="43" style="38" customWidth="1"/>
+    <col min="770" max="771" width="11.42578125" style="38"/>
+    <col min="772" max="772" width="13.28515625" style="38" customWidth="1"/>
+    <col min="773" max="773" width="12.42578125" style="38" customWidth="1"/>
+    <col min="774" max="774" width="11.42578125" style="38"/>
+    <col min="775" max="775" width="23.85546875" style="38" customWidth="1"/>
+    <col min="776" max="1024" width="11.42578125" style="38"/>
+    <col min="1025" max="1025" width="43" style="38" customWidth="1"/>
+    <col min="1026" max="1027" width="11.42578125" style="38"/>
+    <col min="1028" max="1028" width="13.28515625" style="38" customWidth="1"/>
+    <col min="1029" max="1029" width="12.42578125" style="38" customWidth="1"/>
+    <col min="1030" max="1030" width="11.42578125" style="38"/>
+    <col min="1031" max="1031" width="23.85546875" style="38" customWidth="1"/>
+    <col min="1032" max="1280" width="11.42578125" style="38"/>
+    <col min="1281" max="1281" width="43" style="38" customWidth="1"/>
+    <col min="1282" max="1283" width="11.42578125" style="38"/>
+    <col min="1284" max="1284" width="13.28515625" style="38" customWidth="1"/>
+    <col min="1285" max="1285" width="12.42578125" style="38" customWidth="1"/>
+    <col min="1286" max="1286" width="11.42578125" style="38"/>
+    <col min="1287" max="1287" width="23.85546875" style="38" customWidth="1"/>
+    <col min="1288" max="1536" width="11.42578125" style="38"/>
+    <col min="1537" max="1537" width="43" style="38" customWidth="1"/>
+    <col min="1538" max="1539" width="11.42578125" style="38"/>
+    <col min="1540" max="1540" width="13.28515625" style="38" customWidth="1"/>
+    <col min="1541" max="1541" width="12.42578125" style="38" customWidth="1"/>
+    <col min="1542" max="1542" width="11.42578125" style="38"/>
+    <col min="1543" max="1543" width="23.85546875" style="38" customWidth="1"/>
+    <col min="1544" max="1792" width="11.42578125" style="38"/>
+    <col min="1793" max="1793" width="43" style="38" customWidth="1"/>
+    <col min="1794" max="1795" width="11.42578125" style="38"/>
+    <col min="1796" max="1796" width="13.28515625" style="38" customWidth="1"/>
+    <col min="1797" max="1797" width="12.42578125" style="38" customWidth="1"/>
+    <col min="1798" max="1798" width="11.42578125" style="38"/>
+    <col min="1799" max="1799" width="23.85546875" style="38" customWidth="1"/>
+    <col min="1800" max="2048" width="11.42578125" style="38"/>
+    <col min="2049" max="2049" width="43" style="38" customWidth="1"/>
+    <col min="2050" max="2051" width="11.42578125" style="38"/>
+    <col min="2052" max="2052" width="13.28515625" style="38" customWidth="1"/>
+    <col min="2053" max="2053" width="12.42578125" style="38" customWidth="1"/>
+    <col min="2054" max="2054" width="11.42578125" style="38"/>
+    <col min="2055" max="2055" width="23.85546875" style="38" customWidth="1"/>
+    <col min="2056" max="2304" width="11.42578125" style="38"/>
+    <col min="2305" max="2305" width="43" style="38" customWidth="1"/>
+    <col min="2306" max="2307" width="11.42578125" style="38"/>
+    <col min="2308" max="2308" width="13.28515625" style="38" customWidth="1"/>
+    <col min="2309" max="2309" width="12.42578125" style="38" customWidth="1"/>
+    <col min="2310" max="2310" width="11.42578125" style="38"/>
+    <col min="2311" max="2311" width="23.85546875" style="38" customWidth="1"/>
+    <col min="2312" max="2560" width="11.42578125" style="38"/>
+    <col min="2561" max="2561" width="43" style="38" customWidth="1"/>
+    <col min="2562" max="2563" width="11.42578125" style="38"/>
+    <col min="2564" max="2564" width="13.28515625" style="38" customWidth="1"/>
+    <col min="2565" max="2565" width="12.42578125" style="38" customWidth="1"/>
+    <col min="2566" max="2566" width="11.42578125" style="38"/>
+    <col min="2567" max="2567" width="23.85546875" style="38" customWidth="1"/>
+    <col min="2568" max="2816" width="11.42578125" style="38"/>
+    <col min="2817" max="2817" width="43" style="38" customWidth="1"/>
+    <col min="2818" max="2819" width="11.42578125" style="38"/>
+    <col min="2820" max="2820" width="13.28515625" style="38" customWidth="1"/>
+    <col min="2821" max="2821" width="12.42578125" style="38" customWidth="1"/>
+    <col min="2822" max="2822" width="11.42578125" style="38"/>
+    <col min="2823" max="2823" width="23.85546875" style="38" customWidth="1"/>
+    <col min="2824" max="3072" width="11.42578125" style="38"/>
+    <col min="3073" max="3073" width="43" style="38" customWidth="1"/>
+    <col min="3074" max="3075" width="11.42578125" style="38"/>
+    <col min="3076" max="3076" width="13.28515625" style="38" customWidth="1"/>
+    <col min="3077" max="3077" width="12.42578125" style="38" customWidth="1"/>
+    <col min="3078" max="3078" width="11.42578125" style="38"/>
+    <col min="3079" max="3079" width="23.85546875" style="38" customWidth="1"/>
+    <col min="3080" max="3328" width="11.42578125" style="38"/>
+    <col min="3329" max="3329" width="43" style="38" customWidth="1"/>
+    <col min="3330" max="3331" width="11.42578125" style="38"/>
+    <col min="3332" max="3332" width="13.28515625" style="38" customWidth="1"/>
+    <col min="3333" max="3333" width="12.42578125" style="38" customWidth="1"/>
+    <col min="3334" max="3334" width="11.42578125" style="38"/>
+    <col min="3335" max="3335" width="23.85546875" style="38" customWidth="1"/>
+    <col min="3336" max="3584" width="11.42578125" style="38"/>
+    <col min="3585" max="3585" width="43" style="38" customWidth="1"/>
+    <col min="3586" max="3587" width="11.42578125" style="38"/>
+    <col min="3588" max="3588" width="13.28515625" style="38" customWidth="1"/>
+    <col min="3589" max="3589" width="12.42578125" style="38" customWidth="1"/>
+    <col min="3590" max="3590" width="11.42578125" style="38"/>
+    <col min="3591" max="3591" width="23.85546875" style="38" customWidth="1"/>
+    <col min="3592" max="3840" width="11.42578125" style="38"/>
+    <col min="3841" max="3841" width="43" style="38" customWidth="1"/>
+    <col min="3842" max="3843" width="11.42578125" style="38"/>
+    <col min="3844" max="3844" width="13.28515625" style="38" customWidth="1"/>
+    <col min="3845" max="3845" width="12.42578125" style="38" customWidth="1"/>
+    <col min="3846" max="3846" width="11.42578125" style="38"/>
+    <col min="3847" max="3847" width="23.85546875" style="38" customWidth="1"/>
+    <col min="3848" max="4096" width="11.42578125" style="38"/>
+    <col min="4097" max="4097" width="43" style="38" customWidth="1"/>
+    <col min="4098" max="4099" width="11.42578125" style="38"/>
+    <col min="4100" max="4100" width="13.28515625" style="38" customWidth="1"/>
+    <col min="4101" max="4101" width="12.42578125" style="38" customWidth="1"/>
+    <col min="4102" max="4102" width="11.42578125" style="38"/>
+    <col min="4103" max="4103" width="23.85546875" style="38" customWidth="1"/>
+    <col min="4104" max="4352" width="11.42578125" style="38"/>
+    <col min="4353" max="4353" width="43" style="38" customWidth="1"/>
+    <col min="4354" max="4355" width="11.42578125" style="38"/>
+    <col min="4356" max="4356" width="13.28515625" style="38" customWidth="1"/>
+    <col min="4357" max="4357" width="12.42578125" style="38" customWidth="1"/>
+    <col min="4358" max="4358" width="11.42578125" style="38"/>
+    <col min="4359" max="4359" width="23.85546875" style="38" customWidth="1"/>
+    <col min="4360" max="4608" width="11.42578125" style="38"/>
+    <col min="4609" max="4609" width="43" style="38" customWidth="1"/>
+    <col min="4610" max="4611" width="11.42578125" style="38"/>
+    <col min="4612" max="4612" width="13.28515625" style="38" customWidth="1"/>
+    <col min="4613" max="4613" width="12.42578125" style="38" customWidth="1"/>
+    <col min="4614" max="4614" width="11.42578125" style="38"/>
+    <col min="4615" max="4615" width="23.85546875" style="38" customWidth="1"/>
+    <col min="4616" max="4864" width="11.42578125" style="38"/>
+    <col min="4865" max="4865" width="43" style="38" customWidth="1"/>
+    <col min="4866" max="4867" width="11.42578125" style="38"/>
+    <col min="4868" max="4868" width="13.28515625" style="38" customWidth="1"/>
+    <col min="4869" max="4869" width="12.42578125" style="38" customWidth="1"/>
+    <col min="4870" max="4870" width="11.42578125" style="38"/>
+    <col min="4871" max="4871" width="23.85546875" style="38" customWidth="1"/>
+    <col min="4872" max="5120" width="11.42578125" style="38"/>
+    <col min="5121" max="5121" width="43" style="38" customWidth="1"/>
+    <col min="5122" max="5123" width="11.42578125" style="38"/>
+    <col min="5124" max="5124" width="13.28515625" style="38" customWidth="1"/>
+    <col min="5125" max="5125" width="12.42578125" style="38" customWidth="1"/>
+    <col min="5126" max="5126" width="11.42578125" style="38"/>
+    <col min="5127" max="5127" width="23.85546875" style="38" customWidth="1"/>
+    <col min="5128" max="5376" width="11.42578125" style="38"/>
+    <col min="5377" max="5377" width="43" style="38" customWidth="1"/>
+    <col min="5378" max="5379" width="11.42578125" style="38"/>
+    <col min="5380" max="5380" width="13.28515625" style="38" customWidth="1"/>
+    <col min="5381" max="5381" width="12.42578125" style="38" customWidth="1"/>
+    <col min="5382" max="5382" width="11.42578125" style="38"/>
+    <col min="5383" max="5383" width="23.85546875" style="38" customWidth="1"/>
+    <col min="5384" max="5632" width="11.42578125" style="38"/>
+    <col min="5633" max="5633" width="43" style="38" customWidth="1"/>
+    <col min="5634" max="5635" width="11.42578125" style="38"/>
+    <col min="5636" max="5636" width="13.28515625" style="38" customWidth="1"/>
+    <col min="5637" max="5637" width="12.42578125" style="38" customWidth="1"/>
+    <col min="5638" max="5638" width="11.42578125" style="38"/>
+    <col min="5639" max="5639" width="23.85546875" style="38" customWidth="1"/>
+    <col min="5640" max="5888" width="11.42578125" style="38"/>
+    <col min="5889" max="5889" width="43" style="38" customWidth="1"/>
+    <col min="5890" max="5891" width="11.42578125" style="38"/>
+    <col min="5892" max="5892" width="13.28515625" style="38" customWidth="1"/>
+    <col min="5893" max="5893" width="12.42578125" style="38" customWidth="1"/>
+    <col min="5894" max="5894" width="11.42578125" style="38"/>
+    <col min="5895" max="5895" width="23.85546875" style="38" customWidth="1"/>
+    <col min="5896" max="6144" width="11.42578125" style="38"/>
+    <col min="6145" max="6145" width="43" style="38" customWidth="1"/>
+    <col min="6146" max="6147" width="11.42578125" style="38"/>
+    <col min="6148" max="6148" width="13.28515625" style="38" customWidth="1"/>
+    <col min="6149" max="6149" width="12.42578125" style="38" customWidth="1"/>
+    <col min="6150" max="6150" width="11.42578125" style="38"/>
+    <col min="6151" max="6151" width="23.85546875" style="38" customWidth="1"/>
+    <col min="6152" max="6400" width="11.42578125" style="38"/>
+    <col min="6401" max="6401" width="43" style="38" customWidth="1"/>
+    <col min="6402" max="6403" width="11.42578125" style="38"/>
+    <col min="6404" max="6404" width="13.28515625" style="38" customWidth="1"/>
+    <col min="6405" max="6405" width="12.42578125" style="38" customWidth="1"/>
+    <col min="6406" max="6406" width="11.42578125" style="38"/>
+    <col min="6407" max="6407" width="23.85546875" style="38" customWidth="1"/>
+    <col min="6408" max="6656" width="11.42578125" style="38"/>
+    <col min="6657" max="6657" width="43" style="38" customWidth="1"/>
+    <col min="6658" max="6659" width="11.42578125" style="38"/>
+    <col min="6660" max="6660" width="13.28515625" style="38" customWidth="1"/>
+    <col min="6661" max="6661" width="12.42578125" style="38" customWidth="1"/>
+    <col min="6662" max="6662" width="11.42578125" style="38"/>
+    <col min="6663" max="6663" width="23.85546875" style="38" customWidth="1"/>
+    <col min="6664" max="6912" width="11.42578125" style="38"/>
+    <col min="6913" max="6913" width="43" style="38" customWidth="1"/>
+    <col min="6914" max="6915" width="11.42578125" style="38"/>
+    <col min="6916" max="6916" width="13.28515625" style="38" customWidth="1"/>
+    <col min="6917" max="6917" width="12.42578125" style="38" customWidth="1"/>
+    <col min="6918" max="6918" width="11.42578125" style="38"/>
+    <col min="6919" max="6919" width="23.85546875" style="38" customWidth="1"/>
+    <col min="6920" max="7168" width="11.42578125" style="38"/>
+    <col min="7169" max="7169" width="43" style="38" customWidth="1"/>
+    <col min="7170" max="7171" width="11.42578125" style="38"/>
+    <col min="7172" max="7172" width="13.28515625" style="38" customWidth="1"/>
+    <col min="7173" max="7173" width="12.42578125" style="38" customWidth="1"/>
+    <col min="7174" max="7174" width="11.42578125" style="38"/>
+    <col min="7175" max="7175" width="23.85546875" style="38" customWidth="1"/>
+    <col min="7176" max="7424" width="11.42578125" style="38"/>
+    <col min="7425" max="7425" width="43" style="38" customWidth="1"/>
+    <col min="7426" max="7427" width="11.42578125" style="38"/>
+    <col min="7428" max="7428" width="13.28515625" style="38" customWidth="1"/>
+    <col min="7429" max="7429" width="12.42578125" style="38" customWidth="1"/>
+    <col min="7430" max="7430" width="11.42578125" style="38"/>
+    <col min="7431" max="7431" width="23.85546875" style="38" customWidth="1"/>
+    <col min="7432" max="7680" width="11.42578125" style="38"/>
+    <col min="7681" max="7681" width="43" style="38" customWidth="1"/>
+    <col min="7682" max="7683" width="11.42578125" style="38"/>
+    <col min="7684" max="7684" width="13.28515625" style="38" customWidth="1"/>
+    <col min="7685" max="7685" width="12.42578125" style="38" customWidth="1"/>
+    <col min="7686" max="7686" width="11.42578125" style="38"/>
+    <col min="7687" max="7687" width="23.85546875" style="38" customWidth="1"/>
+    <col min="7688" max="7936" width="11.42578125" style="38"/>
+    <col min="7937" max="7937" width="43" style="38" customWidth="1"/>
+    <col min="7938" max="7939" width="11.42578125" style="38"/>
+    <col min="7940" max="7940" width="13.28515625" style="38" customWidth="1"/>
+    <col min="7941" max="7941" width="12.42578125" style="38" customWidth="1"/>
+    <col min="7942" max="7942" width="11.42578125" style="38"/>
+    <col min="7943" max="7943" width="23.85546875" style="38" customWidth="1"/>
+    <col min="7944" max="8192" width="11.42578125" style="38"/>
+    <col min="8193" max="8193" width="43" style="38" customWidth="1"/>
+    <col min="8194" max="8195" width="11.42578125" style="38"/>
+    <col min="8196" max="8196" width="13.28515625" style="38" customWidth="1"/>
+    <col min="8197" max="8197" width="12.42578125" style="38" customWidth="1"/>
+    <col min="8198" max="8198" width="11.42578125" style="38"/>
+    <col min="8199" max="8199" width="23.85546875" style="38" customWidth="1"/>
+    <col min="8200" max="8448" width="11.42578125" style="38"/>
+    <col min="8449" max="8449" width="43" style="38" customWidth="1"/>
+    <col min="8450" max="8451" width="11.42578125" style="38"/>
+    <col min="8452" max="8452" width="13.28515625" style="38" customWidth="1"/>
+    <col min="8453" max="8453" width="12.42578125" style="38" customWidth="1"/>
+    <col min="8454" max="8454" width="11.42578125" style="38"/>
+    <col min="8455" max="8455" width="23.85546875" style="38" customWidth="1"/>
+    <col min="8456" max="8704" width="11.42578125" style="38"/>
+    <col min="8705" max="8705" width="43" style="38" customWidth="1"/>
+    <col min="8706" max="8707" width="11.42578125" style="38"/>
+    <col min="8708" max="8708" width="13.28515625" style="38" customWidth="1"/>
+    <col min="8709" max="8709" width="12.42578125" style="38" customWidth="1"/>
+    <col min="8710" max="8710" width="11.42578125" style="38"/>
+    <col min="8711" max="8711" width="23.85546875" style="38" customWidth="1"/>
+    <col min="8712" max="8960" width="11.42578125" style="38"/>
+    <col min="8961" max="8961" width="43" style="38" customWidth="1"/>
+    <col min="8962" max="8963" width="11.42578125" style="38"/>
+    <col min="8964" max="8964" width="13.28515625" style="38" customWidth="1"/>
+    <col min="8965" max="8965" width="12.42578125" style="38" customWidth="1"/>
+    <col min="8966" max="8966" width="11.42578125" style="38"/>
+    <col min="8967" max="8967" width="23.85546875" style="38" customWidth="1"/>
+    <col min="8968" max="9216" width="11.42578125" style="38"/>
+    <col min="9217" max="9217" width="43" style="38" customWidth="1"/>
+    <col min="9218" max="9219" width="11.42578125" style="38"/>
+    <col min="9220" max="9220" width="13.28515625" style="38" customWidth="1"/>
+    <col min="9221" max="9221" width="12.42578125" style="38" customWidth="1"/>
+    <col min="9222" max="9222" width="11.42578125" style="38"/>
+    <col min="9223" max="9223" width="23.85546875" style="38" customWidth="1"/>
+    <col min="9224" max="9472" width="11.42578125" style="38"/>
+    <col min="9473" max="9473" width="43" style="38" customWidth="1"/>
+    <col min="9474" max="9475" width="11.42578125" style="38"/>
+    <col min="9476" max="9476" width="13.28515625" style="38" customWidth="1"/>
+    <col min="9477" max="9477" width="12.42578125" style="38" customWidth="1"/>
+    <col min="9478" max="9478" width="11.42578125" style="38"/>
+    <col min="9479" max="9479" width="23.85546875" style="38" customWidth="1"/>
+    <col min="9480" max="9728" width="11.42578125" style="38"/>
+    <col min="9729" max="9729" width="43" style="38" customWidth="1"/>
+    <col min="9730" max="9731" width="11.42578125" style="38"/>
+    <col min="9732" max="9732" width="13.28515625" style="38" customWidth="1"/>
+    <col min="9733" max="9733" width="12.42578125" style="38" customWidth="1"/>
+    <col min="9734" max="9734" width="11.42578125" style="38"/>
+    <col min="9735" max="9735" width="23.85546875" style="38" customWidth="1"/>
+    <col min="9736" max="9984" width="11.42578125" style="38"/>
+    <col min="9985" max="9985" width="43" style="38" customWidth="1"/>
+    <col min="9986" max="9987" width="11.42578125" style="38"/>
+    <col min="9988" max="9988" width="13.28515625" style="38" customWidth="1"/>
+    <col min="9989" max="9989" width="12.42578125" style="38" customWidth="1"/>
+    <col min="9990" max="9990" width="11.42578125" style="38"/>
+    <col min="9991" max="9991" width="23.85546875" style="38" customWidth="1"/>
+    <col min="9992" max="10240" width="11.42578125" style="38"/>
+    <col min="10241" max="10241" width="43" style="38" customWidth="1"/>
+    <col min="10242" max="10243" width="11.42578125" style="38"/>
+    <col min="10244" max="10244" width="13.28515625" style="38" customWidth="1"/>
+    <col min="10245" max="10245" width="12.42578125" style="38" customWidth="1"/>
+    <col min="10246" max="10246" width="11.42578125" style="38"/>
+    <col min="10247" max="10247" width="23.85546875" style="38" customWidth="1"/>
+    <col min="10248" max="10496" width="11.42578125" style="38"/>
+    <col min="10497" max="10497" width="43" style="38" customWidth="1"/>
+    <col min="10498" max="10499" width="11.42578125" style="38"/>
+    <col min="10500" max="10500" width="13.28515625" style="38" customWidth="1"/>
+    <col min="10501" max="10501" width="12.42578125" style="38" customWidth="1"/>
+    <col min="10502" max="10502" width="11.42578125" style="38"/>
+    <col min="10503" max="10503" width="23.85546875" style="38" customWidth="1"/>
+    <col min="10504" max="10752" width="11.42578125" style="38"/>
+    <col min="10753" max="10753" width="43" style="38" customWidth="1"/>
+    <col min="10754" max="10755" width="11.42578125" style="38"/>
+    <col min="10756" max="10756" width="13.28515625" style="38" customWidth="1"/>
+    <col min="10757" max="10757" width="12.42578125" style="38" customWidth="1"/>
+    <col min="10758" max="10758" width="11.42578125" style="38"/>
+    <col min="10759" max="10759" width="23.85546875" style="38" customWidth="1"/>
+    <col min="10760" max="11008" width="11.42578125" style="38"/>
+    <col min="11009" max="11009" width="43" style="38" customWidth="1"/>
+    <col min="11010" max="11011" width="11.42578125" style="38"/>
+    <col min="11012" max="11012" width="13.28515625" style="38" customWidth="1"/>
+    <col min="11013" max="11013" width="12.42578125" style="38" customWidth="1"/>
+    <col min="11014" max="11014" width="11.42578125" style="38"/>
+    <col min="11015" max="11015" width="23.85546875" style="38" customWidth="1"/>
+    <col min="11016" max="11264" width="11.42578125" style="38"/>
+    <col min="11265" max="11265" width="43" style="38" customWidth="1"/>
+    <col min="11266" max="11267" width="11.42578125" style="38"/>
+    <col min="11268" max="11268" width="13.28515625" style="38" customWidth="1"/>
+    <col min="11269" max="11269" width="12.42578125" style="38" customWidth="1"/>
+    <col min="11270" max="11270" width="11.42578125" style="38"/>
+    <col min="11271" max="11271" width="23.85546875" style="38" customWidth="1"/>
+    <col min="11272" max="11520" width="11.42578125" style="38"/>
+    <col min="11521" max="11521" width="43" style="38" customWidth="1"/>
+    <col min="11522" max="11523" width="11.42578125" style="38"/>
+    <col min="11524" max="11524" width="13.28515625" style="38" customWidth="1"/>
+    <col min="11525" max="11525" width="12.42578125" style="38" customWidth="1"/>
+    <col min="11526" max="11526" width="11.42578125" style="38"/>
+    <col min="11527" max="11527" width="23.85546875" style="38" customWidth="1"/>
+    <col min="11528" max="11776" width="11.42578125" style="38"/>
+    <col min="11777" max="11777" width="43" style="38" customWidth="1"/>
+    <col min="11778" max="11779" width="11.42578125" style="38"/>
+    <col min="11780" max="11780" width="13.28515625" style="38" customWidth="1"/>
+    <col min="11781" max="11781" width="12.42578125" style="38" customWidth="1"/>
+    <col min="11782" max="11782" width="11.42578125" style="38"/>
+    <col min="11783" max="11783" width="23.85546875" style="38" customWidth="1"/>
+    <col min="11784" max="12032" width="11.42578125" style="38"/>
+    <col min="12033" max="12033" width="43" style="38" customWidth="1"/>
+    <col min="12034" max="12035" width="11.42578125" style="38"/>
+    <col min="12036" max="12036" width="13.28515625" style="38" customWidth="1"/>
+    <col min="12037" max="12037" width="12.42578125" style="38" customWidth="1"/>
+    <col min="12038" max="12038" width="11.42578125" style="38"/>
+    <col min="12039" max="12039" width="23.85546875" style="38" customWidth="1"/>
+    <col min="12040" max="12288" width="11.42578125" style="38"/>
+    <col min="12289" max="12289" width="43" style="38" customWidth="1"/>
+    <col min="12290" max="12291" width="11.42578125" style="38"/>
+    <col min="12292" max="12292" width="13.28515625" style="38" customWidth="1"/>
+    <col min="12293" max="12293" width="12.42578125" style="38" customWidth="1"/>
+    <col min="12294" max="12294" width="11.42578125" style="38"/>
+    <col min="12295" max="12295" width="23.85546875" style="38" customWidth="1"/>
+    <col min="12296" max="12544" width="11.42578125" style="38"/>
+    <col min="12545" max="12545" width="43" style="38" customWidth="1"/>
+    <col min="12546" max="12547" width="11.42578125" style="38"/>
+    <col min="12548" max="12548" width="13.28515625" style="38" customWidth="1"/>
+    <col min="12549" max="12549" width="12.42578125" style="38" customWidth="1"/>
+    <col min="12550" max="12550" width="11.42578125" style="38"/>
+    <col min="12551" max="12551" width="23.85546875" style="38" customWidth="1"/>
+    <col min="12552" max="12800" width="11.42578125" style="38"/>
+    <col min="12801" max="12801" width="43" style="38" customWidth="1"/>
+    <col min="12802" max="12803" width="11.42578125" style="38"/>
+    <col min="12804" max="12804" width="13.28515625" style="38" customWidth="1"/>
+    <col min="12805" max="12805" width="12.42578125" style="38" customWidth="1"/>
+    <col min="12806" max="12806" width="11.42578125" style="38"/>
+    <col min="12807" max="12807" width="23.85546875" style="38" customWidth="1"/>
+    <col min="12808" max="13056" width="11.42578125" style="38"/>
+    <col min="13057" max="13057" width="43" style="38" customWidth="1"/>
+    <col min="13058" max="13059" width="11.42578125" style="38"/>
+    <col min="13060" max="13060" width="13.28515625" style="38" customWidth="1"/>
+    <col min="13061" max="13061" width="12.42578125" style="38" customWidth="1"/>
+    <col min="13062" max="13062" width="11.42578125" style="38"/>
+    <col min="13063" max="13063" width="23.85546875" style="38" customWidth="1"/>
+    <col min="13064" max="13312" width="11.42578125" style="38"/>
+    <col min="13313" max="13313" width="43" style="38" customWidth="1"/>
+    <col min="13314" max="13315" width="11.42578125" style="38"/>
+    <col min="13316" max="13316" width="13.28515625" style="38" customWidth="1"/>
+    <col min="13317" max="13317" width="12.42578125" style="38" customWidth="1"/>
+    <col min="13318" max="13318" width="11.42578125" style="38"/>
+    <col min="13319" max="13319" width="23.85546875" style="38" customWidth="1"/>
+    <col min="13320" max="13568" width="11.42578125" style="38"/>
+    <col min="13569" max="13569" width="43" style="38" customWidth="1"/>
+    <col min="13570" max="13571" width="11.42578125" style="38"/>
+    <col min="13572" max="13572" width="13.28515625" style="38" customWidth="1"/>
+    <col min="13573" max="13573" width="12.42578125" style="38" customWidth="1"/>
+    <col min="13574" max="13574" width="11.42578125" style="38"/>
+    <col min="13575" max="13575" width="23.85546875" style="38" customWidth="1"/>
+    <col min="13576" max="13824" width="11.42578125" style="38"/>
+    <col min="13825" max="13825" width="43" style="38" customWidth="1"/>
+    <col min="13826" max="13827" width="11.42578125" style="38"/>
+    <col min="13828" max="13828" width="13.28515625" style="38" customWidth="1"/>
+    <col min="13829" max="13829" width="12.42578125" style="38" customWidth="1"/>
+    <col min="13830" max="13830" width="11.42578125" style="38"/>
+    <col min="13831" max="13831" width="23.85546875" style="38" customWidth="1"/>
+    <col min="13832" max="14080" width="11.42578125" style="38"/>
+    <col min="14081" max="14081" width="43" style="38" customWidth="1"/>
+    <col min="14082" max="14083" width="11.42578125" style="38"/>
+    <col min="14084" max="14084" width="13.28515625" style="38" customWidth="1"/>
+    <col min="14085" max="14085" width="12.42578125" style="38" customWidth="1"/>
+    <col min="14086" max="14086" width="11.42578125" style="38"/>
+    <col min="14087" max="14087" width="23.85546875" style="38" customWidth="1"/>
+    <col min="14088" max="14336" width="11.42578125" style="38"/>
+    <col min="14337" max="14337" width="43" style="38" customWidth="1"/>
+    <col min="14338" max="14339" width="11.42578125" style="38"/>
+    <col min="14340" max="14340" width="13.28515625" style="38" customWidth="1"/>
+    <col min="14341" max="14341" width="12.42578125" style="38" customWidth="1"/>
+    <col min="14342" max="14342" width="11.42578125" style="38"/>
+    <col min="14343" max="14343" width="23.85546875" style="38" customWidth="1"/>
+    <col min="14344" max="14592" width="11.42578125" style="38"/>
+    <col min="14593" max="14593" width="43" style="38" customWidth="1"/>
+    <col min="14594" max="14595" width="11.42578125" style="38"/>
+    <col min="14596" max="14596" width="13.28515625" style="38" customWidth="1"/>
+    <col min="14597" max="14597" width="12.42578125" style="38" customWidth="1"/>
+    <col min="14598" max="14598" width="11.42578125" style="38"/>
+    <col min="14599" max="14599" width="23.85546875" style="38" customWidth="1"/>
+    <col min="14600" max="14848" width="11.42578125" style="38"/>
+    <col min="14849" max="14849" width="43" style="38" customWidth="1"/>
+    <col min="14850" max="14851" width="11.42578125" style="38"/>
+    <col min="14852" max="14852" width="13.28515625" style="38" customWidth="1"/>
+    <col min="14853" max="14853" width="12.42578125" style="38" customWidth="1"/>
+    <col min="14854" max="14854" width="11.42578125" style="38"/>
+    <col min="14855" max="14855" width="23.85546875" style="38" customWidth="1"/>
+    <col min="14856" max="15104" width="11.42578125" style="38"/>
+    <col min="15105" max="15105" width="43" style="38" customWidth="1"/>
+    <col min="15106" max="15107" width="11.42578125" style="38"/>
+    <col min="15108" max="15108" width="13.28515625" style="38" customWidth="1"/>
+    <col min="15109" max="15109" width="12.42578125" style="38" customWidth="1"/>
+    <col min="15110" max="15110" width="11.42578125" style="38"/>
+    <col min="15111" max="15111" width="23.85546875" style="38" customWidth="1"/>
+    <col min="15112" max="15360" width="11.42578125" style="38"/>
+    <col min="15361" max="15361" width="43" style="38" customWidth="1"/>
+    <col min="15362" max="15363" width="11.42578125" style="38"/>
+    <col min="15364" max="15364" width="13.28515625" style="38" customWidth="1"/>
+    <col min="15365" max="15365" width="12.42578125" style="38" customWidth="1"/>
+    <col min="15366" max="15366" width="11.42578125" style="38"/>
+    <col min="15367" max="15367" width="23.85546875" style="38" customWidth="1"/>
+    <col min="15368" max="15616" width="11.42578125" style="38"/>
+    <col min="15617" max="15617" width="43" style="38" customWidth="1"/>
+    <col min="15618" max="15619" width="11.42578125" style="38"/>
+    <col min="15620" max="15620" width="13.28515625" style="38" customWidth="1"/>
+    <col min="15621" max="15621" width="12.42578125" style="38" customWidth="1"/>
+    <col min="15622" max="15622" width="11.42578125" style="38"/>
+    <col min="15623" max="15623" width="23.85546875" style="38" customWidth="1"/>
+    <col min="15624" max="15872" width="11.42578125" style="38"/>
+    <col min="15873" max="15873" width="43" style="38" customWidth="1"/>
+    <col min="15874" max="15875" width="11.42578125" style="38"/>
+    <col min="15876" max="15876" width="13.28515625" style="38" customWidth="1"/>
+    <col min="15877" max="15877" width="12.42578125" style="38" customWidth="1"/>
+    <col min="15878" max="15878" width="11.42578125" style="38"/>
+    <col min="15879" max="15879" width="23.85546875" style="38" customWidth="1"/>
+    <col min="15880" max="16128" width="11.42578125" style="38"/>
+    <col min="16129" max="16129" width="43" style="38" customWidth="1"/>
+    <col min="16130" max="16131" width="11.42578125" style="38"/>
+    <col min="16132" max="16132" width="13.28515625" style="38" customWidth="1"/>
+    <col min="16133" max="16133" width="12.42578125" style="38" customWidth="1"/>
+    <col min="16134" max="16134" width="11.42578125" style="38"/>
+    <col min="16135" max="16135" width="23.85546875" style="38" customWidth="1"/>
+    <col min="16136" max="16384" width="11.42578125" style="38"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="20" customFormat="1">
-      <c r="A1" s="32"/>
-      <c r="B1" s="36" t="s">
+    <row r="1" spans="1:7" s="34" customFormat="1">
+      <c r="A1" s="33"/>
+      <c r="B1" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="38"/>
-    </row>
-    <row r="2" spans="1:7" s="20" customFormat="1">
-      <c r="A2" s="32"/>
-      <c r="B2" s="40" t="s">
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="29"/>
+    </row>
+    <row r="2" spans="1:7" s="34" customFormat="1">
+      <c r="A2" s="33"/>
+      <c r="B2" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="34" t="s">
+      <c r="C2" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34" t="s">
+      <c r="D2" s="25"/>
+      <c r="E2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="34"/>
-      <c r="G2" s="35"/>
-    </row>
-    <row r="3" spans="1:7" s="20" customFormat="1">
-      <c r="A3" s="32"/>
-      <c r="B3" s="40"/>
-      <c r="C3" s="34" t="s">
+      <c r="F2" s="25"/>
+      <c r="G2" s="26"/>
+    </row>
+    <row r="3" spans="1:7" s="34" customFormat="1">
+      <c r="A3" s="33"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="34" t="s">
+      <c r="D3" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="34" t="s">
+      <c r="E3" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="34" t="s">
+      <c r="F3" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="G3" s="35"/>
-    </row>
-    <row r="4" spans="1:7" s="20" customFormat="1" ht="16.5" thickBot="1">
+      <c r="G3" s="26"/>
+    </row>
+    <row r="4" spans="1:7" s="34" customFormat="1" ht="16.5" thickBot="1">
       <c r="A4" s="33"/>
-      <c r="B4" s="41"/>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="21" t="s">
+      <c r="B4" s="32"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="G4" s="22" t="s">
+      <c r="G4" s="20" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="23"/>
-      <c r="B5" s="24"/>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="26"/>
+      <c r="A5" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="35"/>
+      <c r="C5" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5" s="37" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="28"/>
-      <c r="B6" s="29"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="13"/>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="28"/>
-      <c r="B7" s="29"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="13"/>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="28"/>
-      <c r="B8" s="29"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="13"/>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="28"/>
-      <c r="B9" s="29"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="13"/>
+      <c r="A6" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="39"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="40" t="s">
+        <v>2</v>
+      </c>
+      <c r="G6" s="41" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="16.5" thickBot="1">
+      <c r="A7" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="42" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="43"/>
+      <c r="D7" s="43" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="43"/>
+      <c r="F7" s="43" t="s">
+        <v>2</v>
+      </c>
+      <c r="G7" s="44" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="16.5" thickBot="1">
+      <c r="A8" s="48"/>
+      <c r="B8" s="49"/>
+      <c r="C8" s="49"/>
+      <c r="D8" s="49"/>
+      <c r="E8" s="49"/>
+      <c r="F8" s="49"/>
+      <c r="G8" s="49"/>
+    </row>
+    <row r="9" spans="1:7" ht="16.5" thickBot="1">
+      <c r="A9" s="50" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="49"/>
+      <c r="C9" s="49"/>
+      <c r="D9" s="49"/>
+      <c r="E9" s="49"/>
+      <c r="F9" s="49"/>
+      <c r="G9" s="49"/>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="28"/>
-      <c r="B10" s="29"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="13"/>
+      <c r="A10" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="45" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="36">
+        <v>0</v>
+      </c>
+      <c r="D10" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="36">
+        <v>0</v>
+      </c>
+      <c r="F10" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="G10" s="37" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="28"/>
-      <c r="B11" s="29"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="13"/>
+      <c r="A11" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="46" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="40">
+        <v>0</v>
+      </c>
+      <c r="D11" s="40" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" s="40">
+        <v>0</v>
+      </c>
+      <c r="F11" s="40" t="s">
+        <v>35</v>
+      </c>
+      <c r="G11" s="41" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="28"/>
-      <c r="B12" s="29"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="13"/>
+      <c r="A12" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="46" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="40">
+        <v>0</v>
+      </c>
+      <c r="D12" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" s="40">
+        <v>0</v>
+      </c>
+      <c r="F12" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="G12" s="41" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="28"/>
-      <c r="B13" s="29"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="13"/>
+      <c r="A13" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="46" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="40">
+        <v>0</v>
+      </c>
+      <c r="D13" s="40" t="s">
+        <v>35</v>
+      </c>
+      <c r="E13" s="40">
+        <v>0</v>
+      </c>
+      <c r="F13" s="40" t="s">
+        <v>35</v>
+      </c>
+      <c r="G13" s="41" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="28"/>
-      <c r="B14" s="29"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="13"/>
+      <c r="A14" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="46" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="40" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="40" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14" s="40" t="s">
+        <v>35</v>
+      </c>
+      <c r="F14" s="40" t="s">
+        <v>35</v>
+      </c>
+      <c r="G14" s="41" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="28"/>
-      <c r="B15" s="29"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="13"/>
+      <c r="A15" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="46" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="40">
+        <v>0</v>
+      </c>
+      <c r="D15" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="E15" s="40">
+        <v>0</v>
+      </c>
+      <c r="F15" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="G15" s="41" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="28"/>
-      <c r="B16" s="29"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="13"/>
+      <c r="A16" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="46"/>
+      <c r="C16" s="40"/>
+      <c r="D16" s="40"/>
+      <c r="E16" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="F16" s="40" t="s">
+        <v>35</v>
+      </c>
+      <c r="G16" s="41" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="28"/>
-      <c r="B17" s="29"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="13"/>
-    </row>
-    <row r="18" spans="1:7" ht="16.5" thickBot="1">
-      <c r="A18" s="30"/>
-      <c r="B18" s="31"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="18"/>
+      <c r="A17" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" s="46"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="40" t="s">
+        <v>35</v>
+      </c>
+      <c r="F17" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="G17" s="41" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" s="46"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="40"/>
+      <c r="E18" s="40" t="s">
+        <v>35</v>
+      </c>
+      <c r="F18" s="40" t="s">
+        <v>35</v>
+      </c>
+      <c r="G18" s="41" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="16.5" thickBot="1">
+      <c r="A19" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" s="47"/>
+      <c r="C19" s="43"/>
+      <c r="D19" s="43"/>
+      <c r="E19" s="43" t="s">
+        <v>35</v>
+      </c>
+      <c r="F19" s="43" t="s">
+        <v>33</v>
+      </c>
+      <c r="G19" s="44" t="s">
+        <v>35</v>
+      </c>
     </row>
   </sheetData>
+  <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="9">
     <mergeCell ref="A1:A4"/>
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="B2:B4"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:G2"/>
-    <mergeCell ref="B1:G1"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="D3:D4"/>
-    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:G3"/>
-    <mergeCell ref="E3:E4"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555551" footer="0.51180555555555551"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[478047] Provide more documentation
https://bugs.eclipse.org/bugs/show_bug.cgi?id=478047
</commit_message>
<xml_diff>
--- a/plugins/org.eclipse.emf.cdo.doc/Tables.xlsx
+++ b/plugins/org.eclipse.emf.cdo.doc/Tables.xlsx
@@ -4,18 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="28515" windowHeight="14025" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="28515" windowHeight="14025" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="StoreFeatures" sheetId="1" r:id="rId1"/>
     <sheet name="MappingStrategies" sheetId="3" r:id="rId2"/>
+    <sheet name="AuditingSupport" sheetId="4" r:id="rId3"/>
+    <sheet name="BranchingSupport" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="58">
   <si>
     <t>Branching</t>
   </si>
@@ -147,13 +149,88 @@
   </si>
   <si>
     <t>- read access in branch</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>Store Type</t>
+  </si>
+  <si>
+    <t>DBStore</t>
+  </si>
+  <si>
+    <t>MEMStore</t>
+  </si>
+  <si>
+    <t>HibernateStore</t>
+  </si>
+  <si>
+    <t>ObjectivityStore</t>
+  </si>
+  <si>
+    <t>DB4OStore</t>
+  </si>
+  <si>
+    <t>MongoDBStore</t>
+  </si>
+  <si>
+    <r>
+      <t>true</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF333333"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, if the used mapping strategy supports audits</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">true </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF333333"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>/ false</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>true</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF333333"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, if the used mapping strategy supports branches</t>
+    </r>
+  </si>
+  <si>
+    <t>Allowed Values</t>
+  </si>
+  <si>
+    <t>Default Value</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -199,6 +276,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -753,7 +836,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -827,86 +910,104 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Excel Built-in Normal" xfId="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -921,9 +1022,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Larissa">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -961,7 +1062,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Larissa">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1031,7 +1132,7 @@
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Larissa">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1207,9 +1308,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="26.7109375" style="19" customWidth="1"/>
     <col min="2" max="2" width="10" style="5" customWidth="1"/>
@@ -1509,511 +1612,511 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="43" style="38" customWidth="1"/>
-    <col min="2" max="3" width="11.42578125" style="38"/>
-    <col min="4" max="4" width="13.28515625" style="38" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" style="38" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" style="38"/>
-    <col min="7" max="7" width="23.85546875" style="38" customWidth="1"/>
-    <col min="8" max="256" width="11.42578125" style="38"/>
-    <col min="257" max="257" width="43" style="38" customWidth="1"/>
-    <col min="258" max="259" width="11.42578125" style="38"/>
-    <col min="260" max="260" width="13.28515625" style="38" customWidth="1"/>
-    <col min="261" max="261" width="12.42578125" style="38" customWidth="1"/>
-    <col min="262" max="262" width="11.42578125" style="38"/>
-    <col min="263" max="263" width="23.85546875" style="38" customWidth="1"/>
-    <col min="264" max="512" width="11.42578125" style="38"/>
-    <col min="513" max="513" width="43" style="38" customWidth="1"/>
-    <col min="514" max="515" width="11.42578125" style="38"/>
-    <col min="516" max="516" width="13.28515625" style="38" customWidth="1"/>
-    <col min="517" max="517" width="12.42578125" style="38" customWidth="1"/>
-    <col min="518" max="518" width="11.42578125" style="38"/>
-    <col min="519" max="519" width="23.85546875" style="38" customWidth="1"/>
-    <col min="520" max="768" width="11.42578125" style="38"/>
-    <col min="769" max="769" width="43" style="38" customWidth="1"/>
-    <col min="770" max="771" width="11.42578125" style="38"/>
-    <col min="772" max="772" width="13.28515625" style="38" customWidth="1"/>
-    <col min="773" max="773" width="12.42578125" style="38" customWidth="1"/>
-    <col min="774" max="774" width="11.42578125" style="38"/>
-    <col min="775" max="775" width="23.85546875" style="38" customWidth="1"/>
-    <col min="776" max="1024" width="11.42578125" style="38"/>
-    <col min="1025" max="1025" width="43" style="38" customWidth="1"/>
-    <col min="1026" max="1027" width="11.42578125" style="38"/>
-    <col min="1028" max="1028" width="13.28515625" style="38" customWidth="1"/>
-    <col min="1029" max="1029" width="12.42578125" style="38" customWidth="1"/>
-    <col min="1030" max="1030" width="11.42578125" style="38"/>
-    <col min="1031" max="1031" width="23.85546875" style="38" customWidth="1"/>
-    <col min="1032" max="1280" width="11.42578125" style="38"/>
-    <col min="1281" max="1281" width="43" style="38" customWidth="1"/>
-    <col min="1282" max="1283" width="11.42578125" style="38"/>
-    <col min="1284" max="1284" width="13.28515625" style="38" customWidth="1"/>
-    <col min="1285" max="1285" width="12.42578125" style="38" customWidth="1"/>
-    <col min="1286" max="1286" width="11.42578125" style="38"/>
-    <col min="1287" max="1287" width="23.85546875" style="38" customWidth="1"/>
-    <col min="1288" max="1536" width="11.42578125" style="38"/>
-    <col min="1537" max="1537" width="43" style="38" customWidth="1"/>
-    <col min="1538" max="1539" width="11.42578125" style="38"/>
-    <col min="1540" max="1540" width="13.28515625" style="38" customWidth="1"/>
-    <col min="1541" max="1541" width="12.42578125" style="38" customWidth="1"/>
-    <col min="1542" max="1542" width="11.42578125" style="38"/>
-    <col min="1543" max="1543" width="23.85546875" style="38" customWidth="1"/>
-    <col min="1544" max="1792" width="11.42578125" style="38"/>
-    <col min="1793" max="1793" width="43" style="38" customWidth="1"/>
-    <col min="1794" max="1795" width="11.42578125" style="38"/>
-    <col min="1796" max="1796" width="13.28515625" style="38" customWidth="1"/>
-    <col min="1797" max="1797" width="12.42578125" style="38" customWidth="1"/>
-    <col min="1798" max="1798" width="11.42578125" style="38"/>
-    <col min="1799" max="1799" width="23.85546875" style="38" customWidth="1"/>
-    <col min="1800" max="2048" width="11.42578125" style="38"/>
-    <col min="2049" max="2049" width="43" style="38" customWidth="1"/>
-    <col min="2050" max="2051" width="11.42578125" style="38"/>
-    <col min="2052" max="2052" width="13.28515625" style="38" customWidth="1"/>
-    <col min="2053" max="2053" width="12.42578125" style="38" customWidth="1"/>
-    <col min="2054" max="2054" width="11.42578125" style="38"/>
-    <col min="2055" max="2055" width="23.85546875" style="38" customWidth="1"/>
-    <col min="2056" max="2304" width="11.42578125" style="38"/>
-    <col min="2305" max="2305" width="43" style="38" customWidth="1"/>
-    <col min="2306" max="2307" width="11.42578125" style="38"/>
-    <col min="2308" max="2308" width="13.28515625" style="38" customWidth="1"/>
-    <col min="2309" max="2309" width="12.42578125" style="38" customWidth="1"/>
-    <col min="2310" max="2310" width="11.42578125" style="38"/>
-    <col min="2311" max="2311" width="23.85546875" style="38" customWidth="1"/>
-    <col min="2312" max="2560" width="11.42578125" style="38"/>
-    <col min="2561" max="2561" width="43" style="38" customWidth="1"/>
-    <col min="2562" max="2563" width="11.42578125" style="38"/>
-    <col min="2564" max="2564" width="13.28515625" style="38" customWidth="1"/>
-    <col min="2565" max="2565" width="12.42578125" style="38" customWidth="1"/>
-    <col min="2566" max="2566" width="11.42578125" style="38"/>
-    <col min="2567" max="2567" width="23.85546875" style="38" customWidth="1"/>
-    <col min="2568" max="2816" width="11.42578125" style="38"/>
-    <col min="2817" max="2817" width="43" style="38" customWidth="1"/>
-    <col min="2818" max="2819" width="11.42578125" style="38"/>
-    <col min="2820" max="2820" width="13.28515625" style="38" customWidth="1"/>
-    <col min="2821" max="2821" width="12.42578125" style="38" customWidth="1"/>
-    <col min="2822" max="2822" width="11.42578125" style="38"/>
-    <col min="2823" max="2823" width="23.85546875" style="38" customWidth="1"/>
-    <col min="2824" max="3072" width="11.42578125" style="38"/>
-    <col min="3073" max="3073" width="43" style="38" customWidth="1"/>
-    <col min="3074" max="3075" width="11.42578125" style="38"/>
-    <col min="3076" max="3076" width="13.28515625" style="38" customWidth="1"/>
-    <col min="3077" max="3077" width="12.42578125" style="38" customWidth="1"/>
-    <col min="3078" max="3078" width="11.42578125" style="38"/>
-    <col min="3079" max="3079" width="23.85546875" style="38" customWidth="1"/>
-    <col min="3080" max="3328" width="11.42578125" style="38"/>
-    <col min="3329" max="3329" width="43" style="38" customWidth="1"/>
-    <col min="3330" max="3331" width="11.42578125" style="38"/>
-    <col min="3332" max="3332" width="13.28515625" style="38" customWidth="1"/>
-    <col min="3333" max="3333" width="12.42578125" style="38" customWidth="1"/>
-    <col min="3334" max="3334" width="11.42578125" style="38"/>
-    <col min="3335" max="3335" width="23.85546875" style="38" customWidth="1"/>
-    <col min="3336" max="3584" width="11.42578125" style="38"/>
-    <col min="3585" max="3585" width="43" style="38" customWidth="1"/>
-    <col min="3586" max="3587" width="11.42578125" style="38"/>
-    <col min="3588" max="3588" width="13.28515625" style="38" customWidth="1"/>
-    <col min="3589" max="3589" width="12.42578125" style="38" customWidth="1"/>
-    <col min="3590" max="3590" width="11.42578125" style="38"/>
-    <col min="3591" max="3591" width="23.85546875" style="38" customWidth="1"/>
-    <col min="3592" max="3840" width="11.42578125" style="38"/>
-    <col min="3841" max="3841" width="43" style="38" customWidth="1"/>
-    <col min="3842" max="3843" width="11.42578125" style="38"/>
-    <col min="3844" max="3844" width="13.28515625" style="38" customWidth="1"/>
-    <col min="3845" max="3845" width="12.42578125" style="38" customWidth="1"/>
-    <col min="3846" max="3846" width="11.42578125" style="38"/>
-    <col min="3847" max="3847" width="23.85546875" style="38" customWidth="1"/>
-    <col min="3848" max="4096" width="11.42578125" style="38"/>
-    <col min="4097" max="4097" width="43" style="38" customWidth="1"/>
-    <col min="4098" max="4099" width="11.42578125" style="38"/>
-    <col min="4100" max="4100" width="13.28515625" style="38" customWidth="1"/>
-    <col min="4101" max="4101" width="12.42578125" style="38" customWidth="1"/>
-    <col min="4102" max="4102" width="11.42578125" style="38"/>
-    <col min="4103" max="4103" width="23.85546875" style="38" customWidth="1"/>
-    <col min="4104" max="4352" width="11.42578125" style="38"/>
-    <col min="4353" max="4353" width="43" style="38" customWidth="1"/>
-    <col min="4354" max="4355" width="11.42578125" style="38"/>
-    <col min="4356" max="4356" width="13.28515625" style="38" customWidth="1"/>
-    <col min="4357" max="4357" width="12.42578125" style="38" customWidth="1"/>
-    <col min="4358" max="4358" width="11.42578125" style="38"/>
-    <col min="4359" max="4359" width="23.85546875" style="38" customWidth="1"/>
-    <col min="4360" max="4608" width="11.42578125" style="38"/>
-    <col min="4609" max="4609" width="43" style="38" customWidth="1"/>
-    <col min="4610" max="4611" width="11.42578125" style="38"/>
-    <col min="4612" max="4612" width="13.28515625" style="38" customWidth="1"/>
-    <col min="4613" max="4613" width="12.42578125" style="38" customWidth="1"/>
-    <col min="4614" max="4614" width="11.42578125" style="38"/>
-    <col min="4615" max="4615" width="23.85546875" style="38" customWidth="1"/>
-    <col min="4616" max="4864" width="11.42578125" style="38"/>
-    <col min="4865" max="4865" width="43" style="38" customWidth="1"/>
-    <col min="4866" max="4867" width="11.42578125" style="38"/>
-    <col min="4868" max="4868" width="13.28515625" style="38" customWidth="1"/>
-    <col min="4869" max="4869" width="12.42578125" style="38" customWidth="1"/>
-    <col min="4870" max="4870" width="11.42578125" style="38"/>
-    <col min="4871" max="4871" width="23.85546875" style="38" customWidth="1"/>
-    <col min="4872" max="5120" width="11.42578125" style="38"/>
-    <col min="5121" max="5121" width="43" style="38" customWidth="1"/>
-    <col min="5122" max="5123" width="11.42578125" style="38"/>
-    <col min="5124" max="5124" width="13.28515625" style="38" customWidth="1"/>
-    <col min="5125" max="5125" width="12.42578125" style="38" customWidth="1"/>
-    <col min="5126" max="5126" width="11.42578125" style="38"/>
-    <col min="5127" max="5127" width="23.85546875" style="38" customWidth="1"/>
-    <col min="5128" max="5376" width="11.42578125" style="38"/>
-    <col min="5377" max="5377" width="43" style="38" customWidth="1"/>
-    <col min="5378" max="5379" width="11.42578125" style="38"/>
-    <col min="5380" max="5380" width="13.28515625" style="38" customWidth="1"/>
-    <col min="5381" max="5381" width="12.42578125" style="38" customWidth="1"/>
-    <col min="5382" max="5382" width="11.42578125" style="38"/>
-    <col min="5383" max="5383" width="23.85546875" style="38" customWidth="1"/>
-    <col min="5384" max="5632" width="11.42578125" style="38"/>
-    <col min="5633" max="5633" width="43" style="38" customWidth="1"/>
-    <col min="5634" max="5635" width="11.42578125" style="38"/>
-    <col min="5636" max="5636" width="13.28515625" style="38" customWidth="1"/>
-    <col min="5637" max="5637" width="12.42578125" style="38" customWidth="1"/>
-    <col min="5638" max="5638" width="11.42578125" style="38"/>
-    <col min="5639" max="5639" width="23.85546875" style="38" customWidth="1"/>
-    <col min="5640" max="5888" width="11.42578125" style="38"/>
-    <col min="5889" max="5889" width="43" style="38" customWidth="1"/>
-    <col min="5890" max="5891" width="11.42578125" style="38"/>
-    <col min="5892" max="5892" width="13.28515625" style="38" customWidth="1"/>
-    <col min="5893" max="5893" width="12.42578125" style="38" customWidth="1"/>
-    <col min="5894" max="5894" width="11.42578125" style="38"/>
-    <col min="5895" max="5895" width="23.85546875" style="38" customWidth="1"/>
-    <col min="5896" max="6144" width="11.42578125" style="38"/>
-    <col min="6145" max="6145" width="43" style="38" customWidth="1"/>
-    <col min="6146" max="6147" width="11.42578125" style="38"/>
-    <col min="6148" max="6148" width="13.28515625" style="38" customWidth="1"/>
-    <col min="6149" max="6149" width="12.42578125" style="38" customWidth="1"/>
-    <col min="6150" max="6150" width="11.42578125" style="38"/>
-    <col min="6151" max="6151" width="23.85546875" style="38" customWidth="1"/>
-    <col min="6152" max="6400" width="11.42578125" style="38"/>
-    <col min="6401" max="6401" width="43" style="38" customWidth="1"/>
-    <col min="6402" max="6403" width="11.42578125" style="38"/>
-    <col min="6404" max="6404" width="13.28515625" style="38" customWidth="1"/>
-    <col min="6405" max="6405" width="12.42578125" style="38" customWidth="1"/>
-    <col min="6406" max="6406" width="11.42578125" style="38"/>
-    <col min="6407" max="6407" width="23.85546875" style="38" customWidth="1"/>
-    <col min="6408" max="6656" width="11.42578125" style="38"/>
-    <col min="6657" max="6657" width="43" style="38" customWidth="1"/>
-    <col min="6658" max="6659" width="11.42578125" style="38"/>
-    <col min="6660" max="6660" width="13.28515625" style="38" customWidth="1"/>
-    <col min="6661" max="6661" width="12.42578125" style="38" customWidth="1"/>
-    <col min="6662" max="6662" width="11.42578125" style="38"/>
-    <col min="6663" max="6663" width="23.85546875" style="38" customWidth="1"/>
-    <col min="6664" max="6912" width="11.42578125" style="38"/>
-    <col min="6913" max="6913" width="43" style="38" customWidth="1"/>
-    <col min="6914" max="6915" width="11.42578125" style="38"/>
-    <col min="6916" max="6916" width="13.28515625" style="38" customWidth="1"/>
-    <col min="6917" max="6917" width="12.42578125" style="38" customWidth="1"/>
-    <col min="6918" max="6918" width="11.42578125" style="38"/>
-    <col min="6919" max="6919" width="23.85546875" style="38" customWidth="1"/>
-    <col min="6920" max="7168" width="11.42578125" style="38"/>
-    <col min="7169" max="7169" width="43" style="38" customWidth="1"/>
-    <col min="7170" max="7171" width="11.42578125" style="38"/>
-    <col min="7172" max="7172" width="13.28515625" style="38" customWidth="1"/>
-    <col min="7173" max="7173" width="12.42578125" style="38" customWidth="1"/>
-    <col min="7174" max="7174" width="11.42578125" style="38"/>
-    <col min="7175" max="7175" width="23.85546875" style="38" customWidth="1"/>
-    <col min="7176" max="7424" width="11.42578125" style="38"/>
-    <col min="7425" max="7425" width="43" style="38" customWidth="1"/>
-    <col min="7426" max="7427" width="11.42578125" style="38"/>
-    <col min="7428" max="7428" width="13.28515625" style="38" customWidth="1"/>
-    <col min="7429" max="7429" width="12.42578125" style="38" customWidth="1"/>
-    <col min="7430" max="7430" width="11.42578125" style="38"/>
-    <col min="7431" max="7431" width="23.85546875" style="38" customWidth="1"/>
-    <col min="7432" max="7680" width="11.42578125" style="38"/>
-    <col min="7681" max="7681" width="43" style="38" customWidth="1"/>
-    <col min="7682" max="7683" width="11.42578125" style="38"/>
-    <col min="7684" max="7684" width="13.28515625" style="38" customWidth="1"/>
-    <col min="7685" max="7685" width="12.42578125" style="38" customWidth="1"/>
-    <col min="7686" max="7686" width="11.42578125" style="38"/>
-    <col min="7687" max="7687" width="23.85546875" style="38" customWidth="1"/>
-    <col min="7688" max="7936" width="11.42578125" style="38"/>
-    <col min="7937" max="7937" width="43" style="38" customWidth="1"/>
-    <col min="7938" max="7939" width="11.42578125" style="38"/>
-    <col min="7940" max="7940" width="13.28515625" style="38" customWidth="1"/>
-    <col min="7941" max="7941" width="12.42578125" style="38" customWidth="1"/>
-    <col min="7942" max="7942" width="11.42578125" style="38"/>
-    <col min="7943" max="7943" width="23.85546875" style="38" customWidth="1"/>
-    <col min="7944" max="8192" width="11.42578125" style="38"/>
-    <col min="8193" max="8193" width="43" style="38" customWidth="1"/>
-    <col min="8194" max="8195" width="11.42578125" style="38"/>
-    <col min="8196" max="8196" width="13.28515625" style="38" customWidth="1"/>
-    <col min="8197" max="8197" width="12.42578125" style="38" customWidth="1"/>
-    <col min="8198" max="8198" width="11.42578125" style="38"/>
-    <col min="8199" max="8199" width="23.85546875" style="38" customWidth="1"/>
-    <col min="8200" max="8448" width="11.42578125" style="38"/>
-    <col min="8449" max="8449" width="43" style="38" customWidth="1"/>
-    <col min="8450" max="8451" width="11.42578125" style="38"/>
-    <col min="8452" max="8452" width="13.28515625" style="38" customWidth="1"/>
-    <col min="8453" max="8453" width="12.42578125" style="38" customWidth="1"/>
-    <col min="8454" max="8454" width="11.42578125" style="38"/>
-    <col min="8455" max="8455" width="23.85546875" style="38" customWidth="1"/>
-    <col min="8456" max="8704" width="11.42578125" style="38"/>
-    <col min="8705" max="8705" width="43" style="38" customWidth="1"/>
-    <col min="8706" max="8707" width="11.42578125" style="38"/>
-    <col min="8708" max="8708" width="13.28515625" style="38" customWidth="1"/>
-    <col min="8709" max="8709" width="12.42578125" style="38" customWidth="1"/>
-    <col min="8710" max="8710" width="11.42578125" style="38"/>
-    <col min="8711" max="8711" width="23.85546875" style="38" customWidth="1"/>
-    <col min="8712" max="8960" width="11.42578125" style="38"/>
-    <col min="8961" max="8961" width="43" style="38" customWidth="1"/>
-    <col min="8962" max="8963" width="11.42578125" style="38"/>
-    <col min="8964" max="8964" width="13.28515625" style="38" customWidth="1"/>
-    <col min="8965" max="8965" width="12.42578125" style="38" customWidth="1"/>
-    <col min="8966" max="8966" width="11.42578125" style="38"/>
-    <col min="8967" max="8967" width="23.85546875" style="38" customWidth="1"/>
-    <col min="8968" max="9216" width="11.42578125" style="38"/>
-    <col min="9217" max="9217" width="43" style="38" customWidth="1"/>
-    <col min="9218" max="9219" width="11.42578125" style="38"/>
-    <col min="9220" max="9220" width="13.28515625" style="38" customWidth="1"/>
-    <col min="9221" max="9221" width="12.42578125" style="38" customWidth="1"/>
-    <col min="9222" max="9222" width="11.42578125" style="38"/>
-    <col min="9223" max="9223" width="23.85546875" style="38" customWidth="1"/>
-    <col min="9224" max="9472" width="11.42578125" style="38"/>
-    <col min="9473" max="9473" width="43" style="38" customWidth="1"/>
-    <col min="9474" max="9475" width="11.42578125" style="38"/>
-    <col min="9476" max="9476" width="13.28515625" style="38" customWidth="1"/>
-    <col min="9477" max="9477" width="12.42578125" style="38" customWidth="1"/>
-    <col min="9478" max="9478" width="11.42578125" style="38"/>
-    <col min="9479" max="9479" width="23.85546875" style="38" customWidth="1"/>
-    <col min="9480" max="9728" width="11.42578125" style="38"/>
-    <col min="9729" max="9729" width="43" style="38" customWidth="1"/>
-    <col min="9730" max="9731" width="11.42578125" style="38"/>
-    <col min="9732" max="9732" width="13.28515625" style="38" customWidth="1"/>
-    <col min="9733" max="9733" width="12.42578125" style="38" customWidth="1"/>
-    <col min="9734" max="9734" width="11.42578125" style="38"/>
-    <col min="9735" max="9735" width="23.85546875" style="38" customWidth="1"/>
-    <col min="9736" max="9984" width="11.42578125" style="38"/>
-    <col min="9985" max="9985" width="43" style="38" customWidth="1"/>
-    <col min="9986" max="9987" width="11.42578125" style="38"/>
-    <col min="9988" max="9988" width="13.28515625" style="38" customWidth="1"/>
-    <col min="9989" max="9989" width="12.42578125" style="38" customWidth="1"/>
-    <col min="9990" max="9990" width="11.42578125" style="38"/>
-    <col min="9991" max="9991" width="23.85546875" style="38" customWidth="1"/>
-    <col min="9992" max="10240" width="11.42578125" style="38"/>
-    <col min="10241" max="10241" width="43" style="38" customWidth="1"/>
-    <col min="10242" max="10243" width="11.42578125" style="38"/>
-    <col min="10244" max="10244" width="13.28515625" style="38" customWidth="1"/>
-    <col min="10245" max="10245" width="12.42578125" style="38" customWidth="1"/>
-    <col min="10246" max="10246" width="11.42578125" style="38"/>
-    <col min="10247" max="10247" width="23.85546875" style="38" customWidth="1"/>
-    <col min="10248" max="10496" width="11.42578125" style="38"/>
-    <col min="10497" max="10497" width="43" style="38" customWidth="1"/>
-    <col min="10498" max="10499" width="11.42578125" style="38"/>
-    <col min="10500" max="10500" width="13.28515625" style="38" customWidth="1"/>
-    <col min="10501" max="10501" width="12.42578125" style="38" customWidth="1"/>
-    <col min="10502" max="10502" width="11.42578125" style="38"/>
-    <col min="10503" max="10503" width="23.85546875" style="38" customWidth="1"/>
-    <col min="10504" max="10752" width="11.42578125" style="38"/>
-    <col min="10753" max="10753" width="43" style="38" customWidth="1"/>
-    <col min="10754" max="10755" width="11.42578125" style="38"/>
-    <col min="10756" max="10756" width="13.28515625" style="38" customWidth="1"/>
-    <col min="10757" max="10757" width="12.42578125" style="38" customWidth="1"/>
-    <col min="10758" max="10758" width="11.42578125" style="38"/>
-    <col min="10759" max="10759" width="23.85546875" style="38" customWidth="1"/>
-    <col min="10760" max="11008" width="11.42578125" style="38"/>
-    <col min="11009" max="11009" width="43" style="38" customWidth="1"/>
-    <col min="11010" max="11011" width="11.42578125" style="38"/>
-    <col min="11012" max="11012" width="13.28515625" style="38" customWidth="1"/>
-    <col min="11013" max="11013" width="12.42578125" style="38" customWidth="1"/>
-    <col min="11014" max="11014" width="11.42578125" style="38"/>
-    <col min="11015" max="11015" width="23.85546875" style="38" customWidth="1"/>
-    <col min="11016" max="11264" width="11.42578125" style="38"/>
-    <col min="11265" max="11265" width="43" style="38" customWidth="1"/>
-    <col min="11266" max="11267" width="11.42578125" style="38"/>
-    <col min="11268" max="11268" width="13.28515625" style="38" customWidth="1"/>
-    <col min="11269" max="11269" width="12.42578125" style="38" customWidth="1"/>
-    <col min="11270" max="11270" width="11.42578125" style="38"/>
-    <col min="11271" max="11271" width="23.85546875" style="38" customWidth="1"/>
-    <col min="11272" max="11520" width="11.42578125" style="38"/>
-    <col min="11521" max="11521" width="43" style="38" customWidth="1"/>
-    <col min="11522" max="11523" width="11.42578125" style="38"/>
-    <col min="11524" max="11524" width="13.28515625" style="38" customWidth="1"/>
-    <col min="11525" max="11525" width="12.42578125" style="38" customWidth="1"/>
-    <col min="11526" max="11526" width="11.42578125" style="38"/>
-    <col min="11527" max="11527" width="23.85546875" style="38" customWidth="1"/>
-    <col min="11528" max="11776" width="11.42578125" style="38"/>
-    <col min="11777" max="11777" width="43" style="38" customWidth="1"/>
-    <col min="11778" max="11779" width="11.42578125" style="38"/>
-    <col min="11780" max="11780" width="13.28515625" style="38" customWidth="1"/>
-    <col min="11781" max="11781" width="12.42578125" style="38" customWidth="1"/>
-    <col min="11782" max="11782" width="11.42578125" style="38"/>
-    <col min="11783" max="11783" width="23.85546875" style="38" customWidth="1"/>
-    <col min="11784" max="12032" width="11.42578125" style="38"/>
-    <col min="12033" max="12033" width="43" style="38" customWidth="1"/>
-    <col min="12034" max="12035" width="11.42578125" style="38"/>
-    <col min="12036" max="12036" width="13.28515625" style="38" customWidth="1"/>
-    <col min="12037" max="12037" width="12.42578125" style="38" customWidth="1"/>
-    <col min="12038" max="12038" width="11.42578125" style="38"/>
-    <col min="12039" max="12039" width="23.85546875" style="38" customWidth="1"/>
-    <col min="12040" max="12288" width="11.42578125" style="38"/>
-    <col min="12289" max="12289" width="43" style="38" customWidth="1"/>
-    <col min="12290" max="12291" width="11.42578125" style="38"/>
-    <col min="12292" max="12292" width="13.28515625" style="38" customWidth="1"/>
-    <col min="12293" max="12293" width="12.42578125" style="38" customWidth="1"/>
-    <col min="12294" max="12294" width="11.42578125" style="38"/>
-    <col min="12295" max="12295" width="23.85546875" style="38" customWidth="1"/>
-    <col min="12296" max="12544" width="11.42578125" style="38"/>
-    <col min="12545" max="12545" width="43" style="38" customWidth="1"/>
-    <col min="12546" max="12547" width="11.42578125" style="38"/>
-    <col min="12548" max="12548" width="13.28515625" style="38" customWidth="1"/>
-    <col min="12549" max="12549" width="12.42578125" style="38" customWidth="1"/>
-    <col min="12550" max="12550" width="11.42578125" style="38"/>
-    <col min="12551" max="12551" width="23.85546875" style="38" customWidth="1"/>
-    <col min="12552" max="12800" width="11.42578125" style="38"/>
-    <col min="12801" max="12801" width="43" style="38" customWidth="1"/>
-    <col min="12802" max="12803" width="11.42578125" style="38"/>
-    <col min="12804" max="12804" width="13.28515625" style="38" customWidth="1"/>
-    <col min="12805" max="12805" width="12.42578125" style="38" customWidth="1"/>
-    <col min="12806" max="12806" width="11.42578125" style="38"/>
-    <col min="12807" max="12807" width="23.85546875" style="38" customWidth="1"/>
-    <col min="12808" max="13056" width="11.42578125" style="38"/>
-    <col min="13057" max="13057" width="43" style="38" customWidth="1"/>
-    <col min="13058" max="13059" width="11.42578125" style="38"/>
-    <col min="13060" max="13060" width="13.28515625" style="38" customWidth="1"/>
-    <col min="13061" max="13061" width="12.42578125" style="38" customWidth="1"/>
-    <col min="13062" max="13062" width="11.42578125" style="38"/>
-    <col min="13063" max="13063" width="23.85546875" style="38" customWidth="1"/>
-    <col min="13064" max="13312" width="11.42578125" style="38"/>
-    <col min="13313" max="13313" width="43" style="38" customWidth="1"/>
-    <col min="13314" max="13315" width="11.42578125" style="38"/>
-    <col min="13316" max="13316" width="13.28515625" style="38" customWidth="1"/>
-    <col min="13317" max="13317" width="12.42578125" style="38" customWidth="1"/>
-    <col min="13318" max="13318" width="11.42578125" style="38"/>
-    <col min="13319" max="13319" width="23.85546875" style="38" customWidth="1"/>
-    <col min="13320" max="13568" width="11.42578125" style="38"/>
-    <col min="13569" max="13569" width="43" style="38" customWidth="1"/>
-    <col min="13570" max="13571" width="11.42578125" style="38"/>
-    <col min="13572" max="13572" width="13.28515625" style="38" customWidth="1"/>
-    <col min="13573" max="13573" width="12.42578125" style="38" customWidth="1"/>
-    <col min="13574" max="13574" width="11.42578125" style="38"/>
-    <col min="13575" max="13575" width="23.85546875" style="38" customWidth="1"/>
-    <col min="13576" max="13824" width="11.42578125" style="38"/>
-    <col min="13825" max="13825" width="43" style="38" customWidth="1"/>
-    <col min="13826" max="13827" width="11.42578125" style="38"/>
-    <col min="13828" max="13828" width="13.28515625" style="38" customWidth="1"/>
-    <col min="13829" max="13829" width="12.42578125" style="38" customWidth="1"/>
-    <col min="13830" max="13830" width="11.42578125" style="38"/>
-    <col min="13831" max="13831" width="23.85546875" style="38" customWidth="1"/>
-    <col min="13832" max="14080" width="11.42578125" style="38"/>
-    <col min="14081" max="14081" width="43" style="38" customWidth="1"/>
-    <col min="14082" max="14083" width="11.42578125" style="38"/>
-    <col min="14084" max="14084" width="13.28515625" style="38" customWidth="1"/>
-    <col min="14085" max="14085" width="12.42578125" style="38" customWidth="1"/>
-    <col min="14086" max="14086" width="11.42578125" style="38"/>
-    <col min="14087" max="14087" width="23.85546875" style="38" customWidth="1"/>
-    <col min="14088" max="14336" width="11.42578125" style="38"/>
-    <col min="14337" max="14337" width="43" style="38" customWidth="1"/>
-    <col min="14338" max="14339" width="11.42578125" style="38"/>
-    <col min="14340" max="14340" width="13.28515625" style="38" customWidth="1"/>
-    <col min="14341" max="14341" width="12.42578125" style="38" customWidth="1"/>
-    <col min="14342" max="14342" width="11.42578125" style="38"/>
-    <col min="14343" max="14343" width="23.85546875" style="38" customWidth="1"/>
-    <col min="14344" max="14592" width="11.42578125" style="38"/>
-    <col min="14593" max="14593" width="43" style="38" customWidth="1"/>
-    <col min="14594" max="14595" width="11.42578125" style="38"/>
-    <col min="14596" max="14596" width="13.28515625" style="38" customWidth="1"/>
-    <col min="14597" max="14597" width="12.42578125" style="38" customWidth="1"/>
-    <col min="14598" max="14598" width="11.42578125" style="38"/>
-    <col min="14599" max="14599" width="23.85546875" style="38" customWidth="1"/>
-    <col min="14600" max="14848" width="11.42578125" style="38"/>
-    <col min="14849" max="14849" width="43" style="38" customWidth="1"/>
-    <col min="14850" max="14851" width="11.42578125" style="38"/>
-    <col min="14852" max="14852" width="13.28515625" style="38" customWidth="1"/>
-    <col min="14853" max="14853" width="12.42578125" style="38" customWidth="1"/>
-    <col min="14854" max="14854" width="11.42578125" style="38"/>
-    <col min="14855" max="14855" width="23.85546875" style="38" customWidth="1"/>
-    <col min="14856" max="15104" width="11.42578125" style="38"/>
-    <col min="15105" max="15105" width="43" style="38" customWidth="1"/>
-    <col min="15106" max="15107" width="11.42578125" style="38"/>
-    <col min="15108" max="15108" width="13.28515625" style="38" customWidth="1"/>
-    <col min="15109" max="15109" width="12.42578125" style="38" customWidth="1"/>
-    <col min="15110" max="15110" width="11.42578125" style="38"/>
-    <col min="15111" max="15111" width="23.85546875" style="38" customWidth="1"/>
-    <col min="15112" max="15360" width="11.42578125" style="38"/>
-    <col min="15361" max="15361" width="43" style="38" customWidth="1"/>
-    <col min="15362" max="15363" width="11.42578125" style="38"/>
-    <col min="15364" max="15364" width="13.28515625" style="38" customWidth="1"/>
-    <col min="15365" max="15365" width="12.42578125" style="38" customWidth="1"/>
-    <col min="15366" max="15366" width="11.42578125" style="38"/>
-    <col min="15367" max="15367" width="23.85546875" style="38" customWidth="1"/>
-    <col min="15368" max="15616" width="11.42578125" style="38"/>
-    <col min="15617" max="15617" width="43" style="38" customWidth="1"/>
-    <col min="15618" max="15619" width="11.42578125" style="38"/>
-    <col min="15620" max="15620" width="13.28515625" style="38" customWidth="1"/>
-    <col min="15621" max="15621" width="12.42578125" style="38" customWidth="1"/>
-    <col min="15622" max="15622" width="11.42578125" style="38"/>
-    <col min="15623" max="15623" width="23.85546875" style="38" customWidth="1"/>
-    <col min="15624" max="15872" width="11.42578125" style="38"/>
-    <col min="15873" max="15873" width="43" style="38" customWidth="1"/>
-    <col min="15874" max="15875" width="11.42578125" style="38"/>
-    <col min="15876" max="15876" width="13.28515625" style="38" customWidth="1"/>
-    <col min="15877" max="15877" width="12.42578125" style="38" customWidth="1"/>
-    <col min="15878" max="15878" width="11.42578125" style="38"/>
-    <col min="15879" max="15879" width="23.85546875" style="38" customWidth="1"/>
-    <col min="15880" max="16128" width="11.42578125" style="38"/>
-    <col min="16129" max="16129" width="43" style="38" customWidth="1"/>
-    <col min="16130" max="16131" width="11.42578125" style="38"/>
-    <col min="16132" max="16132" width="13.28515625" style="38" customWidth="1"/>
-    <col min="16133" max="16133" width="12.42578125" style="38" customWidth="1"/>
-    <col min="16134" max="16134" width="11.42578125" style="38"/>
-    <col min="16135" max="16135" width="23.85546875" style="38" customWidth="1"/>
-    <col min="16136" max="16384" width="11.42578125" style="38"/>
+    <col min="1" max="1" width="43" style="29" customWidth="1"/>
+    <col min="2" max="3" width="11.42578125" style="29"/>
+    <col min="4" max="4" width="13.28515625" style="29" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" style="29" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" style="29"/>
+    <col min="7" max="7" width="23.85546875" style="29" customWidth="1"/>
+    <col min="8" max="256" width="11.42578125" style="29"/>
+    <col min="257" max="257" width="43" style="29" customWidth="1"/>
+    <col min="258" max="259" width="11.42578125" style="29"/>
+    <col min="260" max="260" width="13.28515625" style="29" customWidth="1"/>
+    <col min="261" max="261" width="12.42578125" style="29" customWidth="1"/>
+    <col min="262" max="262" width="11.42578125" style="29"/>
+    <col min="263" max="263" width="23.85546875" style="29" customWidth="1"/>
+    <col min="264" max="512" width="11.42578125" style="29"/>
+    <col min="513" max="513" width="43" style="29" customWidth="1"/>
+    <col min="514" max="515" width="11.42578125" style="29"/>
+    <col min="516" max="516" width="13.28515625" style="29" customWidth="1"/>
+    <col min="517" max="517" width="12.42578125" style="29" customWidth="1"/>
+    <col min="518" max="518" width="11.42578125" style="29"/>
+    <col min="519" max="519" width="23.85546875" style="29" customWidth="1"/>
+    <col min="520" max="768" width="11.42578125" style="29"/>
+    <col min="769" max="769" width="43" style="29" customWidth="1"/>
+    <col min="770" max="771" width="11.42578125" style="29"/>
+    <col min="772" max="772" width="13.28515625" style="29" customWidth="1"/>
+    <col min="773" max="773" width="12.42578125" style="29" customWidth="1"/>
+    <col min="774" max="774" width="11.42578125" style="29"/>
+    <col min="775" max="775" width="23.85546875" style="29" customWidth="1"/>
+    <col min="776" max="1024" width="11.42578125" style="29"/>
+    <col min="1025" max="1025" width="43" style="29" customWidth="1"/>
+    <col min="1026" max="1027" width="11.42578125" style="29"/>
+    <col min="1028" max="1028" width="13.28515625" style="29" customWidth="1"/>
+    <col min="1029" max="1029" width="12.42578125" style="29" customWidth="1"/>
+    <col min="1030" max="1030" width="11.42578125" style="29"/>
+    <col min="1031" max="1031" width="23.85546875" style="29" customWidth="1"/>
+    <col min="1032" max="1280" width="11.42578125" style="29"/>
+    <col min="1281" max="1281" width="43" style="29" customWidth="1"/>
+    <col min="1282" max="1283" width="11.42578125" style="29"/>
+    <col min="1284" max="1284" width="13.28515625" style="29" customWidth="1"/>
+    <col min="1285" max="1285" width="12.42578125" style="29" customWidth="1"/>
+    <col min="1286" max="1286" width="11.42578125" style="29"/>
+    <col min="1287" max="1287" width="23.85546875" style="29" customWidth="1"/>
+    <col min="1288" max="1536" width="11.42578125" style="29"/>
+    <col min="1537" max="1537" width="43" style="29" customWidth="1"/>
+    <col min="1538" max="1539" width="11.42578125" style="29"/>
+    <col min="1540" max="1540" width="13.28515625" style="29" customWidth="1"/>
+    <col min="1541" max="1541" width="12.42578125" style="29" customWidth="1"/>
+    <col min="1542" max="1542" width="11.42578125" style="29"/>
+    <col min="1543" max="1543" width="23.85546875" style="29" customWidth="1"/>
+    <col min="1544" max="1792" width="11.42578125" style="29"/>
+    <col min="1793" max="1793" width="43" style="29" customWidth="1"/>
+    <col min="1794" max="1795" width="11.42578125" style="29"/>
+    <col min="1796" max="1796" width="13.28515625" style="29" customWidth="1"/>
+    <col min="1797" max="1797" width="12.42578125" style="29" customWidth="1"/>
+    <col min="1798" max="1798" width="11.42578125" style="29"/>
+    <col min="1799" max="1799" width="23.85546875" style="29" customWidth="1"/>
+    <col min="1800" max="2048" width="11.42578125" style="29"/>
+    <col min="2049" max="2049" width="43" style="29" customWidth="1"/>
+    <col min="2050" max="2051" width="11.42578125" style="29"/>
+    <col min="2052" max="2052" width="13.28515625" style="29" customWidth="1"/>
+    <col min="2053" max="2053" width="12.42578125" style="29" customWidth="1"/>
+    <col min="2054" max="2054" width="11.42578125" style="29"/>
+    <col min="2055" max="2055" width="23.85546875" style="29" customWidth="1"/>
+    <col min="2056" max="2304" width="11.42578125" style="29"/>
+    <col min="2305" max="2305" width="43" style="29" customWidth="1"/>
+    <col min="2306" max="2307" width="11.42578125" style="29"/>
+    <col min="2308" max="2308" width="13.28515625" style="29" customWidth="1"/>
+    <col min="2309" max="2309" width="12.42578125" style="29" customWidth="1"/>
+    <col min="2310" max="2310" width="11.42578125" style="29"/>
+    <col min="2311" max="2311" width="23.85546875" style="29" customWidth="1"/>
+    <col min="2312" max="2560" width="11.42578125" style="29"/>
+    <col min="2561" max="2561" width="43" style="29" customWidth="1"/>
+    <col min="2562" max="2563" width="11.42578125" style="29"/>
+    <col min="2564" max="2564" width="13.28515625" style="29" customWidth="1"/>
+    <col min="2565" max="2565" width="12.42578125" style="29" customWidth="1"/>
+    <col min="2566" max="2566" width="11.42578125" style="29"/>
+    <col min="2567" max="2567" width="23.85546875" style="29" customWidth="1"/>
+    <col min="2568" max="2816" width="11.42578125" style="29"/>
+    <col min="2817" max="2817" width="43" style="29" customWidth="1"/>
+    <col min="2818" max="2819" width="11.42578125" style="29"/>
+    <col min="2820" max="2820" width="13.28515625" style="29" customWidth="1"/>
+    <col min="2821" max="2821" width="12.42578125" style="29" customWidth="1"/>
+    <col min="2822" max="2822" width="11.42578125" style="29"/>
+    <col min="2823" max="2823" width="23.85546875" style="29" customWidth="1"/>
+    <col min="2824" max="3072" width="11.42578125" style="29"/>
+    <col min="3073" max="3073" width="43" style="29" customWidth="1"/>
+    <col min="3074" max="3075" width="11.42578125" style="29"/>
+    <col min="3076" max="3076" width="13.28515625" style="29" customWidth="1"/>
+    <col min="3077" max="3077" width="12.42578125" style="29" customWidth="1"/>
+    <col min="3078" max="3078" width="11.42578125" style="29"/>
+    <col min="3079" max="3079" width="23.85546875" style="29" customWidth="1"/>
+    <col min="3080" max="3328" width="11.42578125" style="29"/>
+    <col min="3329" max="3329" width="43" style="29" customWidth="1"/>
+    <col min="3330" max="3331" width="11.42578125" style="29"/>
+    <col min="3332" max="3332" width="13.28515625" style="29" customWidth="1"/>
+    <col min="3333" max="3333" width="12.42578125" style="29" customWidth="1"/>
+    <col min="3334" max="3334" width="11.42578125" style="29"/>
+    <col min="3335" max="3335" width="23.85546875" style="29" customWidth="1"/>
+    <col min="3336" max="3584" width="11.42578125" style="29"/>
+    <col min="3585" max="3585" width="43" style="29" customWidth="1"/>
+    <col min="3586" max="3587" width="11.42578125" style="29"/>
+    <col min="3588" max="3588" width="13.28515625" style="29" customWidth="1"/>
+    <col min="3589" max="3589" width="12.42578125" style="29" customWidth="1"/>
+    <col min="3590" max="3590" width="11.42578125" style="29"/>
+    <col min="3591" max="3591" width="23.85546875" style="29" customWidth="1"/>
+    <col min="3592" max="3840" width="11.42578125" style="29"/>
+    <col min="3841" max="3841" width="43" style="29" customWidth="1"/>
+    <col min="3842" max="3843" width="11.42578125" style="29"/>
+    <col min="3844" max="3844" width="13.28515625" style="29" customWidth="1"/>
+    <col min="3845" max="3845" width="12.42578125" style="29" customWidth="1"/>
+    <col min="3846" max="3846" width="11.42578125" style="29"/>
+    <col min="3847" max="3847" width="23.85546875" style="29" customWidth="1"/>
+    <col min="3848" max="4096" width="11.42578125" style="29"/>
+    <col min="4097" max="4097" width="43" style="29" customWidth="1"/>
+    <col min="4098" max="4099" width="11.42578125" style="29"/>
+    <col min="4100" max="4100" width="13.28515625" style="29" customWidth="1"/>
+    <col min="4101" max="4101" width="12.42578125" style="29" customWidth="1"/>
+    <col min="4102" max="4102" width="11.42578125" style="29"/>
+    <col min="4103" max="4103" width="23.85546875" style="29" customWidth="1"/>
+    <col min="4104" max="4352" width="11.42578125" style="29"/>
+    <col min="4353" max="4353" width="43" style="29" customWidth="1"/>
+    <col min="4354" max="4355" width="11.42578125" style="29"/>
+    <col min="4356" max="4356" width="13.28515625" style="29" customWidth="1"/>
+    <col min="4357" max="4357" width="12.42578125" style="29" customWidth="1"/>
+    <col min="4358" max="4358" width="11.42578125" style="29"/>
+    <col min="4359" max="4359" width="23.85546875" style="29" customWidth="1"/>
+    <col min="4360" max="4608" width="11.42578125" style="29"/>
+    <col min="4609" max="4609" width="43" style="29" customWidth="1"/>
+    <col min="4610" max="4611" width="11.42578125" style="29"/>
+    <col min="4612" max="4612" width="13.28515625" style="29" customWidth="1"/>
+    <col min="4613" max="4613" width="12.42578125" style="29" customWidth="1"/>
+    <col min="4614" max="4614" width="11.42578125" style="29"/>
+    <col min="4615" max="4615" width="23.85546875" style="29" customWidth="1"/>
+    <col min="4616" max="4864" width="11.42578125" style="29"/>
+    <col min="4865" max="4865" width="43" style="29" customWidth="1"/>
+    <col min="4866" max="4867" width="11.42578125" style="29"/>
+    <col min="4868" max="4868" width="13.28515625" style="29" customWidth="1"/>
+    <col min="4869" max="4869" width="12.42578125" style="29" customWidth="1"/>
+    <col min="4870" max="4870" width="11.42578125" style="29"/>
+    <col min="4871" max="4871" width="23.85546875" style="29" customWidth="1"/>
+    <col min="4872" max="5120" width="11.42578125" style="29"/>
+    <col min="5121" max="5121" width="43" style="29" customWidth="1"/>
+    <col min="5122" max="5123" width="11.42578125" style="29"/>
+    <col min="5124" max="5124" width="13.28515625" style="29" customWidth="1"/>
+    <col min="5125" max="5125" width="12.42578125" style="29" customWidth="1"/>
+    <col min="5126" max="5126" width="11.42578125" style="29"/>
+    <col min="5127" max="5127" width="23.85546875" style="29" customWidth="1"/>
+    <col min="5128" max="5376" width="11.42578125" style="29"/>
+    <col min="5377" max="5377" width="43" style="29" customWidth="1"/>
+    <col min="5378" max="5379" width="11.42578125" style="29"/>
+    <col min="5380" max="5380" width="13.28515625" style="29" customWidth="1"/>
+    <col min="5381" max="5381" width="12.42578125" style="29" customWidth="1"/>
+    <col min="5382" max="5382" width="11.42578125" style="29"/>
+    <col min="5383" max="5383" width="23.85546875" style="29" customWidth="1"/>
+    <col min="5384" max="5632" width="11.42578125" style="29"/>
+    <col min="5633" max="5633" width="43" style="29" customWidth="1"/>
+    <col min="5634" max="5635" width="11.42578125" style="29"/>
+    <col min="5636" max="5636" width="13.28515625" style="29" customWidth="1"/>
+    <col min="5637" max="5637" width="12.42578125" style="29" customWidth="1"/>
+    <col min="5638" max="5638" width="11.42578125" style="29"/>
+    <col min="5639" max="5639" width="23.85546875" style="29" customWidth="1"/>
+    <col min="5640" max="5888" width="11.42578125" style="29"/>
+    <col min="5889" max="5889" width="43" style="29" customWidth="1"/>
+    <col min="5890" max="5891" width="11.42578125" style="29"/>
+    <col min="5892" max="5892" width="13.28515625" style="29" customWidth="1"/>
+    <col min="5893" max="5893" width="12.42578125" style="29" customWidth="1"/>
+    <col min="5894" max="5894" width="11.42578125" style="29"/>
+    <col min="5895" max="5895" width="23.85546875" style="29" customWidth="1"/>
+    <col min="5896" max="6144" width="11.42578125" style="29"/>
+    <col min="6145" max="6145" width="43" style="29" customWidth="1"/>
+    <col min="6146" max="6147" width="11.42578125" style="29"/>
+    <col min="6148" max="6148" width="13.28515625" style="29" customWidth="1"/>
+    <col min="6149" max="6149" width="12.42578125" style="29" customWidth="1"/>
+    <col min="6150" max="6150" width="11.42578125" style="29"/>
+    <col min="6151" max="6151" width="23.85546875" style="29" customWidth="1"/>
+    <col min="6152" max="6400" width="11.42578125" style="29"/>
+    <col min="6401" max="6401" width="43" style="29" customWidth="1"/>
+    <col min="6402" max="6403" width="11.42578125" style="29"/>
+    <col min="6404" max="6404" width="13.28515625" style="29" customWidth="1"/>
+    <col min="6405" max="6405" width="12.42578125" style="29" customWidth="1"/>
+    <col min="6406" max="6406" width="11.42578125" style="29"/>
+    <col min="6407" max="6407" width="23.85546875" style="29" customWidth="1"/>
+    <col min="6408" max="6656" width="11.42578125" style="29"/>
+    <col min="6657" max="6657" width="43" style="29" customWidth="1"/>
+    <col min="6658" max="6659" width="11.42578125" style="29"/>
+    <col min="6660" max="6660" width="13.28515625" style="29" customWidth="1"/>
+    <col min="6661" max="6661" width="12.42578125" style="29" customWidth="1"/>
+    <col min="6662" max="6662" width="11.42578125" style="29"/>
+    <col min="6663" max="6663" width="23.85546875" style="29" customWidth="1"/>
+    <col min="6664" max="6912" width="11.42578125" style="29"/>
+    <col min="6913" max="6913" width="43" style="29" customWidth="1"/>
+    <col min="6914" max="6915" width="11.42578125" style="29"/>
+    <col min="6916" max="6916" width="13.28515625" style="29" customWidth="1"/>
+    <col min="6917" max="6917" width="12.42578125" style="29" customWidth="1"/>
+    <col min="6918" max="6918" width="11.42578125" style="29"/>
+    <col min="6919" max="6919" width="23.85546875" style="29" customWidth="1"/>
+    <col min="6920" max="7168" width="11.42578125" style="29"/>
+    <col min="7169" max="7169" width="43" style="29" customWidth="1"/>
+    <col min="7170" max="7171" width="11.42578125" style="29"/>
+    <col min="7172" max="7172" width="13.28515625" style="29" customWidth="1"/>
+    <col min="7173" max="7173" width="12.42578125" style="29" customWidth="1"/>
+    <col min="7174" max="7174" width="11.42578125" style="29"/>
+    <col min="7175" max="7175" width="23.85546875" style="29" customWidth="1"/>
+    <col min="7176" max="7424" width="11.42578125" style="29"/>
+    <col min="7425" max="7425" width="43" style="29" customWidth="1"/>
+    <col min="7426" max="7427" width="11.42578125" style="29"/>
+    <col min="7428" max="7428" width="13.28515625" style="29" customWidth="1"/>
+    <col min="7429" max="7429" width="12.42578125" style="29" customWidth="1"/>
+    <col min="7430" max="7430" width="11.42578125" style="29"/>
+    <col min="7431" max="7431" width="23.85546875" style="29" customWidth="1"/>
+    <col min="7432" max="7680" width="11.42578125" style="29"/>
+    <col min="7681" max="7681" width="43" style="29" customWidth="1"/>
+    <col min="7682" max="7683" width="11.42578125" style="29"/>
+    <col min="7684" max="7684" width="13.28515625" style="29" customWidth="1"/>
+    <col min="7685" max="7685" width="12.42578125" style="29" customWidth="1"/>
+    <col min="7686" max="7686" width="11.42578125" style="29"/>
+    <col min="7687" max="7687" width="23.85546875" style="29" customWidth="1"/>
+    <col min="7688" max="7936" width="11.42578125" style="29"/>
+    <col min="7937" max="7937" width="43" style="29" customWidth="1"/>
+    <col min="7938" max="7939" width="11.42578125" style="29"/>
+    <col min="7940" max="7940" width="13.28515625" style="29" customWidth="1"/>
+    <col min="7941" max="7941" width="12.42578125" style="29" customWidth="1"/>
+    <col min="7942" max="7942" width="11.42578125" style="29"/>
+    <col min="7943" max="7943" width="23.85546875" style="29" customWidth="1"/>
+    <col min="7944" max="8192" width="11.42578125" style="29"/>
+    <col min="8193" max="8193" width="43" style="29" customWidth="1"/>
+    <col min="8194" max="8195" width="11.42578125" style="29"/>
+    <col min="8196" max="8196" width="13.28515625" style="29" customWidth="1"/>
+    <col min="8197" max="8197" width="12.42578125" style="29" customWidth="1"/>
+    <col min="8198" max="8198" width="11.42578125" style="29"/>
+    <col min="8199" max="8199" width="23.85546875" style="29" customWidth="1"/>
+    <col min="8200" max="8448" width="11.42578125" style="29"/>
+    <col min="8449" max="8449" width="43" style="29" customWidth="1"/>
+    <col min="8450" max="8451" width="11.42578125" style="29"/>
+    <col min="8452" max="8452" width="13.28515625" style="29" customWidth="1"/>
+    <col min="8453" max="8453" width="12.42578125" style="29" customWidth="1"/>
+    <col min="8454" max="8454" width="11.42578125" style="29"/>
+    <col min="8455" max="8455" width="23.85546875" style="29" customWidth="1"/>
+    <col min="8456" max="8704" width="11.42578125" style="29"/>
+    <col min="8705" max="8705" width="43" style="29" customWidth="1"/>
+    <col min="8706" max="8707" width="11.42578125" style="29"/>
+    <col min="8708" max="8708" width="13.28515625" style="29" customWidth="1"/>
+    <col min="8709" max="8709" width="12.42578125" style="29" customWidth="1"/>
+    <col min="8710" max="8710" width="11.42578125" style="29"/>
+    <col min="8711" max="8711" width="23.85546875" style="29" customWidth="1"/>
+    <col min="8712" max="8960" width="11.42578125" style="29"/>
+    <col min="8961" max="8961" width="43" style="29" customWidth="1"/>
+    <col min="8962" max="8963" width="11.42578125" style="29"/>
+    <col min="8964" max="8964" width="13.28515625" style="29" customWidth="1"/>
+    <col min="8965" max="8965" width="12.42578125" style="29" customWidth="1"/>
+    <col min="8966" max="8966" width="11.42578125" style="29"/>
+    <col min="8967" max="8967" width="23.85546875" style="29" customWidth="1"/>
+    <col min="8968" max="9216" width="11.42578125" style="29"/>
+    <col min="9217" max="9217" width="43" style="29" customWidth="1"/>
+    <col min="9218" max="9219" width="11.42578125" style="29"/>
+    <col min="9220" max="9220" width="13.28515625" style="29" customWidth="1"/>
+    <col min="9221" max="9221" width="12.42578125" style="29" customWidth="1"/>
+    <col min="9222" max="9222" width="11.42578125" style="29"/>
+    <col min="9223" max="9223" width="23.85546875" style="29" customWidth="1"/>
+    <col min="9224" max="9472" width="11.42578125" style="29"/>
+    <col min="9473" max="9473" width="43" style="29" customWidth="1"/>
+    <col min="9474" max="9475" width="11.42578125" style="29"/>
+    <col min="9476" max="9476" width="13.28515625" style="29" customWidth="1"/>
+    <col min="9477" max="9477" width="12.42578125" style="29" customWidth="1"/>
+    <col min="9478" max="9478" width="11.42578125" style="29"/>
+    <col min="9479" max="9479" width="23.85546875" style="29" customWidth="1"/>
+    <col min="9480" max="9728" width="11.42578125" style="29"/>
+    <col min="9729" max="9729" width="43" style="29" customWidth="1"/>
+    <col min="9730" max="9731" width="11.42578125" style="29"/>
+    <col min="9732" max="9732" width="13.28515625" style="29" customWidth="1"/>
+    <col min="9733" max="9733" width="12.42578125" style="29" customWidth="1"/>
+    <col min="9734" max="9734" width="11.42578125" style="29"/>
+    <col min="9735" max="9735" width="23.85546875" style="29" customWidth="1"/>
+    <col min="9736" max="9984" width="11.42578125" style="29"/>
+    <col min="9985" max="9985" width="43" style="29" customWidth="1"/>
+    <col min="9986" max="9987" width="11.42578125" style="29"/>
+    <col min="9988" max="9988" width="13.28515625" style="29" customWidth="1"/>
+    <col min="9989" max="9989" width="12.42578125" style="29" customWidth="1"/>
+    <col min="9990" max="9990" width="11.42578125" style="29"/>
+    <col min="9991" max="9991" width="23.85546875" style="29" customWidth="1"/>
+    <col min="9992" max="10240" width="11.42578125" style="29"/>
+    <col min="10241" max="10241" width="43" style="29" customWidth="1"/>
+    <col min="10242" max="10243" width="11.42578125" style="29"/>
+    <col min="10244" max="10244" width="13.28515625" style="29" customWidth="1"/>
+    <col min="10245" max="10245" width="12.42578125" style="29" customWidth="1"/>
+    <col min="10246" max="10246" width="11.42578125" style="29"/>
+    <col min="10247" max="10247" width="23.85546875" style="29" customWidth="1"/>
+    <col min="10248" max="10496" width="11.42578125" style="29"/>
+    <col min="10497" max="10497" width="43" style="29" customWidth="1"/>
+    <col min="10498" max="10499" width="11.42578125" style="29"/>
+    <col min="10500" max="10500" width="13.28515625" style="29" customWidth="1"/>
+    <col min="10501" max="10501" width="12.42578125" style="29" customWidth="1"/>
+    <col min="10502" max="10502" width="11.42578125" style="29"/>
+    <col min="10503" max="10503" width="23.85546875" style="29" customWidth="1"/>
+    <col min="10504" max="10752" width="11.42578125" style="29"/>
+    <col min="10753" max="10753" width="43" style="29" customWidth="1"/>
+    <col min="10754" max="10755" width="11.42578125" style="29"/>
+    <col min="10756" max="10756" width="13.28515625" style="29" customWidth="1"/>
+    <col min="10757" max="10757" width="12.42578125" style="29" customWidth="1"/>
+    <col min="10758" max="10758" width="11.42578125" style="29"/>
+    <col min="10759" max="10759" width="23.85546875" style="29" customWidth="1"/>
+    <col min="10760" max="11008" width="11.42578125" style="29"/>
+    <col min="11009" max="11009" width="43" style="29" customWidth="1"/>
+    <col min="11010" max="11011" width="11.42578125" style="29"/>
+    <col min="11012" max="11012" width="13.28515625" style="29" customWidth="1"/>
+    <col min="11013" max="11013" width="12.42578125" style="29" customWidth="1"/>
+    <col min="11014" max="11014" width="11.42578125" style="29"/>
+    <col min="11015" max="11015" width="23.85546875" style="29" customWidth="1"/>
+    <col min="11016" max="11264" width="11.42578125" style="29"/>
+    <col min="11265" max="11265" width="43" style="29" customWidth="1"/>
+    <col min="11266" max="11267" width="11.42578125" style="29"/>
+    <col min="11268" max="11268" width="13.28515625" style="29" customWidth="1"/>
+    <col min="11269" max="11269" width="12.42578125" style="29" customWidth="1"/>
+    <col min="11270" max="11270" width="11.42578125" style="29"/>
+    <col min="11271" max="11271" width="23.85546875" style="29" customWidth="1"/>
+    <col min="11272" max="11520" width="11.42578125" style="29"/>
+    <col min="11521" max="11521" width="43" style="29" customWidth="1"/>
+    <col min="11522" max="11523" width="11.42578125" style="29"/>
+    <col min="11524" max="11524" width="13.28515625" style="29" customWidth="1"/>
+    <col min="11525" max="11525" width="12.42578125" style="29" customWidth="1"/>
+    <col min="11526" max="11526" width="11.42578125" style="29"/>
+    <col min="11527" max="11527" width="23.85546875" style="29" customWidth="1"/>
+    <col min="11528" max="11776" width="11.42578125" style="29"/>
+    <col min="11777" max="11777" width="43" style="29" customWidth="1"/>
+    <col min="11778" max="11779" width="11.42578125" style="29"/>
+    <col min="11780" max="11780" width="13.28515625" style="29" customWidth="1"/>
+    <col min="11781" max="11781" width="12.42578125" style="29" customWidth="1"/>
+    <col min="11782" max="11782" width="11.42578125" style="29"/>
+    <col min="11783" max="11783" width="23.85546875" style="29" customWidth="1"/>
+    <col min="11784" max="12032" width="11.42578125" style="29"/>
+    <col min="12033" max="12033" width="43" style="29" customWidth="1"/>
+    <col min="12034" max="12035" width="11.42578125" style="29"/>
+    <col min="12036" max="12036" width="13.28515625" style="29" customWidth="1"/>
+    <col min="12037" max="12037" width="12.42578125" style="29" customWidth="1"/>
+    <col min="12038" max="12038" width="11.42578125" style="29"/>
+    <col min="12039" max="12039" width="23.85546875" style="29" customWidth="1"/>
+    <col min="12040" max="12288" width="11.42578125" style="29"/>
+    <col min="12289" max="12289" width="43" style="29" customWidth="1"/>
+    <col min="12290" max="12291" width="11.42578125" style="29"/>
+    <col min="12292" max="12292" width="13.28515625" style="29" customWidth="1"/>
+    <col min="12293" max="12293" width="12.42578125" style="29" customWidth="1"/>
+    <col min="12294" max="12294" width="11.42578125" style="29"/>
+    <col min="12295" max="12295" width="23.85546875" style="29" customWidth="1"/>
+    <col min="12296" max="12544" width="11.42578125" style="29"/>
+    <col min="12545" max="12545" width="43" style="29" customWidth="1"/>
+    <col min="12546" max="12547" width="11.42578125" style="29"/>
+    <col min="12548" max="12548" width="13.28515625" style="29" customWidth="1"/>
+    <col min="12549" max="12549" width="12.42578125" style="29" customWidth="1"/>
+    <col min="12550" max="12550" width="11.42578125" style="29"/>
+    <col min="12551" max="12551" width="23.85546875" style="29" customWidth="1"/>
+    <col min="12552" max="12800" width="11.42578125" style="29"/>
+    <col min="12801" max="12801" width="43" style="29" customWidth="1"/>
+    <col min="12802" max="12803" width="11.42578125" style="29"/>
+    <col min="12804" max="12804" width="13.28515625" style="29" customWidth="1"/>
+    <col min="12805" max="12805" width="12.42578125" style="29" customWidth="1"/>
+    <col min="12806" max="12806" width="11.42578125" style="29"/>
+    <col min="12807" max="12807" width="23.85546875" style="29" customWidth="1"/>
+    <col min="12808" max="13056" width="11.42578125" style="29"/>
+    <col min="13057" max="13057" width="43" style="29" customWidth="1"/>
+    <col min="13058" max="13059" width="11.42578125" style="29"/>
+    <col min="13060" max="13060" width="13.28515625" style="29" customWidth="1"/>
+    <col min="13061" max="13061" width="12.42578125" style="29" customWidth="1"/>
+    <col min="13062" max="13062" width="11.42578125" style="29"/>
+    <col min="13063" max="13063" width="23.85546875" style="29" customWidth="1"/>
+    <col min="13064" max="13312" width="11.42578125" style="29"/>
+    <col min="13313" max="13313" width="43" style="29" customWidth="1"/>
+    <col min="13314" max="13315" width="11.42578125" style="29"/>
+    <col min="13316" max="13316" width="13.28515625" style="29" customWidth="1"/>
+    <col min="13317" max="13317" width="12.42578125" style="29" customWidth="1"/>
+    <col min="13318" max="13318" width="11.42578125" style="29"/>
+    <col min="13319" max="13319" width="23.85546875" style="29" customWidth="1"/>
+    <col min="13320" max="13568" width="11.42578125" style="29"/>
+    <col min="13569" max="13569" width="43" style="29" customWidth="1"/>
+    <col min="13570" max="13571" width="11.42578125" style="29"/>
+    <col min="13572" max="13572" width="13.28515625" style="29" customWidth="1"/>
+    <col min="13573" max="13573" width="12.42578125" style="29" customWidth="1"/>
+    <col min="13574" max="13574" width="11.42578125" style="29"/>
+    <col min="13575" max="13575" width="23.85546875" style="29" customWidth="1"/>
+    <col min="13576" max="13824" width="11.42578125" style="29"/>
+    <col min="13825" max="13825" width="43" style="29" customWidth="1"/>
+    <col min="13826" max="13827" width="11.42578125" style="29"/>
+    <col min="13828" max="13828" width="13.28515625" style="29" customWidth="1"/>
+    <col min="13829" max="13829" width="12.42578125" style="29" customWidth="1"/>
+    <col min="13830" max="13830" width="11.42578125" style="29"/>
+    <col min="13831" max="13831" width="23.85546875" style="29" customWidth="1"/>
+    <col min="13832" max="14080" width="11.42578125" style="29"/>
+    <col min="14081" max="14081" width="43" style="29" customWidth="1"/>
+    <col min="14082" max="14083" width="11.42578125" style="29"/>
+    <col min="14084" max="14084" width="13.28515625" style="29" customWidth="1"/>
+    <col min="14085" max="14085" width="12.42578125" style="29" customWidth="1"/>
+    <col min="14086" max="14086" width="11.42578125" style="29"/>
+    <col min="14087" max="14087" width="23.85546875" style="29" customWidth="1"/>
+    <col min="14088" max="14336" width="11.42578125" style="29"/>
+    <col min="14337" max="14337" width="43" style="29" customWidth="1"/>
+    <col min="14338" max="14339" width="11.42578125" style="29"/>
+    <col min="14340" max="14340" width="13.28515625" style="29" customWidth="1"/>
+    <col min="14341" max="14341" width="12.42578125" style="29" customWidth="1"/>
+    <col min="14342" max="14342" width="11.42578125" style="29"/>
+    <col min="14343" max="14343" width="23.85546875" style="29" customWidth="1"/>
+    <col min="14344" max="14592" width="11.42578125" style="29"/>
+    <col min="14593" max="14593" width="43" style="29" customWidth="1"/>
+    <col min="14594" max="14595" width="11.42578125" style="29"/>
+    <col min="14596" max="14596" width="13.28515625" style="29" customWidth="1"/>
+    <col min="14597" max="14597" width="12.42578125" style="29" customWidth="1"/>
+    <col min="14598" max="14598" width="11.42578125" style="29"/>
+    <col min="14599" max="14599" width="23.85546875" style="29" customWidth="1"/>
+    <col min="14600" max="14848" width="11.42578125" style="29"/>
+    <col min="14849" max="14849" width="43" style="29" customWidth="1"/>
+    <col min="14850" max="14851" width="11.42578125" style="29"/>
+    <col min="14852" max="14852" width="13.28515625" style="29" customWidth="1"/>
+    <col min="14853" max="14853" width="12.42578125" style="29" customWidth="1"/>
+    <col min="14854" max="14854" width="11.42578125" style="29"/>
+    <col min="14855" max="14855" width="23.85546875" style="29" customWidth="1"/>
+    <col min="14856" max="15104" width="11.42578125" style="29"/>
+    <col min="15105" max="15105" width="43" style="29" customWidth="1"/>
+    <col min="15106" max="15107" width="11.42578125" style="29"/>
+    <col min="15108" max="15108" width="13.28515625" style="29" customWidth="1"/>
+    <col min="15109" max="15109" width="12.42578125" style="29" customWidth="1"/>
+    <col min="15110" max="15110" width="11.42578125" style="29"/>
+    <col min="15111" max="15111" width="23.85546875" style="29" customWidth="1"/>
+    <col min="15112" max="15360" width="11.42578125" style="29"/>
+    <col min="15361" max="15361" width="43" style="29" customWidth="1"/>
+    <col min="15362" max="15363" width="11.42578125" style="29"/>
+    <col min="15364" max="15364" width="13.28515625" style="29" customWidth="1"/>
+    <col min="15365" max="15365" width="12.42578125" style="29" customWidth="1"/>
+    <col min="15366" max="15366" width="11.42578125" style="29"/>
+    <col min="15367" max="15367" width="23.85546875" style="29" customWidth="1"/>
+    <col min="15368" max="15616" width="11.42578125" style="29"/>
+    <col min="15617" max="15617" width="43" style="29" customWidth="1"/>
+    <col min="15618" max="15619" width="11.42578125" style="29"/>
+    <col min="15620" max="15620" width="13.28515625" style="29" customWidth="1"/>
+    <col min="15621" max="15621" width="12.42578125" style="29" customWidth="1"/>
+    <col min="15622" max="15622" width="11.42578125" style="29"/>
+    <col min="15623" max="15623" width="23.85546875" style="29" customWidth="1"/>
+    <col min="15624" max="15872" width="11.42578125" style="29"/>
+    <col min="15873" max="15873" width="43" style="29" customWidth="1"/>
+    <col min="15874" max="15875" width="11.42578125" style="29"/>
+    <col min="15876" max="15876" width="13.28515625" style="29" customWidth="1"/>
+    <col min="15877" max="15877" width="12.42578125" style="29" customWidth="1"/>
+    <col min="15878" max="15878" width="11.42578125" style="29"/>
+    <col min="15879" max="15879" width="23.85546875" style="29" customWidth="1"/>
+    <col min="15880" max="16128" width="11.42578125" style="29"/>
+    <col min="16129" max="16129" width="43" style="29" customWidth="1"/>
+    <col min="16130" max="16131" width="11.42578125" style="29"/>
+    <col min="16132" max="16132" width="13.28515625" style="29" customWidth="1"/>
+    <col min="16133" max="16133" width="12.42578125" style="29" customWidth="1"/>
+    <col min="16134" max="16134" width="11.42578125" style="29"/>
+    <col min="16135" max="16135" width="23.85546875" style="29" customWidth="1"/>
+    <col min="16136" max="16384" width="11.42578125" style="29"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="34" customFormat="1">
-      <c r="A1" s="33"/>
-      <c r="B1" s="27" t="s">
+    <row r="1" spans="1:7" s="25" customFormat="1">
+      <c r="A1" s="48"/>
+      <c r="B1" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="29"/>
-    </row>
-    <row r="2" spans="1:7" s="34" customFormat="1">
-      <c r="A2" s="33"/>
-      <c r="B2" s="31" t="s">
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="51"/>
+    </row>
+    <row r="2" spans="1:7" s="25" customFormat="1">
+      <c r="A2" s="48"/>
+      <c r="B2" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="C2" s="54" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25" t="s">
+      <c r="D2" s="54"/>
+      <c r="E2" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="25"/>
-      <c r="G2" s="26"/>
-    </row>
-    <row r="3" spans="1:7" s="34" customFormat="1">
-      <c r="A3" s="33"/>
-      <c r="B3" s="31"/>
-      <c r="C3" s="25" t="s">
+      <c r="F2" s="54"/>
+      <c r="G2" s="55"/>
+    </row>
+    <row r="3" spans="1:7" s="25" customFormat="1">
+      <c r="A3" s="48"/>
+      <c r="B3" s="52"/>
+      <c r="C3" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="25" t="s">
+      <c r="D3" s="54" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="25" t="s">
+      <c r="E3" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="25" t="s">
+      <c r="F3" s="54" t="s">
         <v>25</v>
       </c>
-      <c r="G3" s="26"/>
-    </row>
-    <row r="4" spans="1:7" s="34" customFormat="1" ht="16.5" thickBot="1">
-      <c r="A4" s="33"/>
-      <c r="B4" s="32"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
+      <c r="G3" s="55"/>
+    </row>
+    <row r="4" spans="1:7" s="25" customFormat="1" ht="16.5" thickBot="1">
+      <c r="A4" s="48"/>
+      <c r="B4" s="53"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
+      <c r="E4" s="56"/>
       <c r="F4" s="24" t="s">
         <v>1</v>
       </c>
@@ -2025,20 +2128,20 @@
       <c r="A5" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="35"/>
-      <c r="C5" s="36" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="36" t="s">
-        <v>2</v>
-      </c>
-      <c r="E5" s="36" t="s">
-        <v>2</v>
-      </c>
-      <c r="F5" s="36" t="s">
-        <v>2</v>
-      </c>
-      <c r="G5" s="37" t="s">
+      <c r="B5" s="26"/>
+      <c r="C5" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5" s="28" t="s">
         <v>2</v>
       </c>
     </row>
@@ -2046,16 +2149,16 @@
       <c r="A6" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="39"/>
-      <c r="C6" s="40"/>
-      <c r="D6" s="40"/>
-      <c r="E6" s="40" t="s">
-        <v>2</v>
-      </c>
-      <c r="F6" s="40" t="s">
-        <v>2</v>
-      </c>
-      <c r="G6" s="41" t="s">
+      <c r="B6" s="30"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="G6" s="32" t="s">
         <v>2</v>
       </c>
     </row>
@@ -2063,61 +2166,61 @@
       <c r="A7" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="42" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" s="43"/>
-      <c r="D7" s="43" t="s">
-        <v>2</v>
-      </c>
-      <c r="E7" s="43"/>
-      <c r="F7" s="43" t="s">
-        <v>2</v>
-      </c>
-      <c r="G7" s="44" t="s">
+      <c r="B7" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="34"/>
+      <c r="D7" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="34"/>
+      <c r="F7" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="G7" s="35" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="16.5" thickBot="1">
-      <c r="A8" s="48"/>
-      <c r="B8" s="49"/>
-      <c r="C8" s="49"/>
-      <c r="D8" s="49"/>
-      <c r="E8" s="49"/>
-      <c r="F8" s="49"/>
-      <c r="G8" s="49"/>
+      <c r="A8" s="39"/>
+      <c r="B8" s="40"/>
+      <c r="C8" s="40"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="40"/>
     </row>
     <row r="9" spans="1:7" ht="16.5" thickBot="1">
-      <c r="A9" s="50" t="s">
+      <c r="A9" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="49"/>
-      <c r="C9" s="49"/>
-      <c r="D9" s="49"/>
-      <c r="E9" s="49"/>
-      <c r="F9" s="49"/>
-      <c r="G9" s="49"/>
+      <c r="B9" s="40"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="40"/>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="45" t="s">
+      <c r="B10" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="36">
+      <c r="C10" s="27">
         <v>0</v>
       </c>
-      <c r="D10" s="36" t="s">
+      <c r="D10" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="E10" s="36">
+      <c r="E10" s="27">
         <v>0</v>
       </c>
-      <c r="F10" s="36" t="s">
+      <c r="F10" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="G10" s="37" t="s">
+      <c r="G10" s="28" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2125,22 +2228,22 @@
       <c r="A11" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="46" t="s">
+      <c r="B11" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="40">
+      <c r="C11" s="31">
         <v>0</v>
       </c>
-      <c r="D11" s="40" t="s">
+      <c r="D11" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="E11" s="40">
+      <c r="E11" s="31">
         <v>0</v>
       </c>
-      <c r="F11" s="40" t="s">
+      <c r="F11" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="G11" s="41" t="s">
+      <c r="G11" s="32" t="s">
         <v>35</v>
       </c>
     </row>
@@ -2148,22 +2251,22 @@
       <c r="A12" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="46" t="s">
+      <c r="B12" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="40">
+      <c r="C12" s="31">
         <v>0</v>
       </c>
-      <c r="D12" s="40" t="s">
+      <c r="D12" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="E12" s="40">
+      <c r="E12" s="31">
         <v>0</v>
       </c>
-      <c r="F12" s="40" t="s">
+      <c r="F12" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="G12" s="41" t="s">
+      <c r="G12" s="32" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2171,22 +2274,22 @@
       <c r="A13" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="46" t="s">
+      <c r="B13" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="40">
+      <c r="C13" s="31">
         <v>0</v>
       </c>
-      <c r="D13" s="40" t="s">
+      <c r="D13" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="E13" s="40">
+      <c r="E13" s="31">
         <v>0</v>
       </c>
-      <c r="F13" s="40" t="s">
+      <c r="F13" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="G13" s="41" t="s">
+      <c r="G13" s="32" t="s">
         <v>35</v>
       </c>
     </row>
@@ -2194,22 +2297,22 @@
       <c r="A14" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="B14" s="46" t="s">
+      <c r="B14" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="C14" s="40" t="s">
+      <c r="C14" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="40" t="s">
+      <c r="D14" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="E14" s="40" t="s">
+      <c r="E14" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="F14" s="40" t="s">
+      <c r="F14" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="G14" s="41" t="s">
+      <c r="G14" s="32" t="s">
         <v>35</v>
       </c>
     </row>
@@ -2217,22 +2320,22 @@
       <c r="A15" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="46" t="s">
+      <c r="B15" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="40">
+      <c r="C15" s="31">
         <v>0</v>
       </c>
-      <c r="D15" s="40" t="s">
+      <c r="D15" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="E15" s="40">
+      <c r="E15" s="31">
         <v>0</v>
       </c>
-      <c r="F15" s="40" t="s">
+      <c r="F15" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="G15" s="41" t="s">
+      <c r="G15" s="32" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2240,16 +2343,16 @@
       <c r="A16" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="B16" s="46"/>
-      <c r="C16" s="40"/>
-      <c r="D16" s="40"/>
-      <c r="E16" s="40" t="s">
+      <c r="B16" s="37"/>
+      <c r="C16" s="31"/>
+      <c r="D16" s="31"/>
+      <c r="E16" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="F16" s="40" t="s">
+      <c r="F16" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="G16" s="41" t="s">
+      <c r="G16" s="32" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2257,16 +2360,16 @@
       <c r="A17" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="B17" s="46"/>
-      <c r="C17" s="40"/>
-      <c r="D17" s="40"/>
-      <c r="E17" s="40" t="s">
+      <c r="B17" s="37"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="F17" s="40" t="s">
+      <c r="F17" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="G17" s="41" t="s">
+      <c r="G17" s="32" t="s">
         <v>35</v>
       </c>
     </row>
@@ -2274,16 +2377,16 @@
       <c r="A18" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="B18" s="46"/>
-      <c r="C18" s="40"/>
-      <c r="D18" s="40"/>
-      <c r="E18" s="40" t="s">
+      <c r="B18" s="37"/>
+      <c r="C18" s="31"/>
+      <c r="D18" s="31"/>
+      <c r="E18" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="F18" s="40" t="s">
+      <c r="F18" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="G18" s="41" t="s">
+      <c r="G18" s="32" t="s">
         <v>35</v>
       </c>
     </row>
@@ -2291,16 +2394,16 @@
       <c r="A19" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="B19" s="47"/>
-      <c r="C19" s="43"/>
-      <c r="D19" s="43"/>
-      <c r="E19" s="43" t="s">
+      <c r="B19" s="38"/>
+      <c r="C19" s="34"/>
+      <c r="D19" s="34"/>
+      <c r="E19" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="F19" s="43" t="s">
+      <c r="F19" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="G19" s="44" t="s">
+      <c r="G19" s="35" t="s">
         <v>35</v>
       </c>
     </row>
@@ -2321,4 +2424,200 @@
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="20.28515625" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="51.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="16.5" thickBot="1">
+      <c r="A1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="47" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="45" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="46" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="45" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="46" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" s="42" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="43" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="46" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="42" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="43" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="46" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" s="42" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" s="43" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="46" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="42" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="43" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="20.28515625" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="54.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="16.5" thickBot="1">
+      <c r="A1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="47" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="45" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="46" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="45" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="46" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" s="42" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="43" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="46" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="42" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="43" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="46" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" s="42" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" s="43" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="46" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="42" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="43" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
[297142] Provide more documentation
https://bugs.eclipse.org/bugs/show_bug.cgi?id=297142
</commit_message>
<xml_diff>
--- a/plugins/org.eclipse.emf.cdo.doc/Tables.xlsx
+++ b/plugins/org.eclipse.emf.cdo.doc/Tables.xlsx
@@ -4,18 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="28515" windowHeight="14025" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="28515" windowHeight="14025" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="StoreFeatures" sheetId="1" r:id="rId1"/>
     <sheet name="MappingStrategies" sheetId="3" r:id="rId2"/>
+    <sheet name="AuditingSupport" sheetId="4" r:id="rId3"/>
+    <sheet name="BranchingSupport" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="58">
   <si>
     <t>Branching</t>
   </si>
@@ -147,13 +149,88 @@
   </si>
   <si>
     <t>- read access in branch</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>Store Type</t>
+  </si>
+  <si>
+    <t>DBStore</t>
+  </si>
+  <si>
+    <t>MEMStore</t>
+  </si>
+  <si>
+    <t>HibernateStore</t>
+  </si>
+  <si>
+    <t>ObjectivityStore</t>
+  </si>
+  <si>
+    <t>DB4OStore</t>
+  </si>
+  <si>
+    <t>MongoDBStore</t>
+  </si>
+  <si>
+    <r>
+      <t>true</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF333333"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, if the used mapping strategy supports audits</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">true </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF333333"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>/ false</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>true</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF333333"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, if the used mapping strategy supports branches</t>
+    </r>
+  </si>
+  <si>
+    <t>Allowed Values</t>
+  </si>
+  <si>
+    <t>Default Value</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -199,6 +276,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -753,7 +836,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -827,86 +910,104 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Excel Built-in Normal" xfId="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -921,9 +1022,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Larissa">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -961,7 +1062,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Larissa">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1031,7 +1132,7 @@
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Larissa">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1207,9 +1308,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="26.7109375" style="19" customWidth="1"/>
     <col min="2" max="2" width="10" style="5" customWidth="1"/>
@@ -1509,511 +1612,511 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="43" style="38" customWidth="1"/>
-    <col min="2" max="3" width="11.42578125" style="38"/>
-    <col min="4" max="4" width="13.28515625" style="38" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" style="38" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" style="38"/>
-    <col min="7" max="7" width="23.85546875" style="38" customWidth="1"/>
-    <col min="8" max="256" width="11.42578125" style="38"/>
-    <col min="257" max="257" width="43" style="38" customWidth="1"/>
-    <col min="258" max="259" width="11.42578125" style="38"/>
-    <col min="260" max="260" width="13.28515625" style="38" customWidth="1"/>
-    <col min="261" max="261" width="12.42578125" style="38" customWidth="1"/>
-    <col min="262" max="262" width="11.42578125" style="38"/>
-    <col min="263" max="263" width="23.85546875" style="38" customWidth="1"/>
-    <col min="264" max="512" width="11.42578125" style="38"/>
-    <col min="513" max="513" width="43" style="38" customWidth="1"/>
-    <col min="514" max="515" width="11.42578125" style="38"/>
-    <col min="516" max="516" width="13.28515625" style="38" customWidth="1"/>
-    <col min="517" max="517" width="12.42578125" style="38" customWidth="1"/>
-    <col min="518" max="518" width="11.42578125" style="38"/>
-    <col min="519" max="519" width="23.85546875" style="38" customWidth="1"/>
-    <col min="520" max="768" width="11.42578125" style="38"/>
-    <col min="769" max="769" width="43" style="38" customWidth="1"/>
-    <col min="770" max="771" width="11.42578125" style="38"/>
-    <col min="772" max="772" width="13.28515625" style="38" customWidth="1"/>
-    <col min="773" max="773" width="12.42578125" style="38" customWidth="1"/>
-    <col min="774" max="774" width="11.42578125" style="38"/>
-    <col min="775" max="775" width="23.85546875" style="38" customWidth="1"/>
-    <col min="776" max="1024" width="11.42578125" style="38"/>
-    <col min="1025" max="1025" width="43" style="38" customWidth="1"/>
-    <col min="1026" max="1027" width="11.42578125" style="38"/>
-    <col min="1028" max="1028" width="13.28515625" style="38" customWidth="1"/>
-    <col min="1029" max="1029" width="12.42578125" style="38" customWidth="1"/>
-    <col min="1030" max="1030" width="11.42578125" style="38"/>
-    <col min="1031" max="1031" width="23.85546875" style="38" customWidth="1"/>
-    <col min="1032" max="1280" width="11.42578125" style="38"/>
-    <col min="1281" max="1281" width="43" style="38" customWidth="1"/>
-    <col min="1282" max="1283" width="11.42578125" style="38"/>
-    <col min="1284" max="1284" width="13.28515625" style="38" customWidth="1"/>
-    <col min="1285" max="1285" width="12.42578125" style="38" customWidth="1"/>
-    <col min="1286" max="1286" width="11.42578125" style="38"/>
-    <col min="1287" max="1287" width="23.85546875" style="38" customWidth="1"/>
-    <col min="1288" max="1536" width="11.42578125" style="38"/>
-    <col min="1537" max="1537" width="43" style="38" customWidth="1"/>
-    <col min="1538" max="1539" width="11.42578125" style="38"/>
-    <col min="1540" max="1540" width="13.28515625" style="38" customWidth="1"/>
-    <col min="1541" max="1541" width="12.42578125" style="38" customWidth="1"/>
-    <col min="1542" max="1542" width="11.42578125" style="38"/>
-    <col min="1543" max="1543" width="23.85546875" style="38" customWidth="1"/>
-    <col min="1544" max="1792" width="11.42578125" style="38"/>
-    <col min="1793" max="1793" width="43" style="38" customWidth="1"/>
-    <col min="1794" max="1795" width="11.42578125" style="38"/>
-    <col min="1796" max="1796" width="13.28515625" style="38" customWidth="1"/>
-    <col min="1797" max="1797" width="12.42578125" style="38" customWidth="1"/>
-    <col min="1798" max="1798" width="11.42578125" style="38"/>
-    <col min="1799" max="1799" width="23.85546875" style="38" customWidth="1"/>
-    <col min="1800" max="2048" width="11.42578125" style="38"/>
-    <col min="2049" max="2049" width="43" style="38" customWidth="1"/>
-    <col min="2050" max="2051" width="11.42578125" style="38"/>
-    <col min="2052" max="2052" width="13.28515625" style="38" customWidth="1"/>
-    <col min="2053" max="2053" width="12.42578125" style="38" customWidth="1"/>
-    <col min="2054" max="2054" width="11.42578125" style="38"/>
-    <col min="2055" max="2055" width="23.85546875" style="38" customWidth="1"/>
-    <col min="2056" max="2304" width="11.42578125" style="38"/>
-    <col min="2305" max="2305" width="43" style="38" customWidth="1"/>
-    <col min="2306" max="2307" width="11.42578125" style="38"/>
-    <col min="2308" max="2308" width="13.28515625" style="38" customWidth="1"/>
-    <col min="2309" max="2309" width="12.42578125" style="38" customWidth="1"/>
-    <col min="2310" max="2310" width="11.42578125" style="38"/>
-    <col min="2311" max="2311" width="23.85546875" style="38" customWidth="1"/>
-    <col min="2312" max="2560" width="11.42578125" style="38"/>
-    <col min="2561" max="2561" width="43" style="38" customWidth="1"/>
-    <col min="2562" max="2563" width="11.42578125" style="38"/>
-    <col min="2564" max="2564" width="13.28515625" style="38" customWidth="1"/>
-    <col min="2565" max="2565" width="12.42578125" style="38" customWidth="1"/>
-    <col min="2566" max="2566" width="11.42578125" style="38"/>
-    <col min="2567" max="2567" width="23.85546875" style="38" customWidth="1"/>
-    <col min="2568" max="2816" width="11.42578125" style="38"/>
-    <col min="2817" max="2817" width="43" style="38" customWidth="1"/>
-    <col min="2818" max="2819" width="11.42578125" style="38"/>
-    <col min="2820" max="2820" width="13.28515625" style="38" customWidth="1"/>
-    <col min="2821" max="2821" width="12.42578125" style="38" customWidth="1"/>
-    <col min="2822" max="2822" width="11.42578125" style="38"/>
-    <col min="2823" max="2823" width="23.85546875" style="38" customWidth="1"/>
-    <col min="2824" max="3072" width="11.42578125" style="38"/>
-    <col min="3073" max="3073" width="43" style="38" customWidth="1"/>
-    <col min="3074" max="3075" width="11.42578125" style="38"/>
-    <col min="3076" max="3076" width="13.28515625" style="38" customWidth="1"/>
-    <col min="3077" max="3077" width="12.42578125" style="38" customWidth="1"/>
-    <col min="3078" max="3078" width="11.42578125" style="38"/>
-    <col min="3079" max="3079" width="23.85546875" style="38" customWidth="1"/>
-    <col min="3080" max="3328" width="11.42578125" style="38"/>
-    <col min="3329" max="3329" width="43" style="38" customWidth="1"/>
-    <col min="3330" max="3331" width="11.42578125" style="38"/>
-    <col min="3332" max="3332" width="13.28515625" style="38" customWidth="1"/>
-    <col min="3333" max="3333" width="12.42578125" style="38" customWidth="1"/>
-    <col min="3334" max="3334" width="11.42578125" style="38"/>
-    <col min="3335" max="3335" width="23.85546875" style="38" customWidth="1"/>
-    <col min="3336" max="3584" width="11.42578125" style="38"/>
-    <col min="3585" max="3585" width="43" style="38" customWidth="1"/>
-    <col min="3586" max="3587" width="11.42578125" style="38"/>
-    <col min="3588" max="3588" width="13.28515625" style="38" customWidth="1"/>
-    <col min="3589" max="3589" width="12.42578125" style="38" customWidth="1"/>
-    <col min="3590" max="3590" width="11.42578125" style="38"/>
-    <col min="3591" max="3591" width="23.85546875" style="38" customWidth="1"/>
-    <col min="3592" max="3840" width="11.42578125" style="38"/>
-    <col min="3841" max="3841" width="43" style="38" customWidth="1"/>
-    <col min="3842" max="3843" width="11.42578125" style="38"/>
-    <col min="3844" max="3844" width="13.28515625" style="38" customWidth="1"/>
-    <col min="3845" max="3845" width="12.42578125" style="38" customWidth="1"/>
-    <col min="3846" max="3846" width="11.42578125" style="38"/>
-    <col min="3847" max="3847" width="23.85546875" style="38" customWidth="1"/>
-    <col min="3848" max="4096" width="11.42578125" style="38"/>
-    <col min="4097" max="4097" width="43" style="38" customWidth="1"/>
-    <col min="4098" max="4099" width="11.42578125" style="38"/>
-    <col min="4100" max="4100" width="13.28515625" style="38" customWidth="1"/>
-    <col min="4101" max="4101" width="12.42578125" style="38" customWidth="1"/>
-    <col min="4102" max="4102" width="11.42578125" style="38"/>
-    <col min="4103" max="4103" width="23.85546875" style="38" customWidth="1"/>
-    <col min="4104" max="4352" width="11.42578125" style="38"/>
-    <col min="4353" max="4353" width="43" style="38" customWidth="1"/>
-    <col min="4354" max="4355" width="11.42578125" style="38"/>
-    <col min="4356" max="4356" width="13.28515625" style="38" customWidth="1"/>
-    <col min="4357" max="4357" width="12.42578125" style="38" customWidth="1"/>
-    <col min="4358" max="4358" width="11.42578125" style="38"/>
-    <col min="4359" max="4359" width="23.85546875" style="38" customWidth="1"/>
-    <col min="4360" max="4608" width="11.42578125" style="38"/>
-    <col min="4609" max="4609" width="43" style="38" customWidth="1"/>
-    <col min="4610" max="4611" width="11.42578125" style="38"/>
-    <col min="4612" max="4612" width="13.28515625" style="38" customWidth="1"/>
-    <col min="4613" max="4613" width="12.42578125" style="38" customWidth="1"/>
-    <col min="4614" max="4614" width="11.42578125" style="38"/>
-    <col min="4615" max="4615" width="23.85546875" style="38" customWidth="1"/>
-    <col min="4616" max="4864" width="11.42578125" style="38"/>
-    <col min="4865" max="4865" width="43" style="38" customWidth="1"/>
-    <col min="4866" max="4867" width="11.42578125" style="38"/>
-    <col min="4868" max="4868" width="13.28515625" style="38" customWidth="1"/>
-    <col min="4869" max="4869" width="12.42578125" style="38" customWidth="1"/>
-    <col min="4870" max="4870" width="11.42578125" style="38"/>
-    <col min="4871" max="4871" width="23.85546875" style="38" customWidth="1"/>
-    <col min="4872" max="5120" width="11.42578125" style="38"/>
-    <col min="5121" max="5121" width="43" style="38" customWidth="1"/>
-    <col min="5122" max="5123" width="11.42578125" style="38"/>
-    <col min="5124" max="5124" width="13.28515625" style="38" customWidth="1"/>
-    <col min="5125" max="5125" width="12.42578125" style="38" customWidth="1"/>
-    <col min="5126" max="5126" width="11.42578125" style="38"/>
-    <col min="5127" max="5127" width="23.85546875" style="38" customWidth="1"/>
-    <col min="5128" max="5376" width="11.42578125" style="38"/>
-    <col min="5377" max="5377" width="43" style="38" customWidth="1"/>
-    <col min="5378" max="5379" width="11.42578125" style="38"/>
-    <col min="5380" max="5380" width="13.28515625" style="38" customWidth="1"/>
-    <col min="5381" max="5381" width="12.42578125" style="38" customWidth="1"/>
-    <col min="5382" max="5382" width="11.42578125" style="38"/>
-    <col min="5383" max="5383" width="23.85546875" style="38" customWidth="1"/>
-    <col min="5384" max="5632" width="11.42578125" style="38"/>
-    <col min="5633" max="5633" width="43" style="38" customWidth="1"/>
-    <col min="5634" max="5635" width="11.42578125" style="38"/>
-    <col min="5636" max="5636" width="13.28515625" style="38" customWidth="1"/>
-    <col min="5637" max="5637" width="12.42578125" style="38" customWidth="1"/>
-    <col min="5638" max="5638" width="11.42578125" style="38"/>
-    <col min="5639" max="5639" width="23.85546875" style="38" customWidth="1"/>
-    <col min="5640" max="5888" width="11.42578125" style="38"/>
-    <col min="5889" max="5889" width="43" style="38" customWidth="1"/>
-    <col min="5890" max="5891" width="11.42578125" style="38"/>
-    <col min="5892" max="5892" width="13.28515625" style="38" customWidth="1"/>
-    <col min="5893" max="5893" width="12.42578125" style="38" customWidth="1"/>
-    <col min="5894" max="5894" width="11.42578125" style="38"/>
-    <col min="5895" max="5895" width="23.85546875" style="38" customWidth="1"/>
-    <col min="5896" max="6144" width="11.42578125" style="38"/>
-    <col min="6145" max="6145" width="43" style="38" customWidth="1"/>
-    <col min="6146" max="6147" width="11.42578125" style="38"/>
-    <col min="6148" max="6148" width="13.28515625" style="38" customWidth="1"/>
-    <col min="6149" max="6149" width="12.42578125" style="38" customWidth="1"/>
-    <col min="6150" max="6150" width="11.42578125" style="38"/>
-    <col min="6151" max="6151" width="23.85546875" style="38" customWidth="1"/>
-    <col min="6152" max="6400" width="11.42578125" style="38"/>
-    <col min="6401" max="6401" width="43" style="38" customWidth="1"/>
-    <col min="6402" max="6403" width="11.42578125" style="38"/>
-    <col min="6404" max="6404" width="13.28515625" style="38" customWidth="1"/>
-    <col min="6405" max="6405" width="12.42578125" style="38" customWidth="1"/>
-    <col min="6406" max="6406" width="11.42578125" style="38"/>
-    <col min="6407" max="6407" width="23.85546875" style="38" customWidth="1"/>
-    <col min="6408" max="6656" width="11.42578125" style="38"/>
-    <col min="6657" max="6657" width="43" style="38" customWidth="1"/>
-    <col min="6658" max="6659" width="11.42578125" style="38"/>
-    <col min="6660" max="6660" width="13.28515625" style="38" customWidth="1"/>
-    <col min="6661" max="6661" width="12.42578125" style="38" customWidth="1"/>
-    <col min="6662" max="6662" width="11.42578125" style="38"/>
-    <col min="6663" max="6663" width="23.85546875" style="38" customWidth="1"/>
-    <col min="6664" max="6912" width="11.42578125" style="38"/>
-    <col min="6913" max="6913" width="43" style="38" customWidth="1"/>
-    <col min="6914" max="6915" width="11.42578125" style="38"/>
-    <col min="6916" max="6916" width="13.28515625" style="38" customWidth="1"/>
-    <col min="6917" max="6917" width="12.42578125" style="38" customWidth="1"/>
-    <col min="6918" max="6918" width="11.42578125" style="38"/>
-    <col min="6919" max="6919" width="23.85546875" style="38" customWidth="1"/>
-    <col min="6920" max="7168" width="11.42578125" style="38"/>
-    <col min="7169" max="7169" width="43" style="38" customWidth="1"/>
-    <col min="7170" max="7171" width="11.42578125" style="38"/>
-    <col min="7172" max="7172" width="13.28515625" style="38" customWidth="1"/>
-    <col min="7173" max="7173" width="12.42578125" style="38" customWidth="1"/>
-    <col min="7174" max="7174" width="11.42578125" style="38"/>
-    <col min="7175" max="7175" width="23.85546875" style="38" customWidth="1"/>
-    <col min="7176" max="7424" width="11.42578125" style="38"/>
-    <col min="7425" max="7425" width="43" style="38" customWidth="1"/>
-    <col min="7426" max="7427" width="11.42578125" style="38"/>
-    <col min="7428" max="7428" width="13.28515625" style="38" customWidth="1"/>
-    <col min="7429" max="7429" width="12.42578125" style="38" customWidth="1"/>
-    <col min="7430" max="7430" width="11.42578125" style="38"/>
-    <col min="7431" max="7431" width="23.85546875" style="38" customWidth="1"/>
-    <col min="7432" max="7680" width="11.42578125" style="38"/>
-    <col min="7681" max="7681" width="43" style="38" customWidth="1"/>
-    <col min="7682" max="7683" width="11.42578125" style="38"/>
-    <col min="7684" max="7684" width="13.28515625" style="38" customWidth="1"/>
-    <col min="7685" max="7685" width="12.42578125" style="38" customWidth="1"/>
-    <col min="7686" max="7686" width="11.42578125" style="38"/>
-    <col min="7687" max="7687" width="23.85546875" style="38" customWidth="1"/>
-    <col min="7688" max="7936" width="11.42578125" style="38"/>
-    <col min="7937" max="7937" width="43" style="38" customWidth="1"/>
-    <col min="7938" max="7939" width="11.42578125" style="38"/>
-    <col min="7940" max="7940" width="13.28515625" style="38" customWidth="1"/>
-    <col min="7941" max="7941" width="12.42578125" style="38" customWidth="1"/>
-    <col min="7942" max="7942" width="11.42578125" style="38"/>
-    <col min="7943" max="7943" width="23.85546875" style="38" customWidth="1"/>
-    <col min="7944" max="8192" width="11.42578125" style="38"/>
-    <col min="8193" max="8193" width="43" style="38" customWidth="1"/>
-    <col min="8194" max="8195" width="11.42578125" style="38"/>
-    <col min="8196" max="8196" width="13.28515625" style="38" customWidth="1"/>
-    <col min="8197" max="8197" width="12.42578125" style="38" customWidth="1"/>
-    <col min="8198" max="8198" width="11.42578125" style="38"/>
-    <col min="8199" max="8199" width="23.85546875" style="38" customWidth="1"/>
-    <col min="8200" max="8448" width="11.42578125" style="38"/>
-    <col min="8449" max="8449" width="43" style="38" customWidth="1"/>
-    <col min="8450" max="8451" width="11.42578125" style="38"/>
-    <col min="8452" max="8452" width="13.28515625" style="38" customWidth="1"/>
-    <col min="8453" max="8453" width="12.42578125" style="38" customWidth="1"/>
-    <col min="8454" max="8454" width="11.42578125" style="38"/>
-    <col min="8455" max="8455" width="23.85546875" style="38" customWidth="1"/>
-    <col min="8456" max="8704" width="11.42578125" style="38"/>
-    <col min="8705" max="8705" width="43" style="38" customWidth="1"/>
-    <col min="8706" max="8707" width="11.42578125" style="38"/>
-    <col min="8708" max="8708" width="13.28515625" style="38" customWidth="1"/>
-    <col min="8709" max="8709" width="12.42578125" style="38" customWidth="1"/>
-    <col min="8710" max="8710" width="11.42578125" style="38"/>
-    <col min="8711" max="8711" width="23.85546875" style="38" customWidth="1"/>
-    <col min="8712" max="8960" width="11.42578125" style="38"/>
-    <col min="8961" max="8961" width="43" style="38" customWidth="1"/>
-    <col min="8962" max="8963" width="11.42578125" style="38"/>
-    <col min="8964" max="8964" width="13.28515625" style="38" customWidth="1"/>
-    <col min="8965" max="8965" width="12.42578125" style="38" customWidth="1"/>
-    <col min="8966" max="8966" width="11.42578125" style="38"/>
-    <col min="8967" max="8967" width="23.85546875" style="38" customWidth="1"/>
-    <col min="8968" max="9216" width="11.42578125" style="38"/>
-    <col min="9217" max="9217" width="43" style="38" customWidth="1"/>
-    <col min="9218" max="9219" width="11.42578125" style="38"/>
-    <col min="9220" max="9220" width="13.28515625" style="38" customWidth="1"/>
-    <col min="9221" max="9221" width="12.42578125" style="38" customWidth="1"/>
-    <col min="9222" max="9222" width="11.42578125" style="38"/>
-    <col min="9223" max="9223" width="23.85546875" style="38" customWidth="1"/>
-    <col min="9224" max="9472" width="11.42578125" style="38"/>
-    <col min="9473" max="9473" width="43" style="38" customWidth="1"/>
-    <col min="9474" max="9475" width="11.42578125" style="38"/>
-    <col min="9476" max="9476" width="13.28515625" style="38" customWidth="1"/>
-    <col min="9477" max="9477" width="12.42578125" style="38" customWidth="1"/>
-    <col min="9478" max="9478" width="11.42578125" style="38"/>
-    <col min="9479" max="9479" width="23.85546875" style="38" customWidth="1"/>
-    <col min="9480" max="9728" width="11.42578125" style="38"/>
-    <col min="9729" max="9729" width="43" style="38" customWidth="1"/>
-    <col min="9730" max="9731" width="11.42578125" style="38"/>
-    <col min="9732" max="9732" width="13.28515625" style="38" customWidth="1"/>
-    <col min="9733" max="9733" width="12.42578125" style="38" customWidth="1"/>
-    <col min="9734" max="9734" width="11.42578125" style="38"/>
-    <col min="9735" max="9735" width="23.85546875" style="38" customWidth="1"/>
-    <col min="9736" max="9984" width="11.42578125" style="38"/>
-    <col min="9985" max="9985" width="43" style="38" customWidth="1"/>
-    <col min="9986" max="9987" width="11.42578125" style="38"/>
-    <col min="9988" max="9988" width="13.28515625" style="38" customWidth="1"/>
-    <col min="9989" max="9989" width="12.42578125" style="38" customWidth="1"/>
-    <col min="9990" max="9990" width="11.42578125" style="38"/>
-    <col min="9991" max="9991" width="23.85546875" style="38" customWidth="1"/>
-    <col min="9992" max="10240" width="11.42578125" style="38"/>
-    <col min="10241" max="10241" width="43" style="38" customWidth="1"/>
-    <col min="10242" max="10243" width="11.42578125" style="38"/>
-    <col min="10244" max="10244" width="13.28515625" style="38" customWidth="1"/>
-    <col min="10245" max="10245" width="12.42578125" style="38" customWidth="1"/>
-    <col min="10246" max="10246" width="11.42578125" style="38"/>
-    <col min="10247" max="10247" width="23.85546875" style="38" customWidth="1"/>
-    <col min="10248" max="10496" width="11.42578125" style="38"/>
-    <col min="10497" max="10497" width="43" style="38" customWidth="1"/>
-    <col min="10498" max="10499" width="11.42578125" style="38"/>
-    <col min="10500" max="10500" width="13.28515625" style="38" customWidth="1"/>
-    <col min="10501" max="10501" width="12.42578125" style="38" customWidth="1"/>
-    <col min="10502" max="10502" width="11.42578125" style="38"/>
-    <col min="10503" max="10503" width="23.85546875" style="38" customWidth="1"/>
-    <col min="10504" max="10752" width="11.42578125" style="38"/>
-    <col min="10753" max="10753" width="43" style="38" customWidth="1"/>
-    <col min="10754" max="10755" width="11.42578125" style="38"/>
-    <col min="10756" max="10756" width="13.28515625" style="38" customWidth="1"/>
-    <col min="10757" max="10757" width="12.42578125" style="38" customWidth="1"/>
-    <col min="10758" max="10758" width="11.42578125" style="38"/>
-    <col min="10759" max="10759" width="23.85546875" style="38" customWidth="1"/>
-    <col min="10760" max="11008" width="11.42578125" style="38"/>
-    <col min="11009" max="11009" width="43" style="38" customWidth="1"/>
-    <col min="11010" max="11011" width="11.42578125" style="38"/>
-    <col min="11012" max="11012" width="13.28515625" style="38" customWidth="1"/>
-    <col min="11013" max="11013" width="12.42578125" style="38" customWidth="1"/>
-    <col min="11014" max="11014" width="11.42578125" style="38"/>
-    <col min="11015" max="11015" width="23.85546875" style="38" customWidth="1"/>
-    <col min="11016" max="11264" width="11.42578125" style="38"/>
-    <col min="11265" max="11265" width="43" style="38" customWidth="1"/>
-    <col min="11266" max="11267" width="11.42578125" style="38"/>
-    <col min="11268" max="11268" width="13.28515625" style="38" customWidth="1"/>
-    <col min="11269" max="11269" width="12.42578125" style="38" customWidth="1"/>
-    <col min="11270" max="11270" width="11.42578125" style="38"/>
-    <col min="11271" max="11271" width="23.85546875" style="38" customWidth="1"/>
-    <col min="11272" max="11520" width="11.42578125" style="38"/>
-    <col min="11521" max="11521" width="43" style="38" customWidth="1"/>
-    <col min="11522" max="11523" width="11.42578125" style="38"/>
-    <col min="11524" max="11524" width="13.28515625" style="38" customWidth="1"/>
-    <col min="11525" max="11525" width="12.42578125" style="38" customWidth="1"/>
-    <col min="11526" max="11526" width="11.42578125" style="38"/>
-    <col min="11527" max="11527" width="23.85546875" style="38" customWidth="1"/>
-    <col min="11528" max="11776" width="11.42578125" style="38"/>
-    <col min="11777" max="11777" width="43" style="38" customWidth="1"/>
-    <col min="11778" max="11779" width="11.42578125" style="38"/>
-    <col min="11780" max="11780" width="13.28515625" style="38" customWidth="1"/>
-    <col min="11781" max="11781" width="12.42578125" style="38" customWidth="1"/>
-    <col min="11782" max="11782" width="11.42578125" style="38"/>
-    <col min="11783" max="11783" width="23.85546875" style="38" customWidth="1"/>
-    <col min="11784" max="12032" width="11.42578125" style="38"/>
-    <col min="12033" max="12033" width="43" style="38" customWidth="1"/>
-    <col min="12034" max="12035" width="11.42578125" style="38"/>
-    <col min="12036" max="12036" width="13.28515625" style="38" customWidth="1"/>
-    <col min="12037" max="12037" width="12.42578125" style="38" customWidth="1"/>
-    <col min="12038" max="12038" width="11.42578125" style="38"/>
-    <col min="12039" max="12039" width="23.85546875" style="38" customWidth="1"/>
-    <col min="12040" max="12288" width="11.42578125" style="38"/>
-    <col min="12289" max="12289" width="43" style="38" customWidth="1"/>
-    <col min="12290" max="12291" width="11.42578125" style="38"/>
-    <col min="12292" max="12292" width="13.28515625" style="38" customWidth="1"/>
-    <col min="12293" max="12293" width="12.42578125" style="38" customWidth="1"/>
-    <col min="12294" max="12294" width="11.42578125" style="38"/>
-    <col min="12295" max="12295" width="23.85546875" style="38" customWidth="1"/>
-    <col min="12296" max="12544" width="11.42578125" style="38"/>
-    <col min="12545" max="12545" width="43" style="38" customWidth="1"/>
-    <col min="12546" max="12547" width="11.42578125" style="38"/>
-    <col min="12548" max="12548" width="13.28515625" style="38" customWidth="1"/>
-    <col min="12549" max="12549" width="12.42578125" style="38" customWidth="1"/>
-    <col min="12550" max="12550" width="11.42578125" style="38"/>
-    <col min="12551" max="12551" width="23.85546875" style="38" customWidth="1"/>
-    <col min="12552" max="12800" width="11.42578125" style="38"/>
-    <col min="12801" max="12801" width="43" style="38" customWidth="1"/>
-    <col min="12802" max="12803" width="11.42578125" style="38"/>
-    <col min="12804" max="12804" width="13.28515625" style="38" customWidth="1"/>
-    <col min="12805" max="12805" width="12.42578125" style="38" customWidth="1"/>
-    <col min="12806" max="12806" width="11.42578125" style="38"/>
-    <col min="12807" max="12807" width="23.85546875" style="38" customWidth="1"/>
-    <col min="12808" max="13056" width="11.42578125" style="38"/>
-    <col min="13057" max="13057" width="43" style="38" customWidth="1"/>
-    <col min="13058" max="13059" width="11.42578125" style="38"/>
-    <col min="13060" max="13060" width="13.28515625" style="38" customWidth="1"/>
-    <col min="13061" max="13061" width="12.42578125" style="38" customWidth="1"/>
-    <col min="13062" max="13062" width="11.42578125" style="38"/>
-    <col min="13063" max="13063" width="23.85546875" style="38" customWidth="1"/>
-    <col min="13064" max="13312" width="11.42578125" style="38"/>
-    <col min="13313" max="13313" width="43" style="38" customWidth="1"/>
-    <col min="13314" max="13315" width="11.42578125" style="38"/>
-    <col min="13316" max="13316" width="13.28515625" style="38" customWidth="1"/>
-    <col min="13317" max="13317" width="12.42578125" style="38" customWidth="1"/>
-    <col min="13318" max="13318" width="11.42578125" style="38"/>
-    <col min="13319" max="13319" width="23.85546875" style="38" customWidth="1"/>
-    <col min="13320" max="13568" width="11.42578125" style="38"/>
-    <col min="13569" max="13569" width="43" style="38" customWidth="1"/>
-    <col min="13570" max="13571" width="11.42578125" style="38"/>
-    <col min="13572" max="13572" width="13.28515625" style="38" customWidth="1"/>
-    <col min="13573" max="13573" width="12.42578125" style="38" customWidth="1"/>
-    <col min="13574" max="13574" width="11.42578125" style="38"/>
-    <col min="13575" max="13575" width="23.85546875" style="38" customWidth="1"/>
-    <col min="13576" max="13824" width="11.42578125" style="38"/>
-    <col min="13825" max="13825" width="43" style="38" customWidth="1"/>
-    <col min="13826" max="13827" width="11.42578125" style="38"/>
-    <col min="13828" max="13828" width="13.28515625" style="38" customWidth="1"/>
-    <col min="13829" max="13829" width="12.42578125" style="38" customWidth="1"/>
-    <col min="13830" max="13830" width="11.42578125" style="38"/>
-    <col min="13831" max="13831" width="23.85546875" style="38" customWidth="1"/>
-    <col min="13832" max="14080" width="11.42578125" style="38"/>
-    <col min="14081" max="14081" width="43" style="38" customWidth="1"/>
-    <col min="14082" max="14083" width="11.42578125" style="38"/>
-    <col min="14084" max="14084" width="13.28515625" style="38" customWidth="1"/>
-    <col min="14085" max="14085" width="12.42578125" style="38" customWidth="1"/>
-    <col min="14086" max="14086" width="11.42578125" style="38"/>
-    <col min="14087" max="14087" width="23.85546875" style="38" customWidth="1"/>
-    <col min="14088" max="14336" width="11.42578125" style="38"/>
-    <col min="14337" max="14337" width="43" style="38" customWidth="1"/>
-    <col min="14338" max="14339" width="11.42578125" style="38"/>
-    <col min="14340" max="14340" width="13.28515625" style="38" customWidth="1"/>
-    <col min="14341" max="14341" width="12.42578125" style="38" customWidth="1"/>
-    <col min="14342" max="14342" width="11.42578125" style="38"/>
-    <col min="14343" max="14343" width="23.85546875" style="38" customWidth="1"/>
-    <col min="14344" max="14592" width="11.42578125" style="38"/>
-    <col min="14593" max="14593" width="43" style="38" customWidth="1"/>
-    <col min="14594" max="14595" width="11.42578125" style="38"/>
-    <col min="14596" max="14596" width="13.28515625" style="38" customWidth="1"/>
-    <col min="14597" max="14597" width="12.42578125" style="38" customWidth="1"/>
-    <col min="14598" max="14598" width="11.42578125" style="38"/>
-    <col min="14599" max="14599" width="23.85546875" style="38" customWidth="1"/>
-    <col min="14600" max="14848" width="11.42578125" style="38"/>
-    <col min="14849" max="14849" width="43" style="38" customWidth="1"/>
-    <col min="14850" max="14851" width="11.42578125" style="38"/>
-    <col min="14852" max="14852" width="13.28515625" style="38" customWidth="1"/>
-    <col min="14853" max="14853" width="12.42578125" style="38" customWidth="1"/>
-    <col min="14854" max="14854" width="11.42578125" style="38"/>
-    <col min="14855" max="14855" width="23.85546875" style="38" customWidth="1"/>
-    <col min="14856" max="15104" width="11.42578125" style="38"/>
-    <col min="15105" max="15105" width="43" style="38" customWidth="1"/>
-    <col min="15106" max="15107" width="11.42578125" style="38"/>
-    <col min="15108" max="15108" width="13.28515625" style="38" customWidth="1"/>
-    <col min="15109" max="15109" width="12.42578125" style="38" customWidth="1"/>
-    <col min="15110" max="15110" width="11.42578125" style="38"/>
-    <col min="15111" max="15111" width="23.85546875" style="38" customWidth="1"/>
-    <col min="15112" max="15360" width="11.42578125" style="38"/>
-    <col min="15361" max="15361" width="43" style="38" customWidth="1"/>
-    <col min="15362" max="15363" width="11.42578125" style="38"/>
-    <col min="15364" max="15364" width="13.28515625" style="38" customWidth="1"/>
-    <col min="15365" max="15365" width="12.42578125" style="38" customWidth="1"/>
-    <col min="15366" max="15366" width="11.42578125" style="38"/>
-    <col min="15367" max="15367" width="23.85546875" style="38" customWidth="1"/>
-    <col min="15368" max="15616" width="11.42578125" style="38"/>
-    <col min="15617" max="15617" width="43" style="38" customWidth="1"/>
-    <col min="15618" max="15619" width="11.42578125" style="38"/>
-    <col min="15620" max="15620" width="13.28515625" style="38" customWidth="1"/>
-    <col min="15621" max="15621" width="12.42578125" style="38" customWidth="1"/>
-    <col min="15622" max="15622" width="11.42578125" style="38"/>
-    <col min="15623" max="15623" width="23.85546875" style="38" customWidth="1"/>
-    <col min="15624" max="15872" width="11.42578125" style="38"/>
-    <col min="15873" max="15873" width="43" style="38" customWidth="1"/>
-    <col min="15874" max="15875" width="11.42578125" style="38"/>
-    <col min="15876" max="15876" width="13.28515625" style="38" customWidth="1"/>
-    <col min="15877" max="15877" width="12.42578125" style="38" customWidth="1"/>
-    <col min="15878" max="15878" width="11.42578125" style="38"/>
-    <col min="15879" max="15879" width="23.85546875" style="38" customWidth="1"/>
-    <col min="15880" max="16128" width="11.42578125" style="38"/>
-    <col min="16129" max="16129" width="43" style="38" customWidth="1"/>
-    <col min="16130" max="16131" width="11.42578125" style="38"/>
-    <col min="16132" max="16132" width="13.28515625" style="38" customWidth="1"/>
-    <col min="16133" max="16133" width="12.42578125" style="38" customWidth="1"/>
-    <col min="16134" max="16134" width="11.42578125" style="38"/>
-    <col min="16135" max="16135" width="23.85546875" style="38" customWidth="1"/>
-    <col min="16136" max="16384" width="11.42578125" style="38"/>
+    <col min="1" max="1" width="43" style="29" customWidth="1"/>
+    <col min="2" max="3" width="11.42578125" style="29"/>
+    <col min="4" max="4" width="13.28515625" style="29" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" style="29" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" style="29"/>
+    <col min="7" max="7" width="23.85546875" style="29" customWidth="1"/>
+    <col min="8" max="256" width="11.42578125" style="29"/>
+    <col min="257" max="257" width="43" style="29" customWidth="1"/>
+    <col min="258" max="259" width="11.42578125" style="29"/>
+    <col min="260" max="260" width="13.28515625" style="29" customWidth="1"/>
+    <col min="261" max="261" width="12.42578125" style="29" customWidth="1"/>
+    <col min="262" max="262" width="11.42578125" style="29"/>
+    <col min="263" max="263" width="23.85546875" style="29" customWidth="1"/>
+    <col min="264" max="512" width="11.42578125" style="29"/>
+    <col min="513" max="513" width="43" style="29" customWidth="1"/>
+    <col min="514" max="515" width="11.42578125" style="29"/>
+    <col min="516" max="516" width="13.28515625" style="29" customWidth="1"/>
+    <col min="517" max="517" width="12.42578125" style="29" customWidth="1"/>
+    <col min="518" max="518" width="11.42578125" style="29"/>
+    <col min="519" max="519" width="23.85546875" style="29" customWidth="1"/>
+    <col min="520" max="768" width="11.42578125" style="29"/>
+    <col min="769" max="769" width="43" style="29" customWidth="1"/>
+    <col min="770" max="771" width="11.42578125" style="29"/>
+    <col min="772" max="772" width="13.28515625" style="29" customWidth="1"/>
+    <col min="773" max="773" width="12.42578125" style="29" customWidth="1"/>
+    <col min="774" max="774" width="11.42578125" style="29"/>
+    <col min="775" max="775" width="23.85546875" style="29" customWidth="1"/>
+    <col min="776" max="1024" width="11.42578125" style="29"/>
+    <col min="1025" max="1025" width="43" style="29" customWidth="1"/>
+    <col min="1026" max="1027" width="11.42578125" style="29"/>
+    <col min="1028" max="1028" width="13.28515625" style="29" customWidth="1"/>
+    <col min="1029" max="1029" width="12.42578125" style="29" customWidth="1"/>
+    <col min="1030" max="1030" width="11.42578125" style="29"/>
+    <col min="1031" max="1031" width="23.85546875" style="29" customWidth="1"/>
+    <col min="1032" max="1280" width="11.42578125" style="29"/>
+    <col min="1281" max="1281" width="43" style="29" customWidth="1"/>
+    <col min="1282" max="1283" width="11.42578125" style="29"/>
+    <col min="1284" max="1284" width="13.28515625" style="29" customWidth="1"/>
+    <col min="1285" max="1285" width="12.42578125" style="29" customWidth="1"/>
+    <col min="1286" max="1286" width="11.42578125" style="29"/>
+    <col min="1287" max="1287" width="23.85546875" style="29" customWidth="1"/>
+    <col min="1288" max="1536" width="11.42578125" style="29"/>
+    <col min="1537" max="1537" width="43" style="29" customWidth="1"/>
+    <col min="1538" max="1539" width="11.42578125" style="29"/>
+    <col min="1540" max="1540" width="13.28515625" style="29" customWidth="1"/>
+    <col min="1541" max="1541" width="12.42578125" style="29" customWidth="1"/>
+    <col min="1542" max="1542" width="11.42578125" style="29"/>
+    <col min="1543" max="1543" width="23.85546875" style="29" customWidth="1"/>
+    <col min="1544" max="1792" width="11.42578125" style="29"/>
+    <col min="1793" max="1793" width="43" style="29" customWidth="1"/>
+    <col min="1794" max="1795" width="11.42578125" style="29"/>
+    <col min="1796" max="1796" width="13.28515625" style="29" customWidth="1"/>
+    <col min="1797" max="1797" width="12.42578125" style="29" customWidth="1"/>
+    <col min="1798" max="1798" width="11.42578125" style="29"/>
+    <col min="1799" max="1799" width="23.85546875" style="29" customWidth="1"/>
+    <col min="1800" max="2048" width="11.42578125" style="29"/>
+    <col min="2049" max="2049" width="43" style="29" customWidth="1"/>
+    <col min="2050" max="2051" width="11.42578125" style="29"/>
+    <col min="2052" max="2052" width="13.28515625" style="29" customWidth="1"/>
+    <col min="2053" max="2053" width="12.42578125" style="29" customWidth="1"/>
+    <col min="2054" max="2054" width="11.42578125" style="29"/>
+    <col min="2055" max="2055" width="23.85546875" style="29" customWidth="1"/>
+    <col min="2056" max="2304" width="11.42578125" style="29"/>
+    <col min="2305" max="2305" width="43" style="29" customWidth="1"/>
+    <col min="2306" max="2307" width="11.42578125" style="29"/>
+    <col min="2308" max="2308" width="13.28515625" style="29" customWidth="1"/>
+    <col min="2309" max="2309" width="12.42578125" style="29" customWidth="1"/>
+    <col min="2310" max="2310" width="11.42578125" style="29"/>
+    <col min="2311" max="2311" width="23.85546875" style="29" customWidth="1"/>
+    <col min="2312" max="2560" width="11.42578125" style="29"/>
+    <col min="2561" max="2561" width="43" style="29" customWidth="1"/>
+    <col min="2562" max="2563" width="11.42578125" style="29"/>
+    <col min="2564" max="2564" width="13.28515625" style="29" customWidth="1"/>
+    <col min="2565" max="2565" width="12.42578125" style="29" customWidth="1"/>
+    <col min="2566" max="2566" width="11.42578125" style="29"/>
+    <col min="2567" max="2567" width="23.85546875" style="29" customWidth="1"/>
+    <col min="2568" max="2816" width="11.42578125" style="29"/>
+    <col min="2817" max="2817" width="43" style="29" customWidth="1"/>
+    <col min="2818" max="2819" width="11.42578125" style="29"/>
+    <col min="2820" max="2820" width="13.28515625" style="29" customWidth="1"/>
+    <col min="2821" max="2821" width="12.42578125" style="29" customWidth="1"/>
+    <col min="2822" max="2822" width="11.42578125" style="29"/>
+    <col min="2823" max="2823" width="23.85546875" style="29" customWidth="1"/>
+    <col min="2824" max="3072" width="11.42578125" style="29"/>
+    <col min="3073" max="3073" width="43" style="29" customWidth="1"/>
+    <col min="3074" max="3075" width="11.42578125" style="29"/>
+    <col min="3076" max="3076" width="13.28515625" style="29" customWidth="1"/>
+    <col min="3077" max="3077" width="12.42578125" style="29" customWidth="1"/>
+    <col min="3078" max="3078" width="11.42578125" style="29"/>
+    <col min="3079" max="3079" width="23.85546875" style="29" customWidth="1"/>
+    <col min="3080" max="3328" width="11.42578125" style="29"/>
+    <col min="3329" max="3329" width="43" style="29" customWidth="1"/>
+    <col min="3330" max="3331" width="11.42578125" style="29"/>
+    <col min="3332" max="3332" width="13.28515625" style="29" customWidth="1"/>
+    <col min="3333" max="3333" width="12.42578125" style="29" customWidth="1"/>
+    <col min="3334" max="3334" width="11.42578125" style="29"/>
+    <col min="3335" max="3335" width="23.85546875" style="29" customWidth="1"/>
+    <col min="3336" max="3584" width="11.42578125" style="29"/>
+    <col min="3585" max="3585" width="43" style="29" customWidth="1"/>
+    <col min="3586" max="3587" width="11.42578125" style="29"/>
+    <col min="3588" max="3588" width="13.28515625" style="29" customWidth="1"/>
+    <col min="3589" max="3589" width="12.42578125" style="29" customWidth="1"/>
+    <col min="3590" max="3590" width="11.42578125" style="29"/>
+    <col min="3591" max="3591" width="23.85546875" style="29" customWidth="1"/>
+    <col min="3592" max="3840" width="11.42578125" style="29"/>
+    <col min="3841" max="3841" width="43" style="29" customWidth="1"/>
+    <col min="3842" max="3843" width="11.42578125" style="29"/>
+    <col min="3844" max="3844" width="13.28515625" style="29" customWidth="1"/>
+    <col min="3845" max="3845" width="12.42578125" style="29" customWidth="1"/>
+    <col min="3846" max="3846" width="11.42578125" style="29"/>
+    <col min="3847" max="3847" width="23.85546875" style="29" customWidth="1"/>
+    <col min="3848" max="4096" width="11.42578125" style="29"/>
+    <col min="4097" max="4097" width="43" style="29" customWidth="1"/>
+    <col min="4098" max="4099" width="11.42578125" style="29"/>
+    <col min="4100" max="4100" width="13.28515625" style="29" customWidth="1"/>
+    <col min="4101" max="4101" width="12.42578125" style="29" customWidth="1"/>
+    <col min="4102" max="4102" width="11.42578125" style="29"/>
+    <col min="4103" max="4103" width="23.85546875" style="29" customWidth="1"/>
+    <col min="4104" max="4352" width="11.42578125" style="29"/>
+    <col min="4353" max="4353" width="43" style="29" customWidth="1"/>
+    <col min="4354" max="4355" width="11.42578125" style="29"/>
+    <col min="4356" max="4356" width="13.28515625" style="29" customWidth="1"/>
+    <col min="4357" max="4357" width="12.42578125" style="29" customWidth="1"/>
+    <col min="4358" max="4358" width="11.42578125" style="29"/>
+    <col min="4359" max="4359" width="23.85546875" style="29" customWidth="1"/>
+    <col min="4360" max="4608" width="11.42578125" style="29"/>
+    <col min="4609" max="4609" width="43" style="29" customWidth="1"/>
+    <col min="4610" max="4611" width="11.42578125" style="29"/>
+    <col min="4612" max="4612" width="13.28515625" style="29" customWidth="1"/>
+    <col min="4613" max="4613" width="12.42578125" style="29" customWidth="1"/>
+    <col min="4614" max="4614" width="11.42578125" style="29"/>
+    <col min="4615" max="4615" width="23.85546875" style="29" customWidth="1"/>
+    <col min="4616" max="4864" width="11.42578125" style="29"/>
+    <col min="4865" max="4865" width="43" style="29" customWidth="1"/>
+    <col min="4866" max="4867" width="11.42578125" style="29"/>
+    <col min="4868" max="4868" width="13.28515625" style="29" customWidth="1"/>
+    <col min="4869" max="4869" width="12.42578125" style="29" customWidth="1"/>
+    <col min="4870" max="4870" width="11.42578125" style="29"/>
+    <col min="4871" max="4871" width="23.85546875" style="29" customWidth="1"/>
+    <col min="4872" max="5120" width="11.42578125" style="29"/>
+    <col min="5121" max="5121" width="43" style="29" customWidth="1"/>
+    <col min="5122" max="5123" width="11.42578125" style="29"/>
+    <col min="5124" max="5124" width="13.28515625" style="29" customWidth="1"/>
+    <col min="5125" max="5125" width="12.42578125" style="29" customWidth="1"/>
+    <col min="5126" max="5126" width="11.42578125" style="29"/>
+    <col min="5127" max="5127" width="23.85546875" style="29" customWidth="1"/>
+    <col min="5128" max="5376" width="11.42578125" style="29"/>
+    <col min="5377" max="5377" width="43" style="29" customWidth="1"/>
+    <col min="5378" max="5379" width="11.42578125" style="29"/>
+    <col min="5380" max="5380" width="13.28515625" style="29" customWidth="1"/>
+    <col min="5381" max="5381" width="12.42578125" style="29" customWidth="1"/>
+    <col min="5382" max="5382" width="11.42578125" style="29"/>
+    <col min="5383" max="5383" width="23.85546875" style="29" customWidth="1"/>
+    <col min="5384" max="5632" width="11.42578125" style="29"/>
+    <col min="5633" max="5633" width="43" style="29" customWidth="1"/>
+    <col min="5634" max="5635" width="11.42578125" style="29"/>
+    <col min="5636" max="5636" width="13.28515625" style="29" customWidth="1"/>
+    <col min="5637" max="5637" width="12.42578125" style="29" customWidth="1"/>
+    <col min="5638" max="5638" width="11.42578125" style="29"/>
+    <col min="5639" max="5639" width="23.85546875" style="29" customWidth="1"/>
+    <col min="5640" max="5888" width="11.42578125" style="29"/>
+    <col min="5889" max="5889" width="43" style="29" customWidth="1"/>
+    <col min="5890" max="5891" width="11.42578125" style="29"/>
+    <col min="5892" max="5892" width="13.28515625" style="29" customWidth="1"/>
+    <col min="5893" max="5893" width="12.42578125" style="29" customWidth="1"/>
+    <col min="5894" max="5894" width="11.42578125" style="29"/>
+    <col min="5895" max="5895" width="23.85546875" style="29" customWidth="1"/>
+    <col min="5896" max="6144" width="11.42578125" style="29"/>
+    <col min="6145" max="6145" width="43" style="29" customWidth="1"/>
+    <col min="6146" max="6147" width="11.42578125" style="29"/>
+    <col min="6148" max="6148" width="13.28515625" style="29" customWidth="1"/>
+    <col min="6149" max="6149" width="12.42578125" style="29" customWidth="1"/>
+    <col min="6150" max="6150" width="11.42578125" style="29"/>
+    <col min="6151" max="6151" width="23.85546875" style="29" customWidth="1"/>
+    <col min="6152" max="6400" width="11.42578125" style="29"/>
+    <col min="6401" max="6401" width="43" style="29" customWidth="1"/>
+    <col min="6402" max="6403" width="11.42578125" style="29"/>
+    <col min="6404" max="6404" width="13.28515625" style="29" customWidth="1"/>
+    <col min="6405" max="6405" width="12.42578125" style="29" customWidth="1"/>
+    <col min="6406" max="6406" width="11.42578125" style="29"/>
+    <col min="6407" max="6407" width="23.85546875" style="29" customWidth="1"/>
+    <col min="6408" max="6656" width="11.42578125" style="29"/>
+    <col min="6657" max="6657" width="43" style="29" customWidth="1"/>
+    <col min="6658" max="6659" width="11.42578125" style="29"/>
+    <col min="6660" max="6660" width="13.28515625" style="29" customWidth="1"/>
+    <col min="6661" max="6661" width="12.42578125" style="29" customWidth="1"/>
+    <col min="6662" max="6662" width="11.42578125" style="29"/>
+    <col min="6663" max="6663" width="23.85546875" style="29" customWidth="1"/>
+    <col min="6664" max="6912" width="11.42578125" style="29"/>
+    <col min="6913" max="6913" width="43" style="29" customWidth="1"/>
+    <col min="6914" max="6915" width="11.42578125" style="29"/>
+    <col min="6916" max="6916" width="13.28515625" style="29" customWidth="1"/>
+    <col min="6917" max="6917" width="12.42578125" style="29" customWidth="1"/>
+    <col min="6918" max="6918" width="11.42578125" style="29"/>
+    <col min="6919" max="6919" width="23.85546875" style="29" customWidth="1"/>
+    <col min="6920" max="7168" width="11.42578125" style="29"/>
+    <col min="7169" max="7169" width="43" style="29" customWidth="1"/>
+    <col min="7170" max="7171" width="11.42578125" style="29"/>
+    <col min="7172" max="7172" width="13.28515625" style="29" customWidth="1"/>
+    <col min="7173" max="7173" width="12.42578125" style="29" customWidth="1"/>
+    <col min="7174" max="7174" width="11.42578125" style="29"/>
+    <col min="7175" max="7175" width="23.85546875" style="29" customWidth="1"/>
+    <col min="7176" max="7424" width="11.42578125" style="29"/>
+    <col min="7425" max="7425" width="43" style="29" customWidth="1"/>
+    <col min="7426" max="7427" width="11.42578125" style="29"/>
+    <col min="7428" max="7428" width="13.28515625" style="29" customWidth="1"/>
+    <col min="7429" max="7429" width="12.42578125" style="29" customWidth="1"/>
+    <col min="7430" max="7430" width="11.42578125" style="29"/>
+    <col min="7431" max="7431" width="23.85546875" style="29" customWidth="1"/>
+    <col min="7432" max="7680" width="11.42578125" style="29"/>
+    <col min="7681" max="7681" width="43" style="29" customWidth="1"/>
+    <col min="7682" max="7683" width="11.42578125" style="29"/>
+    <col min="7684" max="7684" width="13.28515625" style="29" customWidth="1"/>
+    <col min="7685" max="7685" width="12.42578125" style="29" customWidth="1"/>
+    <col min="7686" max="7686" width="11.42578125" style="29"/>
+    <col min="7687" max="7687" width="23.85546875" style="29" customWidth="1"/>
+    <col min="7688" max="7936" width="11.42578125" style="29"/>
+    <col min="7937" max="7937" width="43" style="29" customWidth="1"/>
+    <col min="7938" max="7939" width="11.42578125" style="29"/>
+    <col min="7940" max="7940" width="13.28515625" style="29" customWidth="1"/>
+    <col min="7941" max="7941" width="12.42578125" style="29" customWidth="1"/>
+    <col min="7942" max="7942" width="11.42578125" style="29"/>
+    <col min="7943" max="7943" width="23.85546875" style="29" customWidth="1"/>
+    <col min="7944" max="8192" width="11.42578125" style="29"/>
+    <col min="8193" max="8193" width="43" style="29" customWidth="1"/>
+    <col min="8194" max="8195" width="11.42578125" style="29"/>
+    <col min="8196" max="8196" width="13.28515625" style="29" customWidth="1"/>
+    <col min="8197" max="8197" width="12.42578125" style="29" customWidth="1"/>
+    <col min="8198" max="8198" width="11.42578125" style="29"/>
+    <col min="8199" max="8199" width="23.85546875" style="29" customWidth="1"/>
+    <col min="8200" max="8448" width="11.42578125" style="29"/>
+    <col min="8449" max="8449" width="43" style="29" customWidth="1"/>
+    <col min="8450" max="8451" width="11.42578125" style="29"/>
+    <col min="8452" max="8452" width="13.28515625" style="29" customWidth="1"/>
+    <col min="8453" max="8453" width="12.42578125" style="29" customWidth="1"/>
+    <col min="8454" max="8454" width="11.42578125" style="29"/>
+    <col min="8455" max="8455" width="23.85546875" style="29" customWidth="1"/>
+    <col min="8456" max="8704" width="11.42578125" style="29"/>
+    <col min="8705" max="8705" width="43" style="29" customWidth="1"/>
+    <col min="8706" max="8707" width="11.42578125" style="29"/>
+    <col min="8708" max="8708" width="13.28515625" style="29" customWidth="1"/>
+    <col min="8709" max="8709" width="12.42578125" style="29" customWidth="1"/>
+    <col min="8710" max="8710" width="11.42578125" style="29"/>
+    <col min="8711" max="8711" width="23.85546875" style="29" customWidth="1"/>
+    <col min="8712" max="8960" width="11.42578125" style="29"/>
+    <col min="8961" max="8961" width="43" style="29" customWidth="1"/>
+    <col min="8962" max="8963" width="11.42578125" style="29"/>
+    <col min="8964" max="8964" width="13.28515625" style="29" customWidth="1"/>
+    <col min="8965" max="8965" width="12.42578125" style="29" customWidth="1"/>
+    <col min="8966" max="8966" width="11.42578125" style="29"/>
+    <col min="8967" max="8967" width="23.85546875" style="29" customWidth="1"/>
+    <col min="8968" max="9216" width="11.42578125" style="29"/>
+    <col min="9217" max="9217" width="43" style="29" customWidth="1"/>
+    <col min="9218" max="9219" width="11.42578125" style="29"/>
+    <col min="9220" max="9220" width="13.28515625" style="29" customWidth="1"/>
+    <col min="9221" max="9221" width="12.42578125" style="29" customWidth="1"/>
+    <col min="9222" max="9222" width="11.42578125" style="29"/>
+    <col min="9223" max="9223" width="23.85546875" style="29" customWidth="1"/>
+    <col min="9224" max="9472" width="11.42578125" style="29"/>
+    <col min="9473" max="9473" width="43" style="29" customWidth="1"/>
+    <col min="9474" max="9475" width="11.42578125" style="29"/>
+    <col min="9476" max="9476" width="13.28515625" style="29" customWidth="1"/>
+    <col min="9477" max="9477" width="12.42578125" style="29" customWidth="1"/>
+    <col min="9478" max="9478" width="11.42578125" style="29"/>
+    <col min="9479" max="9479" width="23.85546875" style="29" customWidth="1"/>
+    <col min="9480" max="9728" width="11.42578125" style="29"/>
+    <col min="9729" max="9729" width="43" style="29" customWidth="1"/>
+    <col min="9730" max="9731" width="11.42578125" style="29"/>
+    <col min="9732" max="9732" width="13.28515625" style="29" customWidth="1"/>
+    <col min="9733" max="9733" width="12.42578125" style="29" customWidth="1"/>
+    <col min="9734" max="9734" width="11.42578125" style="29"/>
+    <col min="9735" max="9735" width="23.85546875" style="29" customWidth="1"/>
+    <col min="9736" max="9984" width="11.42578125" style="29"/>
+    <col min="9985" max="9985" width="43" style="29" customWidth="1"/>
+    <col min="9986" max="9987" width="11.42578125" style="29"/>
+    <col min="9988" max="9988" width="13.28515625" style="29" customWidth="1"/>
+    <col min="9989" max="9989" width="12.42578125" style="29" customWidth="1"/>
+    <col min="9990" max="9990" width="11.42578125" style="29"/>
+    <col min="9991" max="9991" width="23.85546875" style="29" customWidth="1"/>
+    <col min="9992" max="10240" width="11.42578125" style="29"/>
+    <col min="10241" max="10241" width="43" style="29" customWidth="1"/>
+    <col min="10242" max="10243" width="11.42578125" style="29"/>
+    <col min="10244" max="10244" width="13.28515625" style="29" customWidth="1"/>
+    <col min="10245" max="10245" width="12.42578125" style="29" customWidth="1"/>
+    <col min="10246" max="10246" width="11.42578125" style="29"/>
+    <col min="10247" max="10247" width="23.85546875" style="29" customWidth="1"/>
+    <col min="10248" max="10496" width="11.42578125" style="29"/>
+    <col min="10497" max="10497" width="43" style="29" customWidth="1"/>
+    <col min="10498" max="10499" width="11.42578125" style="29"/>
+    <col min="10500" max="10500" width="13.28515625" style="29" customWidth="1"/>
+    <col min="10501" max="10501" width="12.42578125" style="29" customWidth="1"/>
+    <col min="10502" max="10502" width="11.42578125" style="29"/>
+    <col min="10503" max="10503" width="23.85546875" style="29" customWidth="1"/>
+    <col min="10504" max="10752" width="11.42578125" style="29"/>
+    <col min="10753" max="10753" width="43" style="29" customWidth="1"/>
+    <col min="10754" max="10755" width="11.42578125" style="29"/>
+    <col min="10756" max="10756" width="13.28515625" style="29" customWidth="1"/>
+    <col min="10757" max="10757" width="12.42578125" style="29" customWidth="1"/>
+    <col min="10758" max="10758" width="11.42578125" style="29"/>
+    <col min="10759" max="10759" width="23.85546875" style="29" customWidth="1"/>
+    <col min="10760" max="11008" width="11.42578125" style="29"/>
+    <col min="11009" max="11009" width="43" style="29" customWidth="1"/>
+    <col min="11010" max="11011" width="11.42578125" style="29"/>
+    <col min="11012" max="11012" width="13.28515625" style="29" customWidth="1"/>
+    <col min="11013" max="11013" width="12.42578125" style="29" customWidth="1"/>
+    <col min="11014" max="11014" width="11.42578125" style="29"/>
+    <col min="11015" max="11015" width="23.85546875" style="29" customWidth="1"/>
+    <col min="11016" max="11264" width="11.42578125" style="29"/>
+    <col min="11265" max="11265" width="43" style="29" customWidth="1"/>
+    <col min="11266" max="11267" width="11.42578125" style="29"/>
+    <col min="11268" max="11268" width="13.28515625" style="29" customWidth="1"/>
+    <col min="11269" max="11269" width="12.42578125" style="29" customWidth="1"/>
+    <col min="11270" max="11270" width="11.42578125" style="29"/>
+    <col min="11271" max="11271" width="23.85546875" style="29" customWidth="1"/>
+    <col min="11272" max="11520" width="11.42578125" style="29"/>
+    <col min="11521" max="11521" width="43" style="29" customWidth="1"/>
+    <col min="11522" max="11523" width="11.42578125" style="29"/>
+    <col min="11524" max="11524" width="13.28515625" style="29" customWidth="1"/>
+    <col min="11525" max="11525" width="12.42578125" style="29" customWidth="1"/>
+    <col min="11526" max="11526" width="11.42578125" style="29"/>
+    <col min="11527" max="11527" width="23.85546875" style="29" customWidth="1"/>
+    <col min="11528" max="11776" width="11.42578125" style="29"/>
+    <col min="11777" max="11777" width="43" style="29" customWidth="1"/>
+    <col min="11778" max="11779" width="11.42578125" style="29"/>
+    <col min="11780" max="11780" width="13.28515625" style="29" customWidth="1"/>
+    <col min="11781" max="11781" width="12.42578125" style="29" customWidth="1"/>
+    <col min="11782" max="11782" width="11.42578125" style="29"/>
+    <col min="11783" max="11783" width="23.85546875" style="29" customWidth="1"/>
+    <col min="11784" max="12032" width="11.42578125" style="29"/>
+    <col min="12033" max="12033" width="43" style="29" customWidth="1"/>
+    <col min="12034" max="12035" width="11.42578125" style="29"/>
+    <col min="12036" max="12036" width="13.28515625" style="29" customWidth="1"/>
+    <col min="12037" max="12037" width="12.42578125" style="29" customWidth="1"/>
+    <col min="12038" max="12038" width="11.42578125" style="29"/>
+    <col min="12039" max="12039" width="23.85546875" style="29" customWidth="1"/>
+    <col min="12040" max="12288" width="11.42578125" style="29"/>
+    <col min="12289" max="12289" width="43" style="29" customWidth="1"/>
+    <col min="12290" max="12291" width="11.42578125" style="29"/>
+    <col min="12292" max="12292" width="13.28515625" style="29" customWidth="1"/>
+    <col min="12293" max="12293" width="12.42578125" style="29" customWidth="1"/>
+    <col min="12294" max="12294" width="11.42578125" style="29"/>
+    <col min="12295" max="12295" width="23.85546875" style="29" customWidth="1"/>
+    <col min="12296" max="12544" width="11.42578125" style="29"/>
+    <col min="12545" max="12545" width="43" style="29" customWidth="1"/>
+    <col min="12546" max="12547" width="11.42578125" style="29"/>
+    <col min="12548" max="12548" width="13.28515625" style="29" customWidth="1"/>
+    <col min="12549" max="12549" width="12.42578125" style="29" customWidth="1"/>
+    <col min="12550" max="12550" width="11.42578125" style="29"/>
+    <col min="12551" max="12551" width="23.85546875" style="29" customWidth="1"/>
+    <col min="12552" max="12800" width="11.42578125" style="29"/>
+    <col min="12801" max="12801" width="43" style="29" customWidth="1"/>
+    <col min="12802" max="12803" width="11.42578125" style="29"/>
+    <col min="12804" max="12804" width="13.28515625" style="29" customWidth="1"/>
+    <col min="12805" max="12805" width="12.42578125" style="29" customWidth="1"/>
+    <col min="12806" max="12806" width="11.42578125" style="29"/>
+    <col min="12807" max="12807" width="23.85546875" style="29" customWidth="1"/>
+    <col min="12808" max="13056" width="11.42578125" style="29"/>
+    <col min="13057" max="13057" width="43" style="29" customWidth="1"/>
+    <col min="13058" max="13059" width="11.42578125" style="29"/>
+    <col min="13060" max="13060" width="13.28515625" style="29" customWidth="1"/>
+    <col min="13061" max="13061" width="12.42578125" style="29" customWidth="1"/>
+    <col min="13062" max="13062" width="11.42578125" style="29"/>
+    <col min="13063" max="13063" width="23.85546875" style="29" customWidth="1"/>
+    <col min="13064" max="13312" width="11.42578125" style="29"/>
+    <col min="13313" max="13313" width="43" style="29" customWidth="1"/>
+    <col min="13314" max="13315" width="11.42578125" style="29"/>
+    <col min="13316" max="13316" width="13.28515625" style="29" customWidth="1"/>
+    <col min="13317" max="13317" width="12.42578125" style="29" customWidth="1"/>
+    <col min="13318" max="13318" width="11.42578125" style="29"/>
+    <col min="13319" max="13319" width="23.85546875" style="29" customWidth="1"/>
+    <col min="13320" max="13568" width="11.42578125" style="29"/>
+    <col min="13569" max="13569" width="43" style="29" customWidth="1"/>
+    <col min="13570" max="13571" width="11.42578125" style="29"/>
+    <col min="13572" max="13572" width="13.28515625" style="29" customWidth="1"/>
+    <col min="13573" max="13573" width="12.42578125" style="29" customWidth="1"/>
+    <col min="13574" max="13574" width="11.42578125" style="29"/>
+    <col min="13575" max="13575" width="23.85546875" style="29" customWidth="1"/>
+    <col min="13576" max="13824" width="11.42578125" style="29"/>
+    <col min="13825" max="13825" width="43" style="29" customWidth="1"/>
+    <col min="13826" max="13827" width="11.42578125" style="29"/>
+    <col min="13828" max="13828" width="13.28515625" style="29" customWidth="1"/>
+    <col min="13829" max="13829" width="12.42578125" style="29" customWidth="1"/>
+    <col min="13830" max="13830" width="11.42578125" style="29"/>
+    <col min="13831" max="13831" width="23.85546875" style="29" customWidth="1"/>
+    <col min="13832" max="14080" width="11.42578125" style="29"/>
+    <col min="14081" max="14081" width="43" style="29" customWidth="1"/>
+    <col min="14082" max="14083" width="11.42578125" style="29"/>
+    <col min="14084" max="14084" width="13.28515625" style="29" customWidth="1"/>
+    <col min="14085" max="14085" width="12.42578125" style="29" customWidth="1"/>
+    <col min="14086" max="14086" width="11.42578125" style="29"/>
+    <col min="14087" max="14087" width="23.85546875" style="29" customWidth="1"/>
+    <col min="14088" max="14336" width="11.42578125" style="29"/>
+    <col min="14337" max="14337" width="43" style="29" customWidth="1"/>
+    <col min="14338" max="14339" width="11.42578125" style="29"/>
+    <col min="14340" max="14340" width="13.28515625" style="29" customWidth="1"/>
+    <col min="14341" max="14341" width="12.42578125" style="29" customWidth="1"/>
+    <col min="14342" max="14342" width="11.42578125" style="29"/>
+    <col min="14343" max="14343" width="23.85546875" style="29" customWidth="1"/>
+    <col min="14344" max="14592" width="11.42578125" style="29"/>
+    <col min="14593" max="14593" width="43" style="29" customWidth="1"/>
+    <col min="14594" max="14595" width="11.42578125" style="29"/>
+    <col min="14596" max="14596" width="13.28515625" style="29" customWidth="1"/>
+    <col min="14597" max="14597" width="12.42578125" style="29" customWidth="1"/>
+    <col min="14598" max="14598" width="11.42578125" style="29"/>
+    <col min="14599" max="14599" width="23.85546875" style="29" customWidth="1"/>
+    <col min="14600" max="14848" width="11.42578125" style="29"/>
+    <col min="14849" max="14849" width="43" style="29" customWidth="1"/>
+    <col min="14850" max="14851" width="11.42578125" style="29"/>
+    <col min="14852" max="14852" width="13.28515625" style="29" customWidth="1"/>
+    <col min="14853" max="14853" width="12.42578125" style="29" customWidth="1"/>
+    <col min="14854" max="14854" width="11.42578125" style="29"/>
+    <col min="14855" max="14855" width="23.85546875" style="29" customWidth="1"/>
+    <col min="14856" max="15104" width="11.42578125" style="29"/>
+    <col min="15105" max="15105" width="43" style="29" customWidth="1"/>
+    <col min="15106" max="15107" width="11.42578125" style="29"/>
+    <col min="15108" max="15108" width="13.28515625" style="29" customWidth="1"/>
+    <col min="15109" max="15109" width="12.42578125" style="29" customWidth="1"/>
+    <col min="15110" max="15110" width="11.42578125" style="29"/>
+    <col min="15111" max="15111" width="23.85546875" style="29" customWidth="1"/>
+    <col min="15112" max="15360" width="11.42578125" style="29"/>
+    <col min="15361" max="15361" width="43" style="29" customWidth="1"/>
+    <col min="15362" max="15363" width="11.42578125" style="29"/>
+    <col min="15364" max="15364" width="13.28515625" style="29" customWidth="1"/>
+    <col min="15365" max="15365" width="12.42578125" style="29" customWidth="1"/>
+    <col min="15366" max="15366" width="11.42578125" style="29"/>
+    <col min="15367" max="15367" width="23.85546875" style="29" customWidth="1"/>
+    <col min="15368" max="15616" width="11.42578125" style="29"/>
+    <col min="15617" max="15617" width="43" style="29" customWidth="1"/>
+    <col min="15618" max="15619" width="11.42578125" style="29"/>
+    <col min="15620" max="15620" width="13.28515625" style="29" customWidth="1"/>
+    <col min="15621" max="15621" width="12.42578125" style="29" customWidth="1"/>
+    <col min="15622" max="15622" width="11.42578125" style="29"/>
+    <col min="15623" max="15623" width="23.85546875" style="29" customWidth="1"/>
+    <col min="15624" max="15872" width="11.42578125" style="29"/>
+    <col min="15873" max="15873" width="43" style="29" customWidth="1"/>
+    <col min="15874" max="15875" width="11.42578125" style="29"/>
+    <col min="15876" max="15876" width="13.28515625" style="29" customWidth="1"/>
+    <col min="15877" max="15877" width="12.42578125" style="29" customWidth="1"/>
+    <col min="15878" max="15878" width="11.42578125" style="29"/>
+    <col min="15879" max="15879" width="23.85546875" style="29" customWidth="1"/>
+    <col min="15880" max="16128" width="11.42578125" style="29"/>
+    <col min="16129" max="16129" width="43" style="29" customWidth="1"/>
+    <col min="16130" max="16131" width="11.42578125" style="29"/>
+    <col min="16132" max="16132" width="13.28515625" style="29" customWidth="1"/>
+    <col min="16133" max="16133" width="12.42578125" style="29" customWidth="1"/>
+    <col min="16134" max="16134" width="11.42578125" style="29"/>
+    <col min="16135" max="16135" width="23.85546875" style="29" customWidth="1"/>
+    <col min="16136" max="16384" width="11.42578125" style="29"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="34" customFormat="1">
-      <c r="A1" s="33"/>
-      <c r="B1" s="27" t="s">
+    <row r="1" spans="1:7" s="25" customFormat="1">
+      <c r="A1" s="48"/>
+      <c r="B1" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="29"/>
-    </row>
-    <row r="2" spans="1:7" s="34" customFormat="1">
-      <c r="A2" s="33"/>
-      <c r="B2" s="31" t="s">
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="51"/>
+    </row>
+    <row r="2" spans="1:7" s="25" customFormat="1">
+      <c r="A2" s="48"/>
+      <c r="B2" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="C2" s="54" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25" t="s">
+      <c r="D2" s="54"/>
+      <c r="E2" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="25"/>
-      <c r="G2" s="26"/>
-    </row>
-    <row r="3" spans="1:7" s="34" customFormat="1">
-      <c r="A3" s="33"/>
-      <c r="B3" s="31"/>
-      <c r="C3" s="25" t="s">
+      <c r="F2" s="54"/>
+      <c r="G2" s="55"/>
+    </row>
+    <row r="3" spans="1:7" s="25" customFormat="1">
+      <c r="A3" s="48"/>
+      <c r="B3" s="52"/>
+      <c r="C3" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="25" t="s">
+      <c r="D3" s="54" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="25" t="s">
+      <c r="E3" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="25" t="s">
+      <c r="F3" s="54" t="s">
         <v>25</v>
       </c>
-      <c r="G3" s="26"/>
-    </row>
-    <row r="4" spans="1:7" s="34" customFormat="1" ht="16.5" thickBot="1">
-      <c r="A4" s="33"/>
-      <c r="B4" s="32"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
+      <c r="G3" s="55"/>
+    </row>
+    <row r="4" spans="1:7" s="25" customFormat="1" ht="16.5" thickBot="1">
+      <c r="A4" s="48"/>
+      <c r="B4" s="53"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
+      <c r="E4" s="56"/>
       <c r="F4" s="24" t="s">
         <v>1</v>
       </c>
@@ -2025,20 +2128,20 @@
       <c r="A5" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="35"/>
-      <c r="C5" s="36" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="36" t="s">
-        <v>2</v>
-      </c>
-      <c r="E5" s="36" t="s">
-        <v>2</v>
-      </c>
-      <c r="F5" s="36" t="s">
-        <v>2</v>
-      </c>
-      <c r="G5" s="37" t="s">
+      <c r="B5" s="26"/>
+      <c r="C5" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5" s="28" t="s">
         <v>2</v>
       </c>
     </row>
@@ -2046,16 +2149,16 @@
       <c r="A6" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="39"/>
-      <c r="C6" s="40"/>
-      <c r="D6" s="40"/>
-      <c r="E6" s="40" t="s">
-        <v>2</v>
-      </c>
-      <c r="F6" s="40" t="s">
-        <v>2</v>
-      </c>
-      <c r="G6" s="41" t="s">
+      <c r="B6" s="30"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="G6" s="32" t="s">
         <v>2</v>
       </c>
     </row>
@@ -2063,61 +2166,61 @@
       <c r="A7" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="42" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" s="43"/>
-      <c r="D7" s="43" t="s">
-        <v>2</v>
-      </c>
-      <c r="E7" s="43"/>
-      <c r="F7" s="43" t="s">
-        <v>2</v>
-      </c>
-      <c r="G7" s="44" t="s">
+      <c r="B7" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="34"/>
+      <c r="D7" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="34"/>
+      <c r="F7" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="G7" s="35" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="16.5" thickBot="1">
-      <c r="A8" s="48"/>
-      <c r="B8" s="49"/>
-      <c r="C8" s="49"/>
-      <c r="D8" s="49"/>
-      <c r="E8" s="49"/>
-      <c r="F8" s="49"/>
-      <c r="G8" s="49"/>
+      <c r="A8" s="39"/>
+      <c r="B8" s="40"/>
+      <c r="C8" s="40"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="40"/>
     </row>
     <row r="9" spans="1:7" ht="16.5" thickBot="1">
-      <c r="A9" s="50" t="s">
+      <c r="A9" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="49"/>
-      <c r="C9" s="49"/>
-      <c r="D9" s="49"/>
-      <c r="E9" s="49"/>
-      <c r="F9" s="49"/>
-      <c r="G9" s="49"/>
+      <c r="B9" s="40"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="40"/>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="45" t="s">
+      <c r="B10" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="36">
+      <c r="C10" s="27">
         <v>0</v>
       </c>
-      <c r="D10" s="36" t="s">
+      <c r="D10" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="E10" s="36">
+      <c r="E10" s="27">
         <v>0</v>
       </c>
-      <c r="F10" s="36" t="s">
+      <c r="F10" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="G10" s="37" t="s">
+      <c r="G10" s="28" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2125,22 +2228,22 @@
       <c r="A11" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="46" t="s">
+      <c r="B11" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="40">
+      <c r="C11" s="31">
         <v>0</v>
       </c>
-      <c r="D11" s="40" t="s">
+      <c r="D11" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="E11" s="40">
+      <c r="E11" s="31">
         <v>0</v>
       </c>
-      <c r="F11" s="40" t="s">
+      <c r="F11" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="G11" s="41" t="s">
+      <c r="G11" s="32" t="s">
         <v>35</v>
       </c>
     </row>
@@ -2148,22 +2251,22 @@
       <c r="A12" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="46" t="s">
+      <c r="B12" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="40">
+      <c r="C12" s="31">
         <v>0</v>
       </c>
-      <c r="D12" s="40" t="s">
+      <c r="D12" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="E12" s="40">
+      <c r="E12" s="31">
         <v>0</v>
       </c>
-      <c r="F12" s="40" t="s">
+      <c r="F12" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="G12" s="41" t="s">
+      <c r="G12" s="32" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2171,22 +2274,22 @@
       <c r="A13" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="46" t="s">
+      <c r="B13" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="40">
+      <c r="C13" s="31">
         <v>0</v>
       </c>
-      <c r="D13" s="40" t="s">
+      <c r="D13" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="E13" s="40">
+      <c r="E13" s="31">
         <v>0</v>
       </c>
-      <c r="F13" s="40" t="s">
+      <c r="F13" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="G13" s="41" t="s">
+      <c r="G13" s="32" t="s">
         <v>35</v>
       </c>
     </row>
@@ -2194,22 +2297,22 @@
       <c r="A14" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="B14" s="46" t="s">
+      <c r="B14" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="C14" s="40" t="s">
+      <c r="C14" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="40" t="s">
+      <c r="D14" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="E14" s="40" t="s">
+      <c r="E14" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="F14" s="40" t="s">
+      <c r="F14" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="G14" s="41" t="s">
+      <c r="G14" s="32" t="s">
         <v>35</v>
       </c>
     </row>
@@ -2217,22 +2320,22 @@
       <c r="A15" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="46" t="s">
+      <c r="B15" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="40">
+      <c r="C15" s="31">
         <v>0</v>
       </c>
-      <c r="D15" s="40" t="s">
+      <c r="D15" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="E15" s="40">
+      <c r="E15" s="31">
         <v>0</v>
       </c>
-      <c r="F15" s="40" t="s">
+      <c r="F15" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="G15" s="41" t="s">
+      <c r="G15" s="32" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2240,16 +2343,16 @@
       <c r="A16" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="B16" s="46"/>
-      <c r="C16" s="40"/>
-      <c r="D16" s="40"/>
-      <c r="E16" s="40" t="s">
+      <c r="B16" s="37"/>
+      <c r="C16" s="31"/>
+      <c r="D16" s="31"/>
+      <c r="E16" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="F16" s="40" t="s">
+      <c r="F16" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="G16" s="41" t="s">
+      <c r="G16" s="32" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2257,16 +2360,16 @@
       <c r="A17" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="B17" s="46"/>
-      <c r="C17" s="40"/>
-      <c r="D17" s="40"/>
-      <c r="E17" s="40" t="s">
+      <c r="B17" s="37"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="F17" s="40" t="s">
+      <c r="F17" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="G17" s="41" t="s">
+      <c r="G17" s="32" t="s">
         <v>35</v>
       </c>
     </row>
@@ -2274,16 +2377,16 @@
       <c r="A18" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="B18" s="46"/>
-      <c r="C18" s="40"/>
-      <c r="D18" s="40"/>
-      <c r="E18" s="40" t="s">
+      <c r="B18" s="37"/>
+      <c r="C18" s="31"/>
+      <c r="D18" s="31"/>
+      <c r="E18" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="F18" s="40" t="s">
+      <c r="F18" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="G18" s="41" t="s">
+      <c r="G18" s="32" t="s">
         <v>35</v>
       </c>
     </row>
@@ -2291,16 +2394,16 @@
       <c r="A19" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="B19" s="47"/>
-      <c r="C19" s="43"/>
-      <c r="D19" s="43"/>
-      <c r="E19" s="43" t="s">
+      <c r="B19" s="38"/>
+      <c r="C19" s="34"/>
+      <c r="D19" s="34"/>
+      <c r="E19" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="F19" s="43" t="s">
+      <c r="F19" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="G19" s="44" t="s">
+      <c r="G19" s="35" t="s">
         <v>35</v>
       </c>
     </row>
@@ -2321,4 +2424,200 @@
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="20.28515625" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="51.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="16.5" thickBot="1">
+      <c r="A1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="47" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="45" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="46" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="45" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="46" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" s="42" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="43" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="46" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="42" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="43" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="46" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" s="42" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" s="43" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="46" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="42" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="43" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="20.28515625" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="54.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="16.5" thickBot="1">
+      <c r="A1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="47" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="45" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="46" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="45" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="46" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" s="42" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="43" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="46" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="42" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="43" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="46" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" s="42" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" s="43" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="46" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="42" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="43" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>